<commit_message>
Implement Login&Register Scene, Custom GUI under construction
</commit_message>
<xml_diff>
--- a/References/Layout.xlsx
+++ b/References/Layout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="420" windowWidth="21795" windowHeight="6180" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="420" windowWidth="21795" windowHeight="6180"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
   <si>
     <t>Login</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t>Character Model / Avatar</t>
+  </si>
+  <si>
+    <t>Error message</t>
   </si>
 </sst>
 </file>
@@ -813,7 +816,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -888,12 +891,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -907,6 +904,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -952,6 +955,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1260,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AW28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA21" sqref="AA21:AF22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AJ25" sqref="AJ25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2082,7 +2094,7 @@
       <c r="AV17" s="11"/>
       <c r="AW17" s="12"/>
     </row>
-    <row r="18" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -2131,7 +2143,7 @@
       <c r="AV18" s="11"/>
       <c r="AW18" s="12"/>
     </row>
-    <row r="19" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -2149,19 +2161,22 @@
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
-      <c r="V19" s="11"/>
-      <c r="W19" s="11"/>
-      <c r="X19" s="11"/>
-      <c r="Y19" s="11"/>
-      <c r="Z19" s="11"/>
-      <c r="AA19" s="11"/>
-      <c r="AB19" s="11"/>
-      <c r="AC19" s="11"/>
-      <c r="AD19" s="11"/>
-      <c r="AE19" s="11"/>
-      <c r="AF19" s="11"/>
+      <c r="S19" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="T19" s="53"/>
+      <c r="U19" s="53"/>
+      <c r="V19" s="53"/>
+      <c r="W19" s="53"/>
+      <c r="X19" s="53"/>
+      <c r="Y19" s="53"/>
+      <c r="Z19" s="53"/>
+      <c r="AA19" s="53"/>
+      <c r="AB19" s="53"/>
+      <c r="AC19" s="53"/>
+      <c r="AD19" s="53"/>
+      <c r="AE19" s="53"/>
+      <c r="AF19" s="54"/>
       <c r="AG19" s="11"/>
       <c r="AH19" s="11"/>
       <c r="AI19" s="11"/>
@@ -2636,11 +2651,12 @@
       <c r="AW28" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="S21:X22"/>
     <mergeCell ref="AB6:AE8"/>
     <mergeCell ref="S4:AA7"/>
     <mergeCell ref="AA21:AF22"/>
+    <mergeCell ref="S19:AF19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AA21:AF22" location="Register!A1" display="Register"/>
@@ -2655,7 +2671,7 @@
   <dimension ref="B1:AW28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U21" sqref="U21:AD22"/>
+      <selection activeCell="AE20" sqref="AE20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3933,6 +3949,7 @@
     <hyperlink ref="W21:AB22" location="Lobby!A1" display="Register"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3941,7 +3958,7 @@
   <dimension ref="A1:AW28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:N14"/>
+      <selection activeCell="AG25" sqref="AG25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3956,17 +3973,17 @@
     <row r="2" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -4217,12 +4234,12 @@
       <c r="AO7" s="11"/>
       <c r="AP7" s="18"/>
       <c r="AQ7" s="19"/>
-      <c r="AR7" s="30" t="s">
+      <c r="AR7" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="AS7" s="30"/>
-      <c r="AT7" s="30"/>
-      <c r="AU7" s="30"/>
+      <c r="AS7" s="36"/>
+      <c r="AT7" s="36"/>
+      <c r="AU7" s="36"/>
       <c r="AV7" s="19"/>
       <c r="AW7" s="20"/>
     </row>
@@ -4230,44 +4247,44 @@
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
       <c r="O8" s="11"/>
-      <c r="P8" s="31" t="s">
+      <c r="P8" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="31"/>
-      <c r="V8" s="31"/>
-      <c r="W8" s="31"/>
-      <c r="X8" s="31"/>
-      <c r="Y8" s="31"/>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="35"/>
+      <c r="S8" s="35"/>
+      <c r="T8" s="35"/>
+      <c r="U8" s="35"/>
+      <c r="V8" s="35"/>
+      <c r="W8" s="35"/>
+      <c r="X8" s="35"/>
+      <c r="Y8" s="35"/>
       <c r="Z8" s="3"/>
-      <c r="AA8" s="31" t="s">
+      <c r="AA8" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="AB8" s="31"/>
-      <c r="AC8" s="31"/>
-      <c r="AD8" s="31"/>
-      <c r="AE8" s="31"/>
-      <c r="AF8" s="31"/>
-      <c r="AG8" s="31"/>
-      <c r="AH8" s="31"/>
-      <c r="AI8" s="31"/>
-      <c r="AJ8" s="31"/>
+      <c r="AB8" s="35"/>
+      <c r="AC8" s="35"/>
+      <c r="AD8" s="35"/>
+      <c r="AE8" s="35"/>
+      <c r="AF8" s="35"/>
+      <c r="AG8" s="35"/>
+      <c r="AH8" s="35"/>
+      <c r="AI8" s="35"/>
+      <c r="AJ8" s="35"/>
       <c r="AK8" s="12"/>
       <c r="AL8" s="11"/>
       <c r="AM8" s="11"/>
@@ -4286,38 +4303,38 @@
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
       <c r="O9" s="11"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
-      <c r="T9" s="31"/>
-      <c r="U9" s="31"/>
-      <c r="V9" s="31"/>
-      <c r="W9" s="31"/>
-      <c r="X9" s="31"/>
-      <c r="Y9" s="31"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="35"/>
+      <c r="W9" s="35"/>
+      <c r="X9" s="35"/>
+      <c r="Y9" s="35"/>
       <c r="Z9" s="3"/>
-      <c r="AA9" s="31"/>
-      <c r="AB9" s="31"/>
-      <c r="AC9" s="31"/>
-      <c r="AD9" s="31"/>
-      <c r="AE9" s="31"/>
-      <c r="AF9" s="31"/>
-      <c r="AG9" s="31"/>
-      <c r="AH9" s="31"/>
-      <c r="AI9" s="31"/>
-      <c r="AJ9" s="31"/>
+      <c r="AA9" s="35"/>
+      <c r="AB9" s="35"/>
+      <c r="AC9" s="35"/>
+      <c r="AD9" s="35"/>
+      <c r="AE9" s="35"/>
+      <c r="AF9" s="35"/>
+      <c r="AG9" s="35"/>
+      <c r="AH9" s="35"/>
+      <c r="AI9" s="35"/>
+      <c r="AJ9" s="35"/>
       <c r="AK9" s="4"/>
       <c r="AP9" s="10"/>
       <c r="AQ9" s="3"/>
@@ -4332,38 +4349,38 @@
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
       <c r="O10" s="11"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="31"/>
-      <c r="T10" s="31"/>
-      <c r="U10" s="31"/>
-      <c r="V10" s="31"/>
-      <c r="W10" s="31"/>
-      <c r="X10" s="31"/>
-      <c r="Y10" s="31"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="35"/>
+      <c r="S10" s="35"/>
+      <c r="T10" s="35"/>
+      <c r="U10" s="35"/>
+      <c r="V10" s="35"/>
+      <c r="W10" s="35"/>
+      <c r="X10" s="35"/>
+      <c r="Y10" s="35"/>
       <c r="Z10" s="3"/>
-      <c r="AA10" s="31"/>
-      <c r="AB10" s="31"/>
-      <c r="AC10" s="31"/>
-      <c r="AD10" s="31"/>
-      <c r="AE10" s="31"/>
-      <c r="AF10" s="31"/>
-      <c r="AG10" s="31"/>
-      <c r="AH10" s="31"/>
-      <c r="AI10" s="31"/>
-      <c r="AJ10" s="31"/>
+      <c r="AA10" s="35"/>
+      <c r="AB10" s="35"/>
+      <c r="AC10" s="35"/>
+      <c r="AD10" s="35"/>
+      <c r="AE10" s="35"/>
+      <c r="AF10" s="35"/>
+      <c r="AG10" s="35"/>
+      <c r="AH10" s="35"/>
+      <c r="AI10" s="35"/>
+      <c r="AJ10" s="35"/>
       <c r="AK10" s="4"/>
       <c r="AP10" s="10"/>
       <c r="AQ10" s="11"/>
@@ -4424,44 +4441,44 @@
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
       <c r="O12" s="11"/>
-      <c r="P12" s="31" t="s">
+      <c r="P12" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="31"/>
-      <c r="T12" s="31"/>
-      <c r="U12" s="31"/>
-      <c r="V12" s="31"/>
-      <c r="W12" s="31"/>
-      <c r="X12" s="31"/>
-      <c r="Y12" s="31"/>
+      <c r="Q12" s="35"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="35"/>
+      <c r="T12" s="35"/>
+      <c r="U12" s="35"/>
+      <c r="V12" s="35"/>
+      <c r="W12" s="35"/>
+      <c r="X12" s="35"/>
+      <c r="Y12" s="35"/>
       <c r="Z12" s="3"/>
-      <c r="AA12" s="31" t="s">
+      <c r="AA12" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="AB12" s="31"/>
-      <c r="AC12" s="31"/>
-      <c r="AD12" s="31"/>
-      <c r="AE12" s="31"/>
-      <c r="AF12" s="31"/>
-      <c r="AG12" s="31"/>
-      <c r="AH12" s="31"/>
-      <c r="AI12" s="31"/>
-      <c r="AJ12" s="31"/>
+      <c r="AB12" s="35"/>
+      <c r="AC12" s="35"/>
+      <c r="AD12" s="35"/>
+      <c r="AE12" s="35"/>
+      <c r="AF12" s="35"/>
+      <c r="AG12" s="35"/>
+      <c r="AH12" s="35"/>
+      <c r="AI12" s="35"/>
+      <c r="AJ12" s="35"/>
       <c r="AK12" s="4"/>
       <c r="AP12" s="10"/>
       <c r="AQ12" s="11"/>
@@ -4476,38 +4493,38 @@
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
       <c r="O13" s="11"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="31"/>
-      <c r="S13" s="31"/>
-      <c r="T13" s="31"/>
-      <c r="U13" s="31"/>
-      <c r="V13" s="31"/>
-      <c r="W13" s="31"/>
-      <c r="X13" s="31"/>
-      <c r="Y13" s="31"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="35"/>
+      <c r="T13" s="35"/>
+      <c r="U13" s="35"/>
+      <c r="V13" s="35"/>
+      <c r="W13" s="35"/>
+      <c r="X13" s="35"/>
+      <c r="Y13" s="35"/>
       <c r="Z13" s="3"/>
-      <c r="AA13" s="31"/>
-      <c r="AB13" s="31"/>
-      <c r="AC13" s="31"/>
-      <c r="AD13" s="31"/>
-      <c r="AE13" s="31"/>
-      <c r="AF13" s="31"/>
-      <c r="AG13" s="31"/>
-      <c r="AH13" s="31"/>
-      <c r="AI13" s="31"/>
-      <c r="AJ13" s="31"/>
+      <c r="AA13" s="35"/>
+      <c r="AB13" s="35"/>
+      <c r="AC13" s="35"/>
+      <c r="AD13" s="35"/>
+      <c r="AE13" s="35"/>
+      <c r="AF13" s="35"/>
+      <c r="AG13" s="35"/>
+      <c r="AH13" s="35"/>
+      <c r="AI13" s="35"/>
+      <c r="AJ13" s="35"/>
       <c r="AK13" s="4"/>
       <c r="AP13" s="10"/>
       <c r="AQ13" s="11"/>
@@ -4522,38 +4539,38 @@
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
       <c r="O14" s="11"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="31"/>
-      <c r="R14" s="31"/>
-      <c r="S14" s="31"/>
-      <c r="T14" s="31"/>
-      <c r="U14" s="31"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="31"/>
-      <c r="X14" s="31"/>
-      <c r="Y14" s="31"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="35"/>
+      <c r="U14" s="35"/>
+      <c r="V14" s="35"/>
+      <c r="W14" s="35"/>
+      <c r="X14" s="35"/>
+      <c r="Y14" s="35"/>
       <c r="Z14" s="3"/>
-      <c r="AA14" s="31"/>
-      <c r="AB14" s="31"/>
-      <c r="AC14" s="31"/>
-      <c r="AD14" s="31"/>
-      <c r="AE14" s="31"/>
-      <c r="AF14" s="31"/>
-      <c r="AG14" s="31"/>
-      <c r="AH14" s="31"/>
-      <c r="AI14" s="31"/>
-      <c r="AJ14" s="31"/>
+      <c r="AA14" s="35"/>
+      <c r="AB14" s="35"/>
+      <c r="AC14" s="35"/>
+      <c r="AD14" s="35"/>
+      <c r="AE14" s="35"/>
+      <c r="AF14" s="35"/>
+      <c r="AG14" s="35"/>
+      <c r="AH14" s="35"/>
+      <c r="AI14" s="35"/>
+      <c r="AJ14" s="35"/>
       <c r="AK14" s="4"/>
       <c r="AP14" s="10"/>
       <c r="AQ14" s="11"/>
@@ -4614,44 +4631,44 @@
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
       <c r="O16" s="11"/>
-      <c r="P16" s="31" t="s">
+      <c r="P16" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="31"/>
-      <c r="S16" s="31"/>
-      <c r="T16" s="31"/>
-      <c r="U16" s="31"/>
-      <c r="V16" s="31"/>
-      <c r="W16" s="31"/>
-      <c r="X16" s="31"/>
-      <c r="Y16" s="31"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="35"/>
+      <c r="S16" s="35"/>
+      <c r="T16" s="35"/>
+      <c r="U16" s="35"/>
+      <c r="V16" s="35"/>
+      <c r="W16" s="35"/>
+      <c r="X16" s="35"/>
+      <c r="Y16" s="35"/>
       <c r="Z16" s="3"/>
-      <c r="AA16" s="31" t="s">
+      <c r="AA16" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="AB16" s="31"/>
-      <c r="AC16" s="31"/>
-      <c r="AD16" s="31"/>
-      <c r="AE16" s="31"/>
-      <c r="AF16" s="31"/>
-      <c r="AG16" s="31"/>
-      <c r="AH16" s="31"/>
-      <c r="AI16" s="31"/>
-      <c r="AJ16" s="31"/>
+      <c r="AB16" s="35"/>
+      <c r="AC16" s="35"/>
+      <c r="AD16" s="35"/>
+      <c r="AE16" s="35"/>
+      <c r="AF16" s="35"/>
+      <c r="AG16" s="35"/>
+      <c r="AH16" s="35"/>
+      <c r="AI16" s="35"/>
+      <c r="AJ16" s="35"/>
       <c r="AK16" s="4"/>
       <c r="AP16" s="10"/>
       <c r="AQ16" s="11"/>
@@ -4666,38 +4683,38 @@
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
       <c r="O17" s="11"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="31"/>
-      <c r="R17" s="31"/>
-      <c r="S17" s="31"/>
-      <c r="T17" s="31"/>
-      <c r="U17" s="31"/>
-      <c r="V17" s="31"/>
-      <c r="W17" s="31"/>
-      <c r="X17" s="31"/>
-      <c r="Y17" s="31"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="35"/>
+      <c r="U17" s="35"/>
+      <c r="V17" s="35"/>
+      <c r="W17" s="35"/>
+      <c r="X17" s="35"/>
+      <c r="Y17" s="35"/>
       <c r="Z17" s="3"/>
-      <c r="AA17" s="31"/>
-      <c r="AB17" s="31"/>
-      <c r="AC17" s="31"/>
-      <c r="AD17" s="31"/>
-      <c r="AE17" s="31"/>
-      <c r="AF17" s="31"/>
-      <c r="AG17" s="31"/>
-      <c r="AH17" s="31"/>
-      <c r="AI17" s="31"/>
-      <c r="AJ17" s="31"/>
+      <c r="AA17" s="35"/>
+      <c r="AB17" s="35"/>
+      <c r="AC17" s="35"/>
+      <c r="AD17" s="35"/>
+      <c r="AE17" s="35"/>
+      <c r="AF17" s="35"/>
+      <c r="AG17" s="35"/>
+      <c r="AH17" s="35"/>
+      <c r="AI17" s="35"/>
+      <c r="AJ17" s="35"/>
       <c r="AK17" s="4"/>
       <c r="AP17" s="10"/>
       <c r="AQ17" s="11"/>
@@ -4712,38 +4729,38 @@
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
       <c r="D18" s="10"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
       <c r="O18" s="11"/>
-      <c r="P18" s="31"/>
-      <c r="Q18" s="31"/>
-      <c r="R18" s="31"/>
-      <c r="S18" s="31"/>
-      <c r="T18" s="31"/>
-      <c r="U18" s="31"/>
-      <c r="V18" s="31"/>
-      <c r="W18" s="31"/>
-      <c r="X18" s="31"/>
-      <c r="Y18" s="31"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="35"/>
+      <c r="T18" s="35"/>
+      <c r="U18" s="35"/>
+      <c r="V18" s="35"/>
+      <c r="W18" s="35"/>
+      <c r="X18" s="35"/>
+      <c r="Y18" s="35"/>
       <c r="Z18" s="3"/>
-      <c r="AA18" s="31"/>
-      <c r="AB18" s="31"/>
-      <c r="AC18" s="31"/>
-      <c r="AD18" s="31"/>
-      <c r="AE18" s="31"/>
-      <c r="AF18" s="31"/>
-      <c r="AG18" s="31"/>
-      <c r="AH18" s="31"/>
-      <c r="AI18" s="31"/>
-      <c r="AJ18" s="31"/>
+      <c r="AA18" s="35"/>
+      <c r="AB18" s="35"/>
+      <c r="AC18" s="35"/>
+      <c r="AD18" s="35"/>
+      <c r="AE18" s="35"/>
+      <c r="AF18" s="35"/>
+      <c r="AG18" s="35"/>
+      <c r="AH18" s="35"/>
+      <c r="AI18" s="35"/>
+      <c r="AJ18" s="35"/>
       <c r="AK18" s="4"/>
       <c r="AP18" s="10"/>
       <c r="AQ18" s="11"/>
@@ -4804,44 +4821,44 @@
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
       <c r="D20" s="10"/>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
       <c r="O20" s="11"/>
-      <c r="P20" s="31" t="s">
+      <c r="P20" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="Q20" s="31"/>
-      <c r="R20" s="31"/>
-      <c r="S20" s="31"/>
-      <c r="T20" s="31"/>
-      <c r="U20" s="31"/>
-      <c r="V20" s="31"/>
-      <c r="W20" s="31"/>
-      <c r="X20" s="31"/>
-      <c r="Y20" s="31"/>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="35"/>
+      <c r="T20" s="35"/>
+      <c r="U20" s="35"/>
+      <c r="V20" s="35"/>
+      <c r="W20" s="35"/>
+      <c r="X20" s="35"/>
+      <c r="Y20" s="35"/>
       <c r="Z20" s="3"/>
-      <c r="AA20" s="31" t="s">
+      <c r="AA20" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="AB20" s="31"/>
-      <c r="AC20" s="31"/>
-      <c r="AD20" s="31"/>
-      <c r="AE20" s="31"/>
-      <c r="AF20" s="31"/>
-      <c r="AG20" s="31"/>
-      <c r="AH20" s="31"/>
-      <c r="AI20" s="31"/>
-      <c r="AJ20" s="31"/>
+      <c r="AB20" s="35"/>
+      <c r="AC20" s="35"/>
+      <c r="AD20" s="35"/>
+      <c r="AE20" s="35"/>
+      <c r="AF20" s="35"/>
+      <c r="AG20" s="35"/>
+      <c r="AH20" s="35"/>
+      <c r="AI20" s="35"/>
+      <c r="AJ20" s="35"/>
       <c r="AK20" s="4"/>
       <c r="AP20" s="10"/>
       <c r="AQ20" s="11"/>
@@ -4856,38 +4873,38 @@
       <c r="B21" s="10"/>
       <c r="C21" s="11"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
       <c r="O21" s="11"/>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="31"/>
-      <c r="R21" s="31"/>
-      <c r="S21" s="31"/>
-      <c r="T21" s="31"/>
-      <c r="U21" s="31"/>
-      <c r="V21" s="31"/>
-      <c r="W21" s="31"/>
-      <c r="X21" s="31"/>
-      <c r="Y21" s="31"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="35"/>
+      <c r="U21" s="35"/>
+      <c r="V21" s="35"/>
+      <c r="W21" s="35"/>
+      <c r="X21" s="35"/>
+      <c r="Y21" s="35"/>
       <c r="Z21" s="3"/>
-      <c r="AA21" s="31"/>
-      <c r="AB21" s="31"/>
-      <c r="AC21" s="31"/>
-      <c r="AD21" s="31"/>
-      <c r="AE21" s="31"/>
-      <c r="AF21" s="31"/>
-      <c r="AG21" s="31"/>
-      <c r="AH21" s="31"/>
-      <c r="AI21" s="31"/>
-      <c r="AJ21" s="31"/>
+      <c r="AA21" s="35"/>
+      <c r="AB21" s="35"/>
+      <c r="AC21" s="35"/>
+      <c r="AD21" s="35"/>
+      <c r="AE21" s="35"/>
+      <c r="AF21" s="35"/>
+      <c r="AG21" s="35"/>
+      <c r="AH21" s="35"/>
+      <c r="AI21" s="35"/>
+      <c r="AJ21" s="35"/>
       <c r="AK21" s="4"/>
       <c r="AP21" s="10"/>
       <c r="AQ21" s="11"/>
@@ -4902,38 +4919,38 @@
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
       <c r="O22" s="11"/>
-      <c r="P22" s="31"/>
-      <c r="Q22" s="31"/>
-      <c r="R22" s="31"/>
-      <c r="S22" s="31"/>
-      <c r="T22" s="31"/>
-      <c r="U22" s="31"/>
-      <c r="V22" s="31"/>
-      <c r="W22" s="31"/>
-      <c r="X22" s="31"/>
-      <c r="Y22" s="31"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="35"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="35"/>
+      <c r="U22" s="35"/>
+      <c r="V22" s="35"/>
+      <c r="W22" s="35"/>
+      <c r="X22" s="35"/>
+      <c r="Y22" s="35"/>
       <c r="Z22" s="3"/>
-      <c r="AA22" s="31"/>
-      <c r="AB22" s="31"/>
-      <c r="AC22" s="31"/>
-      <c r="AD22" s="31"/>
-      <c r="AE22" s="31"/>
-      <c r="AF22" s="31"/>
-      <c r="AG22" s="31"/>
-      <c r="AH22" s="31"/>
-      <c r="AI22" s="31"/>
-      <c r="AJ22" s="31"/>
+      <c r="AA22" s="35"/>
+      <c r="AB22" s="35"/>
+      <c r="AC22" s="35"/>
+      <c r="AD22" s="35"/>
+      <c r="AE22" s="35"/>
+      <c r="AF22" s="35"/>
+      <c r="AG22" s="35"/>
+      <c r="AH22" s="35"/>
+      <c r="AI22" s="35"/>
+      <c r="AJ22" s="35"/>
       <c r="AK22" s="4"/>
       <c r="AP22" s="10"/>
       <c r="AQ22" s="11"/>
@@ -5178,16 +5195,16 @@
       <c r="AM27" s="11"/>
       <c r="AN27" s="11"/>
       <c r="AO27" s="11"/>
-      <c r="AP27" s="33" t="s">
+      <c r="AP27" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="AQ27" s="33"/>
-      <c r="AR27" s="33"/>
-      <c r="AS27" s="33"/>
-      <c r="AT27" s="33"/>
-      <c r="AU27" s="33"/>
-      <c r="AV27" s="33"/>
-      <c r="AW27" s="34"/>
+      <c r="AQ27" s="31"/>
+      <c r="AR27" s="31"/>
+      <c r="AS27" s="31"/>
+      <c r="AT27" s="31"/>
+      <c r="AU27" s="31"/>
+      <c r="AV27" s="31"/>
+      <c r="AW27" s="32"/>
     </row>
     <row r="28" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="13"/>
@@ -5230,17 +5247,20 @@
       <c r="AM28" s="14"/>
       <c r="AN28" s="14"/>
       <c r="AO28" s="14"/>
-      <c r="AP28" s="35"/>
-      <c r="AQ28" s="35"/>
-      <c r="AR28" s="35"/>
-      <c r="AS28" s="35"/>
-      <c r="AT28" s="35"/>
-      <c r="AU28" s="35"/>
-      <c r="AV28" s="35"/>
-      <c r="AW28" s="36"/>
+      <c r="AP28" s="33"/>
+      <c r="AQ28" s="33"/>
+      <c r="AR28" s="33"/>
+      <c r="AS28" s="33"/>
+      <c r="AT28" s="33"/>
+      <c r="AU28" s="33"/>
+      <c r="AV28" s="33"/>
+      <c r="AW28" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="AA12:AJ14"/>
+    <mergeCell ref="AA16:AJ18"/>
+    <mergeCell ref="AA20:AJ22"/>
     <mergeCell ref="D2:L5"/>
     <mergeCell ref="M4:P6"/>
     <mergeCell ref="AP27:AW28"/>
@@ -5257,9 +5277,6 @@
     <mergeCell ref="P16:Y18"/>
     <mergeCell ref="P20:Y22"/>
     <mergeCell ref="AA8:AJ10"/>
-    <mergeCell ref="AA12:AJ14"/>
-    <mergeCell ref="AA16:AJ18"/>
-    <mergeCell ref="AA20:AJ22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="V25:AA26" location="CreateRoom!A1" display="Create Room"/>
@@ -5288,8 +5305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AW28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AJ28" sqref="AJ28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="BD24" sqref="BD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5302,17 +5319,17 @@
     <row r="2" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -5563,12 +5580,12 @@
       <c r="AO7" s="11"/>
       <c r="AP7" s="18"/>
       <c r="AQ7" s="19"/>
-      <c r="AR7" s="30" t="s">
+      <c r="AR7" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="AS7" s="30"/>
-      <c r="AT7" s="30"/>
-      <c r="AU7" s="30"/>
+      <c r="AS7" s="36"/>
+      <c r="AT7" s="36"/>
+      <c r="AU7" s="36"/>
       <c r="AV7" s="19"/>
       <c r="AW7" s="20"/>
     </row>
@@ -6466,16 +6483,16 @@
       <c r="AM27" s="11"/>
       <c r="AN27" s="11"/>
       <c r="AO27" s="11"/>
-      <c r="AP27" s="33" t="s">
+      <c r="AP27" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="AQ27" s="33"/>
-      <c r="AR27" s="33"/>
-      <c r="AS27" s="33"/>
-      <c r="AT27" s="33"/>
-      <c r="AU27" s="33"/>
-      <c r="AV27" s="33"/>
-      <c r="AW27" s="34"/>
+      <c r="AQ27" s="31"/>
+      <c r="AR27" s="31"/>
+      <c r="AS27" s="31"/>
+      <c r="AT27" s="31"/>
+      <c r="AU27" s="31"/>
+      <c r="AV27" s="31"/>
+      <c r="AW27" s="32"/>
     </row>
     <row r="28" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="13"/>
@@ -6518,28 +6535,28 @@
       <c r="AM28" s="14"/>
       <c r="AN28" s="14"/>
       <c r="AO28" s="14"/>
-      <c r="AP28" s="35"/>
-      <c r="AQ28" s="35"/>
-      <c r="AR28" s="35"/>
-      <c r="AS28" s="35"/>
-      <c r="AT28" s="35"/>
-      <c r="AU28" s="35"/>
-      <c r="AV28" s="35"/>
-      <c r="AW28" s="36"/>
+      <c r="AP28" s="33"/>
+      <c r="AQ28" s="33"/>
+      <c r="AR28" s="33"/>
+      <c r="AS28" s="33"/>
+      <c r="AT28" s="33"/>
+      <c r="AU28" s="33"/>
+      <c r="AV28" s="33"/>
+      <c r="AW28" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D2:L5"/>
-    <mergeCell ref="AU3:AV4"/>
-    <mergeCell ref="M4:P6"/>
-    <mergeCell ref="N25:S26"/>
-    <mergeCell ref="V25:AA26"/>
     <mergeCell ref="AP27:AW28"/>
     <mergeCell ref="AR7:AU7"/>
     <mergeCell ref="F8:S18"/>
     <mergeCell ref="V8:AI18"/>
     <mergeCell ref="G20:R21"/>
     <mergeCell ref="W20:AH21"/>
+    <mergeCell ref="D2:L5"/>
+    <mergeCell ref="AU3:AV4"/>
+    <mergeCell ref="M4:P6"/>
+    <mergeCell ref="N25:S26"/>
+    <mergeCell ref="V25:AA26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N25:S26" location="Lobby!A1" display="Cancel"/>

</xml_diff>

<commit_message>
Finish Login Scene with custom GUI Skin
</commit_message>
<xml_diff>
--- a/References/Layout.xlsx
+++ b/References/Layout.xlsx
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
   <si>
     <t>Login</t>
   </si>
@@ -440,6 +440,9 @@
   </si>
   <si>
     <t>Error message</t>
+  </si>
+  <si>
+    <t>Back</t>
   </si>
 </sst>
 </file>
@@ -547,7 +550,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -747,68 +750,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -816,7 +757,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -873,22 +814,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -904,9 +839,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -955,15 +887,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1273,7 +1196,7 @@
   <dimension ref="B1:AW28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AJ25" sqref="AJ25"/>
+      <selection activeCell="AZ24" sqref="AZ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2161,22 +2084,22 @@
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
-      <c r="S19" s="52" t="s">
+      <c r="S19" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="T19" s="53"/>
-      <c r="U19" s="53"/>
-      <c r="V19" s="53"/>
-      <c r="W19" s="53"/>
-      <c r="X19" s="53"/>
-      <c r="Y19" s="53"/>
-      <c r="Z19" s="53"/>
-      <c r="AA19" s="53"/>
-      <c r="AB19" s="53"/>
-      <c r="AC19" s="53"/>
-      <c r="AD19" s="53"/>
-      <c r="AE19" s="53"/>
-      <c r="AF19" s="54"/>
+      <c r="T19" s="25"/>
+      <c r="U19" s="25"/>
+      <c r="V19" s="25"/>
+      <c r="W19" s="25"/>
+      <c r="X19" s="25"/>
+      <c r="Y19" s="25"/>
+      <c r="Z19" s="25"/>
+      <c r="AA19" s="25"/>
+      <c r="AB19" s="25"/>
+      <c r="AC19" s="25"/>
+      <c r="AD19" s="25"/>
+      <c r="AE19" s="25"/>
+      <c r="AF19" s="26"/>
       <c r="AG19" s="11"/>
       <c r="AH19" s="11"/>
       <c r="AI19" s="11"/>
@@ -2264,11 +2187,11 @@
       <c r="N21" s="11"/>
       <c r="O21" s="11"/>
       <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="21" t="s">
+      <c r="Q21" s="21" t="s">
         <v>0</v>
       </c>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
       <c r="T21" s="21"/>
       <c r="U21" s="21"/>
       <c r="V21" s="21"/>
@@ -2283,8 +2206,8 @@
       <c r="AD21" s="21"/>
       <c r="AE21" s="21"/>
       <c r="AF21" s="21"/>
-      <c r="AG21" s="11"/>
-      <c r="AH21" s="11"/>
+      <c r="AG21" s="21"/>
+      <c r="AH21" s="21"/>
       <c r="AI21" s="11"/>
       <c r="AJ21" s="11"/>
       <c r="AK21" s="11"/>
@@ -2317,8 +2240,8 @@
       <c r="N22" s="11"/>
       <c r="O22" s="11"/>
       <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="21"/>
       <c r="S22" s="21"/>
       <c r="T22" s="21"/>
       <c r="U22" s="21"/>
@@ -2332,8 +2255,8 @@
       <c r="AD22" s="21"/>
       <c r="AE22" s="21"/>
       <c r="AF22" s="21"/>
-      <c r="AG22" s="11"/>
-      <c r="AH22" s="11"/>
+      <c r="AG22" s="21"/>
+      <c r="AH22" s="21"/>
       <c r="AI22" s="11"/>
       <c r="AJ22" s="11"/>
       <c r="AK22" s="11"/>
@@ -2366,24 +2289,24 @@
       <c r="N23" s="11"/>
       <c r="O23" s="11"/>
       <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="11"/>
+      <c r="Q23" s="21"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="21"/>
+      <c r="U23" s="21"/>
+      <c r="V23" s="21"/>
+      <c r="W23" s="21"/>
+      <c r="X23" s="21"/>
       <c r="Y23" s="11"/>
       <c r="Z23" s="11"/>
-      <c r="AA23" s="11"/>
-      <c r="AB23" s="11"/>
-      <c r="AC23" s="11"/>
-      <c r="AD23" s="11"/>
-      <c r="AE23" s="11"/>
-      <c r="AF23" s="11"/>
-      <c r="AG23" s="11"/>
-      <c r="AH23" s="11"/>
+      <c r="AA23" s="21"/>
+      <c r="AB23" s="21"/>
+      <c r="AC23" s="21"/>
+      <c r="AD23" s="21"/>
+      <c r="AE23" s="21"/>
+      <c r="AF23" s="21"/>
+      <c r="AG23" s="21"/>
+      <c r="AH23" s="21"/>
       <c r="AI23" s="11"/>
       <c r="AJ23" s="11"/>
       <c r="AK23" s="11"/>
@@ -2416,24 +2339,24 @@
       <c r="N24" s="11"/>
       <c r="O24" s="11"/>
       <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="11"/>
-      <c r="T24" s="11"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="21"/>
+      <c r="V24" s="21"/>
+      <c r="W24" s="21"/>
+      <c r="X24" s="21"/>
       <c r="Y24" s="11"/>
       <c r="Z24" s="11"/>
-      <c r="AA24" s="11"/>
-      <c r="AB24" s="11"/>
-      <c r="AC24" s="11"/>
-      <c r="AD24" s="11"/>
-      <c r="AE24" s="11"/>
-      <c r="AF24" s="11"/>
-      <c r="AG24" s="11"/>
-      <c r="AH24" s="11"/>
+      <c r="AA24" s="21"/>
+      <c r="AB24" s="21"/>
+      <c r="AC24" s="21"/>
+      <c r="AD24" s="21"/>
+      <c r="AE24" s="21"/>
+      <c r="AF24" s="21"/>
+      <c r="AG24" s="21"/>
+      <c r="AH24" s="21"/>
       <c r="AI24" s="11"/>
       <c r="AJ24" s="11"/>
       <c r="AK24" s="11"/>
@@ -2652,11 +2575,11 @@
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="S21:X22"/>
     <mergeCell ref="AB6:AE8"/>
     <mergeCell ref="S4:AA7"/>
-    <mergeCell ref="AA21:AF22"/>
     <mergeCell ref="S19:AF19"/>
+    <mergeCell ref="Q21:X24"/>
+    <mergeCell ref="AA21:AH24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AA21:AF22" location="Register!A1" display="Register"/>
@@ -2671,7 +2594,7 @@
   <dimension ref="B1:AW28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AE20" sqref="AE20"/>
+      <selection activeCell="Q21" sqref="Q21:X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3062,9 +2985,10 @@
       <c r="V9" s="11"/>
       <c r="W9" s="11"/>
       <c r="X9" s="11"/>
-      <c r="AC9" s="11" t="s">
+      <c r="AB9" s="11" t="s">
         <v>8</v>
       </c>
+      <c r="AC9" s="11"/>
       <c r="AD9" s="11"/>
       <c r="AE9" s="11"/>
       <c r="AF9" s="11"/>
@@ -3076,7 +3000,6 @@
       <c r="AL9" s="11"/>
       <c r="AM9" s="11"/>
       <c r="AN9" s="11"/>
-      <c r="AO9" s="11"/>
       <c r="AU9" s="11"/>
       <c r="AV9" s="11"/>
       <c r="AW9" s="12"/>
@@ -3104,6 +3027,7 @@
       <c r="V10" s="11"/>
       <c r="W10" s="11"/>
       <c r="X10" s="11"/>
+      <c r="AB10" s="11"/>
       <c r="AC10" s="11"/>
       <c r="AD10" s="11"/>
       <c r="AE10" s="11"/>
@@ -3116,7 +3040,6 @@
       <c r="AL10" s="11"/>
       <c r="AM10" s="11"/>
       <c r="AN10" s="11"/>
-      <c r="AO10" s="11"/>
       <c r="AU10" s="11"/>
       <c r="AV10" s="11"/>
       <c r="AW10" s="12"/>
@@ -3145,7 +3068,8 @@
       <c r="V11" s="8"/>
       <c r="W11" s="8"/>
       <c r="X11" s="9"/>
-      <c r="AB11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="8"/>
       <c r="AC11" s="8"/>
       <c r="AD11" s="8"/>
       <c r="AE11" s="8"/>
@@ -3157,8 +3081,7 @@
       <c r="AK11" s="8"/>
       <c r="AL11" s="8"/>
       <c r="AM11" s="8"/>
-      <c r="AN11" s="8"/>
-      <c r="AO11" s="9"/>
+      <c r="AN11" s="9"/>
       <c r="AU11" s="11"/>
       <c r="AV11" s="11"/>
       <c r="AW11" s="12"/>
@@ -3187,7 +3110,8 @@
       <c r="V12" s="14"/>
       <c r="W12" s="14"/>
       <c r="X12" s="15"/>
-      <c r="AB12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="14"/>
       <c r="AC12" s="14"/>
       <c r="AD12" s="14"/>
       <c r="AE12" s="14"/>
@@ -3199,8 +3123,7 @@
       <c r="AK12" s="14"/>
       <c r="AL12" s="14"/>
       <c r="AM12" s="14"/>
-      <c r="AN12" s="14"/>
-      <c r="AO12" s="15"/>
+      <c r="AN12" s="15"/>
       <c r="AU12" s="11"/>
       <c r="AV12" s="11"/>
       <c r="AW12" s="12"/>
@@ -3228,6 +3151,7 @@
       <c r="V13" s="11"/>
       <c r="W13" s="11"/>
       <c r="X13" s="11"/>
+      <c r="AB13" s="11"/>
       <c r="AC13" s="11"/>
       <c r="AD13" s="11"/>
       <c r="AE13" s="11"/>
@@ -3240,7 +3164,6 @@
       <c r="AL13" s="11"/>
       <c r="AM13" s="11"/>
       <c r="AN13" s="11"/>
-      <c r="AO13" s="11"/>
       <c r="AU13" s="11"/>
       <c r="AV13" s="11"/>
       <c r="AW13" s="12"/>
@@ -3272,9 +3195,10 @@
       <c r="V14" s="11"/>
       <c r="W14" s="11"/>
       <c r="X14" s="11"/>
-      <c r="AC14" s="11" t="s">
+      <c r="AB14" s="11" t="s">
         <v>7</v>
       </c>
+      <c r="AC14" s="11"/>
       <c r="AD14" s="11"/>
       <c r="AE14" s="11"/>
       <c r="AF14" s="11"/>
@@ -3286,7 +3210,6 @@
       <c r="AL14" s="11"/>
       <c r="AM14" s="11"/>
       <c r="AN14" s="11"/>
-      <c r="AO14" s="11"/>
       <c r="AU14" s="11"/>
       <c r="AV14" s="11"/>
       <c r="AW14" s="12"/>
@@ -3314,6 +3237,7 @@
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
       <c r="X15" s="11"/>
+      <c r="AB15" s="11"/>
       <c r="AC15" s="11"/>
       <c r="AD15" s="11"/>
       <c r="AE15" s="11"/>
@@ -3326,7 +3250,6 @@
       <c r="AL15" s="11"/>
       <c r="AM15" s="11"/>
       <c r="AN15" s="11"/>
-      <c r="AO15" s="11"/>
       <c r="AU15" s="11"/>
       <c r="AV15" s="11"/>
       <c r="AW15" s="12"/>
@@ -3355,7 +3278,8 @@
       <c r="V16" s="8"/>
       <c r="W16" s="8"/>
       <c r="X16" s="9"/>
-      <c r="AB16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="8"/>
       <c r="AC16" s="8"/>
       <c r="AD16" s="8"/>
       <c r="AE16" s="8"/>
@@ -3367,8 +3291,7 @@
       <c r="AK16" s="8"/>
       <c r="AL16" s="8"/>
       <c r="AM16" s="8"/>
-      <c r="AN16" s="8"/>
-      <c r="AO16" s="9"/>
+      <c r="AN16" s="9"/>
       <c r="AU16" s="11"/>
       <c r="AV16" s="11"/>
       <c r="AW16" s="12"/>
@@ -3397,7 +3320,8 @@
       <c r="V17" s="14"/>
       <c r="W17" s="14"/>
       <c r="X17" s="15"/>
-      <c r="AB17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="14"/>
       <c r="AC17" s="14"/>
       <c r="AD17" s="14"/>
       <c r="AE17" s="14"/>
@@ -3409,8 +3333,7 @@
       <c r="AK17" s="14"/>
       <c r="AL17" s="14"/>
       <c r="AM17" s="14"/>
-      <c r="AN17" s="14"/>
-      <c r="AO17" s="15"/>
+      <c r="AN17" s="15"/>
       <c r="AU17" s="11"/>
       <c r="AV17" s="11"/>
       <c r="AW17" s="12"/>
@@ -3579,26 +3502,27 @@
       <c r="N21" s="11"/>
       <c r="O21" s="11"/>
       <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="24" t="s">
+      <c r="Q21" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="21"/>
+      <c r="V21" s="21"/>
+      <c r="W21" s="21"/>
+      <c r="X21" s="21"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="V21" s="25"/>
-      <c r="W21" s="25"/>
-      <c r="X21" s="25"/>
-      <c r="Y21" s="25"/>
-      <c r="Z21" s="25"/>
-      <c r="AA21" s="25"/>
-      <c r="AB21" s="25"/>
-      <c r="AC21" s="25"/>
-      <c r="AD21" s="26"/>
-      <c r="AE21" s="11"/>
-      <c r="AF21" s="11"/>
-      <c r="AG21" s="11"/>
-      <c r="AH21" s="11"/>
+      <c r="AB21" s="21"/>
+      <c r="AC21" s="21"/>
+      <c r="AD21" s="21"/>
+      <c r="AE21" s="21"/>
+      <c r="AF21" s="21"/>
+      <c r="AG21" s="21"/>
+      <c r="AH21" s="21"/>
       <c r="AI21" s="11"/>
       <c r="AJ21" s="11"/>
       <c r="AK21" s="11"/>
@@ -3631,24 +3555,23 @@
       <c r="N22" s="11"/>
       <c r="O22" s="11"/>
       <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="11"/>
-      <c r="U22" s="27"/>
-      <c r="V22" s="28"/>
-      <c r="W22" s="28"/>
-      <c r="X22" s="28"/>
-      <c r="Y22" s="28"/>
-      <c r="Z22" s="28"/>
-      <c r="AA22" s="28"/>
-      <c r="AB22" s="28"/>
-      <c r="AC22" s="28"/>
-      <c r="AD22" s="29"/>
-      <c r="AE22" s="11"/>
-      <c r="AF22" s="11"/>
-      <c r="AG22" s="11"/>
-      <c r="AH22" s="11"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="21"/>
+      <c r="V22" s="21"/>
+      <c r="W22" s="21"/>
+      <c r="X22" s="21"/>
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="21"/>
+      <c r="AB22" s="21"/>
+      <c r="AC22" s="21"/>
+      <c r="AD22" s="21"/>
+      <c r="AE22" s="21"/>
+      <c r="AF22" s="21"/>
+      <c r="AG22" s="21"/>
+      <c r="AH22" s="21"/>
       <c r="AI22" s="11"/>
       <c r="AJ22" s="11"/>
       <c r="AK22" s="11"/>
@@ -3681,18 +3604,24 @@
       <c r="N23" s="11"/>
       <c r="O23" s="11"/>
       <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="AC23" s="11"/>
-      <c r="AD23" s="11"/>
-      <c r="AE23" s="11"/>
-      <c r="AF23" s="11"/>
-      <c r="AG23" s="11"/>
-      <c r="AH23" s="11"/>
+      <c r="Q23" s="21"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="21"/>
+      <c r="U23" s="21"/>
+      <c r="V23" s="21"/>
+      <c r="W23" s="21"/>
+      <c r="X23" s="21"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="21"/>
+      <c r="AB23" s="21"/>
+      <c r="AC23" s="21"/>
+      <c r="AD23" s="21"/>
+      <c r="AE23" s="21"/>
+      <c r="AF23" s="21"/>
+      <c r="AG23" s="21"/>
+      <c r="AH23" s="21"/>
       <c r="AI23" s="11"/>
       <c r="AJ23" s="11"/>
       <c r="AK23" s="11"/>
@@ -3725,18 +3654,24 @@
       <c r="N24" s="11"/>
       <c r="O24" s="11"/>
       <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="11"/>
-      <c r="T24" s="11"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="AC24" s="11"/>
-      <c r="AD24" s="11"/>
-      <c r="AE24" s="11"/>
-      <c r="AF24" s="11"/>
-      <c r="AG24" s="11"/>
-      <c r="AH24" s="11"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="21"/>
+      <c r="V24" s="21"/>
+      <c r="W24" s="21"/>
+      <c r="X24" s="21"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="21"/>
+      <c r="AB24" s="21"/>
+      <c r="AC24" s="21"/>
+      <c r="AD24" s="21"/>
+      <c r="AE24" s="21"/>
+      <c r="AF24" s="21"/>
+      <c r="AG24" s="21"/>
+      <c r="AH24" s="21"/>
       <c r="AI24" s="11"/>
       <c r="AJ24" s="11"/>
       <c r="AK24" s="11"/>
@@ -3940,13 +3875,17 @@
       <c r="AW28" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="S4:AA7"/>
     <mergeCell ref="AB6:AE8"/>
-    <mergeCell ref="U21:AD22"/>
+    <mergeCell ref="Q21:X24"/>
+    <mergeCell ref="AA21:AH24"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="W21:AB22" location="Lobby!A1" display="Register"/>
+    <hyperlink ref="AA21:AF22" location="Register!A1" display="Register"/>
+    <hyperlink ref="S21:X22" location="Lobby!A1" display="Login"/>
+    <hyperlink ref="Q21:X24" location="Login!A1" display="Back"/>
+    <hyperlink ref="AA21:AH24" location="Lobby!A1" display="Register"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3957,9 +3896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AG25" sqref="AG25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3973,17 +3910,17 @@
     <row r="2" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -4234,12 +4171,12 @@
       <c r="AO7" s="11"/>
       <c r="AP7" s="18"/>
       <c r="AQ7" s="19"/>
-      <c r="AR7" s="36" t="s">
+      <c r="AR7" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="AS7" s="36"/>
-      <c r="AT7" s="36"/>
-      <c r="AU7" s="36"/>
+      <c r="AS7" s="33"/>
+      <c r="AT7" s="33"/>
+      <c r="AU7" s="33"/>
       <c r="AV7" s="19"/>
       <c r="AW7" s="20"/>
     </row>
@@ -4247,44 +4184,44 @@
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
       <c r="O8" s="11"/>
-      <c r="P8" s="35" t="s">
+      <c r="P8" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="35"/>
-      <c r="T8" s="35"/>
-      <c r="U8" s="35"/>
-      <c r="V8" s="35"/>
-      <c r="W8" s="35"/>
-      <c r="X8" s="35"/>
-      <c r="Y8" s="35"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="27"/>
+      <c r="Y8" s="27"/>
       <c r="Z8" s="3"/>
-      <c r="AA8" s="35" t="s">
+      <c r="AA8" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="AB8" s="35"/>
-      <c r="AC8" s="35"/>
-      <c r="AD8" s="35"/>
-      <c r="AE8" s="35"/>
-      <c r="AF8" s="35"/>
-      <c r="AG8" s="35"/>
-      <c r="AH8" s="35"/>
-      <c r="AI8" s="35"/>
-      <c r="AJ8" s="35"/>
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+      <c r="AD8" s="27"/>
+      <c r="AE8" s="27"/>
+      <c r="AF8" s="27"/>
+      <c r="AG8" s="27"/>
+      <c r="AH8" s="27"/>
+      <c r="AI8" s="27"/>
+      <c r="AJ8" s="27"/>
       <c r="AK8" s="12"/>
       <c r="AL8" s="11"/>
       <c r="AM8" s="11"/>
@@ -4303,38 +4240,38 @@
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
       <c r="O9" s="11"/>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="35"/>
-      <c r="T9" s="35"/>
-      <c r="U9" s="35"/>
-      <c r="V9" s="35"/>
-      <c r="W9" s="35"/>
-      <c r="X9" s="35"/>
-      <c r="Y9" s="35"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="27"/>
+      <c r="U9" s="27"/>
+      <c r="V9" s="27"/>
+      <c r="W9" s="27"/>
+      <c r="X9" s="27"/>
+      <c r="Y9" s="27"/>
       <c r="Z9" s="3"/>
-      <c r="AA9" s="35"/>
-      <c r="AB9" s="35"/>
-      <c r="AC9" s="35"/>
-      <c r="AD9" s="35"/>
-      <c r="AE9" s="35"/>
-      <c r="AF9" s="35"/>
-      <c r="AG9" s="35"/>
-      <c r="AH9" s="35"/>
-      <c r="AI9" s="35"/>
-      <c r="AJ9" s="35"/>
+      <c r="AA9" s="27"/>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="27"/>
+      <c r="AD9" s="27"/>
+      <c r="AE9" s="27"/>
+      <c r="AF9" s="27"/>
+      <c r="AG9" s="27"/>
+      <c r="AH9" s="27"/>
+      <c r="AI9" s="27"/>
+      <c r="AJ9" s="27"/>
       <c r="AK9" s="4"/>
       <c r="AP9" s="10"/>
       <c r="AQ9" s="3"/>
@@ -4349,38 +4286,38 @@
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
       <c r="O10" s="11"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="35"/>
-      <c r="S10" s="35"/>
-      <c r="T10" s="35"/>
-      <c r="U10" s="35"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="35"/>
-      <c r="X10" s="35"/>
-      <c r="Y10" s="35"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="27"/>
+      <c r="X10" s="27"/>
+      <c r="Y10" s="27"/>
       <c r="Z10" s="3"/>
-      <c r="AA10" s="35"/>
-      <c r="AB10" s="35"/>
-      <c r="AC10" s="35"/>
-      <c r="AD10" s="35"/>
-      <c r="AE10" s="35"/>
-      <c r="AF10" s="35"/>
-      <c r="AG10" s="35"/>
-      <c r="AH10" s="35"/>
-      <c r="AI10" s="35"/>
-      <c r="AJ10" s="35"/>
+      <c r="AA10" s="27"/>
+      <c r="AB10" s="27"/>
+      <c r="AC10" s="27"/>
+      <c r="AD10" s="27"/>
+      <c r="AE10" s="27"/>
+      <c r="AF10" s="27"/>
+      <c r="AG10" s="27"/>
+      <c r="AH10" s="27"/>
+      <c r="AI10" s="27"/>
+      <c r="AJ10" s="27"/>
       <c r="AK10" s="4"/>
       <c r="AP10" s="10"/>
       <c r="AQ10" s="11"/>
@@ -4441,44 +4378,44 @@
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="35"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
       <c r="O12" s="11"/>
-      <c r="P12" s="35" t="s">
+      <c r="P12" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="35"/>
-      <c r="T12" s="35"/>
-      <c r="U12" s="35"/>
-      <c r="V12" s="35"/>
-      <c r="W12" s="35"/>
-      <c r="X12" s="35"/>
-      <c r="Y12" s="35"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="27"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="27"/>
+      <c r="Y12" s="27"/>
       <c r="Z12" s="3"/>
-      <c r="AA12" s="35" t="s">
+      <c r="AA12" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="AB12" s="35"/>
-      <c r="AC12" s="35"/>
-      <c r="AD12" s="35"/>
-      <c r="AE12" s="35"/>
-      <c r="AF12" s="35"/>
-      <c r="AG12" s="35"/>
-      <c r="AH12" s="35"/>
-      <c r="AI12" s="35"/>
-      <c r="AJ12" s="35"/>
+      <c r="AB12" s="27"/>
+      <c r="AC12" s="27"/>
+      <c r="AD12" s="27"/>
+      <c r="AE12" s="27"/>
+      <c r="AF12" s="27"/>
+      <c r="AG12" s="27"/>
+      <c r="AH12" s="27"/>
+      <c r="AI12" s="27"/>
+      <c r="AJ12" s="27"/>
       <c r="AK12" s="4"/>
       <c r="AP12" s="10"/>
       <c r="AQ12" s="11"/>
@@ -4493,38 +4430,38 @@
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
       <c r="O13" s="11"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="35"/>
-      <c r="U13" s="35"/>
-      <c r="V13" s="35"/>
-      <c r="W13" s="35"/>
-      <c r="X13" s="35"/>
-      <c r="Y13" s="35"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="27"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="27"/>
       <c r="Z13" s="3"/>
-      <c r="AA13" s="35"/>
-      <c r="AB13" s="35"/>
-      <c r="AC13" s="35"/>
-      <c r="AD13" s="35"/>
-      <c r="AE13" s="35"/>
-      <c r="AF13" s="35"/>
-      <c r="AG13" s="35"/>
-      <c r="AH13" s="35"/>
-      <c r="AI13" s="35"/>
-      <c r="AJ13" s="35"/>
+      <c r="AA13" s="27"/>
+      <c r="AB13" s="27"/>
+      <c r="AC13" s="27"/>
+      <c r="AD13" s="27"/>
+      <c r="AE13" s="27"/>
+      <c r="AF13" s="27"/>
+      <c r="AG13" s="27"/>
+      <c r="AH13" s="27"/>
+      <c r="AI13" s="27"/>
+      <c r="AJ13" s="27"/>
       <c r="AK13" s="4"/>
       <c r="AP13" s="10"/>
       <c r="AQ13" s="11"/>
@@ -4539,38 +4476,38 @@
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
       <c r="O14" s="11"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
-      <c r="X14" s="35"/>
-      <c r="Y14" s="35"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27"/>
       <c r="Z14" s="3"/>
-      <c r="AA14" s="35"/>
-      <c r="AB14" s="35"/>
-      <c r="AC14" s="35"/>
-      <c r="AD14" s="35"/>
-      <c r="AE14" s="35"/>
-      <c r="AF14" s="35"/>
-      <c r="AG14" s="35"/>
-      <c r="AH14" s="35"/>
-      <c r="AI14" s="35"/>
-      <c r="AJ14" s="35"/>
+      <c r="AA14" s="27"/>
+      <c r="AB14" s="27"/>
+      <c r="AC14" s="27"/>
+      <c r="AD14" s="27"/>
+      <c r="AE14" s="27"/>
+      <c r="AF14" s="27"/>
+      <c r="AG14" s="27"/>
+      <c r="AH14" s="27"/>
+      <c r="AI14" s="27"/>
+      <c r="AJ14" s="27"/>
       <c r="AK14" s="4"/>
       <c r="AP14" s="10"/>
       <c r="AQ14" s="11"/>
@@ -4631,44 +4568,44 @@
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
       <c r="O16" s="11"/>
-      <c r="P16" s="35" t="s">
+      <c r="P16" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
-      <c r="X16" s="35"/>
-      <c r="Y16" s="35"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27"/>
+      <c r="U16" s="27"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="27"/>
+      <c r="X16" s="27"/>
+      <c r="Y16" s="27"/>
       <c r="Z16" s="3"/>
-      <c r="AA16" s="35" t="s">
+      <c r="AA16" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="AB16" s="35"/>
-      <c r="AC16" s="35"/>
-      <c r="AD16" s="35"/>
-      <c r="AE16" s="35"/>
-      <c r="AF16" s="35"/>
-      <c r="AG16" s="35"/>
-      <c r="AH16" s="35"/>
-      <c r="AI16" s="35"/>
-      <c r="AJ16" s="35"/>
+      <c r="AB16" s="27"/>
+      <c r="AC16" s="27"/>
+      <c r="AD16" s="27"/>
+      <c r="AE16" s="27"/>
+      <c r="AF16" s="27"/>
+      <c r="AG16" s="27"/>
+      <c r="AH16" s="27"/>
+      <c r="AI16" s="27"/>
+      <c r="AJ16" s="27"/>
       <c r="AK16" s="4"/>
       <c r="AP16" s="10"/>
       <c r="AQ16" s="11"/>
@@ -4683,38 +4620,38 @@
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
       <c r="O17" s="11"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="35"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
-      <c r="X17" s="35"/>
-      <c r="Y17" s="35"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="27"/>
+      <c r="S17" s="27"/>
+      <c r="T17" s="27"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="27"/>
+      <c r="Y17" s="27"/>
       <c r="Z17" s="3"/>
-      <c r="AA17" s="35"/>
-      <c r="AB17" s="35"/>
-      <c r="AC17" s="35"/>
-      <c r="AD17" s="35"/>
-      <c r="AE17" s="35"/>
-      <c r="AF17" s="35"/>
-      <c r="AG17" s="35"/>
-      <c r="AH17" s="35"/>
-      <c r="AI17" s="35"/>
-      <c r="AJ17" s="35"/>
+      <c r="AA17" s="27"/>
+      <c r="AB17" s="27"/>
+      <c r="AC17" s="27"/>
+      <c r="AD17" s="27"/>
+      <c r="AE17" s="27"/>
+      <c r="AF17" s="27"/>
+      <c r="AG17" s="27"/>
+      <c r="AH17" s="27"/>
+      <c r="AI17" s="27"/>
+      <c r="AJ17" s="27"/>
       <c r="AK17" s="4"/>
       <c r="AP17" s="10"/>
       <c r="AQ17" s="11"/>
@@ -4729,38 +4666,38 @@
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
       <c r="D18" s="10"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
       <c r="O18" s="11"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
-      <c r="X18" s="35"/>
-      <c r="Y18" s="35"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="27"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="27"/>
+      <c r="V18" s="27"/>
+      <c r="W18" s="27"/>
+      <c r="X18" s="27"/>
+      <c r="Y18" s="27"/>
       <c r="Z18" s="3"/>
-      <c r="AA18" s="35"/>
-      <c r="AB18" s="35"/>
-      <c r="AC18" s="35"/>
-      <c r="AD18" s="35"/>
-      <c r="AE18" s="35"/>
-      <c r="AF18" s="35"/>
-      <c r="AG18" s="35"/>
-      <c r="AH18" s="35"/>
-      <c r="AI18" s="35"/>
-      <c r="AJ18" s="35"/>
+      <c r="AA18" s="27"/>
+      <c r="AB18" s="27"/>
+      <c r="AC18" s="27"/>
+      <c r="AD18" s="27"/>
+      <c r="AE18" s="27"/>
+      <c r="AF18" s="27"/>
+      <c r="AG18" s="27"/>
+      <c r="AH18" s="27"/>
+      <c r="AI18" s="27"/>
+      <c r="AJ18" s="27"/>
       <c r="AK18" s="4"/>
       <c r="AP18" s="10"/>
       <c r="AQ18" s="11"/>
@@ -4821,44 +4758,44 @@
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
       <c r="D20" s="10"/>
-      <c r="E20" s="35" t="s">
+      <c r="E20" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
       <c r="O20" s="11"/>
-      <c r="P20" s="35" t="s">
+      <c r="P20" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="Q20" s="35"/>
-      <c r="R20" s="35"/>
-      <c r="S20" s="35"/>
-      <c r="T20" s="35"/>
-      <c r="U20" s="35"/>
-      <c r="V20" s="35"/>
-      <c r="W20" s="35"/>
-      <c r="X20" s="35"/>
-      <c r="Y20" s="35"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="27"/>
+      <c r="X20" s="27"/>
+      <c r="Y20" s="27"/>
       <c r="Z20" s="3"/>
-      <c r="AA20" s="35" t="s">
+      <c r="AA20" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="AB20" s="35"/>
-      <c r="AC20" s="35"/>
-      <c r="AD20" s="35"/>
-      <c r="AE20" s="35"/>
-      <c r="AF20" s="35"/>
-      <c r="AG20" s="35"/>
-      <c r="AH20" s="35"/>
-      <c r="AI20" s="35"/>
-      <c r="AJ20" s="35"/>
+      <c r="AB20" s="27"/>
+      <c r="AC20" s="27"/>
+      <c r="AD20" s="27"/>
+      <c r="AE20" s="27"/>
+      <c r="AF20" s="27"/>
+      <c r="AG20" s="27"/>
+      <c r="AH20" s="27"/>
+      <c r="AI20" s="27"/>
+      <c r="AJ20" s="27"/>
       <c r="AK20" s="4"/>
       <c r="AP20" s="10"/>
       <c r="AQ20" s="11"/>
@@ -4873,38 +4810,38 @@
       <c r="B21" s="10"/>
       <c r="C21" s="11"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
       <c r="O21" s="11"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="35"/>
-      <c r="S21" s="35"/>
-      <c r="T21" s="35"/>
-      <c r="U21" s="35"/>
-      <c r="V21" s="35"/>
-      <c r="W21" s="35"/>
-      <c r="X21" s="35"/>
-      <c r="Y21" s="35"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="U21" s="27"/>
+      <c r="V21" s="27"/>
+      <c r="W21" s="27"/>
+      <c r="X21" s="27"/>
+      <c r="Y21" s="27"/>
       <c r="Z21" s="3"/>
-      <c r="AA21" s="35"/>
-      <c r="AB21" s="35"/>
-      <c r="AC21" s="35"/>
-      <c r="AD21" s="35"/>
-      <c r="AE21" s="35"/>
-      <c r="AF21" s="35"/>
-      <c r="AG21" s="35"/>
-      <c r="AH21" s="35"/>
-      <c r="AI21" s="35"/>
-      <c r="AJ21" s="35"/>
+      <c r="AA21" s="27"/>
+      <c r="AB21" s="27"/>
+      <c r="AC21" s="27"/>
+      <c r="AD21" s="27"/>
+      <c r="AE21" s="27"/>
+      <c r="AF21" s="27"/>
+      <c r="AG21" s="27"/>
+      <c r="AH21" s="27"/>
+      <c r="AI21" s="27"/>
+      <c r="AJ21" s="27"/>
       <c r="AK21" s="4"/>
       <c r="AP21" s="10"/>
       <c r="AQ21" s="11"/>
@@ -4919,38 +4856,38 @@
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
       <c r="O22" s="11"/>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="35"/>
-      <c r="S22" s="35"/>
-      <c r="T22" s="35"/>
-      <c r="U22" s="35"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="35"/>
-      <c r="X22" s="35"/>
-      <c r="Y22" s="35"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="27"/>
+      <c r="S22" s="27"/>
+      <c r="T22" s="27"/>
+      <c r="U22" s="27"/>
+      <c r="V22" s="27"/>
+      <c r="W22" s="27"/>
+      <c r="X22" s="27"/>
+      <c r="Y22" s="27"/>
       <c r="Z22" s="3"/>
-      <c r="AA22" s="35"/>
-      <c r="AB22" s="35"/>
-      <c r="AC22" s="35"/>
-      <c r="AD22" s="35"/>
-      <c r="AE22" s="35"/>
-      <c r="AF22" s="35"/>
-      <c r="AG22" s="35"/>
-      <c r="AH22" s="35"/>
-      <c r="AI22" s="35"/>
-      <c r="AJ22" s="35"/>
+      <c r="AA22" s="27"/>
+      <c r="AB22" s="27"/>
+      <c r="AC22" s="27"/>
+      <c r="AD22" s="27"/>
+      <c r="AE22" s="27"/>
+      <c r="AF22" s="27"/>
+      <c r="AG22" s="27"/>
+      <c r="AH22" s="27"/>
+      <c r="AI22" s="27"/>
+      <c r="AJ22" s="27"/>
       <c r="AK22" s="4"/>
       <c r="AP22" s="10"/>
       <c r="AQ22" s="11"/>
@@ -5195,16 +5132,16 @@
       <c r="AM27" s="11"/>
       <c r="AN27" s="11"/>
       <c r="AO27" s="11"/>
-      <c r="AP27" s="31" t="s">
+      <c r="AP27" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="AQ27" s="31"/>
-      <c r="AR27" s="31"/>
-      <c r="AS27" s="31"/>
-      <c r="AT27" s="31"/>
-      <c r="AU27" s="31"/>
-      <c r="AV27" s="31"/>
-      <c r="AW27" s="32"/>
+      <c r="AQ27" s="29"/>
+      <c r="AR27" s="29"/>
+      <c r="AS27" s="29"/>
+      <c r="AT27" s="29"/>
+      <c r="AU27" s="29"/>
+      <c r="AV27" s="29"/>
+      <c r="AW27" s="30"/>
     </row>
     <row r="28" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="13"/>
@@ -5247,22 +5184,17 @@
       <c r="AM28" s="14"/>
       <c r="AN28" s="14"/>
       <c r="AO28" s="14"/>
-      <c r="AP28" s="33"/>
-      <c r="AQ28" s="33"/>
-      <c r="AR28" s="33"/>
-      <c r="AS28" s="33"/>
-      <c r="AT28" s="33"/>
-      <c r="AU28" s="33"/>
-      <c r="AV28" s="33"/>
-      <c r="AW28" s="34"/>
+      <c r="AP28" s="31"/>
+      <c r="AQ28" s="31"/>
+      <c r="AR28" s="31"/>
+      <c r="AS28" s="31"/>
+      <c r="AT28" s="31"/>
+      <c r="AU28" s="31"/>
+      <c r="AV28" s="31"/>
+      <c r="AW28" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="AA12:AJ14"/>
-    <mergeCell ref="AA16:AJ18"/>
-    <mergeCell ref="AA20:AJ22"/>
-    <mergeCell ref="D2:L5"/>
-    <mergeCell ref="M4:P6"/>
     <mergeCell ref="AP27:AW28"/>
     <mergeCell ref="AU3:AV4"/>
     <mergeCell ref="E8:N10"/>
@@ -5277,6 +5209,11 @@
     <mergeCell ref="P16:Y18"/>
     <mergeCell ref="P20:Y22"/>
     <mergeCell ref="AA8:AJ10"/>
+    <mergeCell ref="AA12:AJ14"/>
+    <mergeCell ref="AA16:AJ18"/>
+    <mergeCell ref="AA20:AJ22"/>
+    <mergeCell ref="D2:L5"/>
+    <mergeCell ref="M4:P6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="V25:AA26" location="CreateRoom!A1" display="Create Room"/>
@@ -5319,17 +5256,17 @@
     <row r="2" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -5580,12 +5517,12 @@
       <c r="AO7" s="11"/>
       <c r="AP7" s="18"/>
       <c r="AQ7" s="19"/>
-      <c r="AR7" s="36" t="s">
+      <c r="AR7" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="AS7" s="36"/>
-      <c r="AT7" s="36"/>
-      <c r="AU7" s="36"/>
+      <c r="AS7" s="33"/>
+      <c r="AT7" s="33"/>
+      <c r="AU7" s="33"/>
       <c r="AV7" s="19"/>
       <c r="AW7" s="20"/>
     </row>
@@ -5594,40 +5531,40 @@
       <c r="C8" s="11"/>
       <c r="D8" s="10"/>
       <c r="E8" s="17"/>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="38"/>
-      <c r="S8" s="39"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="35"/>
+      <c r="S8" s="36"/>
       <c r="T8" s="17"/>
       <c r="U8" s="17"/>
-      <c r="V8" s="37" t="s">
+      <c r="V8" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="W8" s="38"/>
-      <c r="X8" s="38"/>
-      <c r="Y8" s="38"/>
-      <c r="Z8" s="38"/>
-      <c r="AA8" s="38"/>
-      <c r="AB8" s="38"/>
-      <c r="AC8" s="38"/>
-      <c r="AD8" s="38"/>
-      <c r="AE8" s="38"/>
-      <c r="AF8" s="38"/>
-      <c r="AG8" s="38"/>
-      <c r="AH8" s="38"/>
-      <c r="AI8" s="39"/>
+      <c r="W8" s="35"/>
+      <c r="X8" s="35"/>
+      <c r="Y8" s="35"/>
+      <c r="Z8" s="35"/>
+      <c r="AA8" s="35"/>
+      <c r="AB8" s="35"/>
+      <c r="AC8" s="35"/>
+      <c r="AD8" s="35"/>
+      <c r="AE8" s="35"/>
+      <c r="AF8" s="35"/>
+      <c r="AG8" s="35"/>
+      <c r="AH8" s="35"/>
+      <c r="AI8" s="36"/>
       <c r="AJ8" s="17"/>
       <c r="AK8" s="12"/>
       <c r="AL8" s="11"/>
@@ -5648,36 +5585,36 @@
       <c r="C9" s="11"/>
       <c r="D9" s="10"/>
       <c r="E9" s="17"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="41"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="41"/>
-      <c r="S9" s="42"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="39"/>
       <c r="T9" s="17"/>
       <c r="U9" s="17"/>
-      <c r="V9" s="40"/>
-      <c r="W9" s="41"/>
-      <c r="X9" s="41"/>
-      <c r="Y9" s="41"/>
-      <c r="Z9" s="41"/>
-      <c r="AA9" s="41"/>
-      <c r="AB9" s="41"/>
-      <c r="AC9" s="41"/>
-      <c r="AD9" s="41"/>
-      <c r="AE9" s="41"/>
-      <c r="AF9" s="41"/>
-      <c r="AG9" s="41"/>
-      <c r="AH9" s="41"/>
-      <c r="AI9" s="42"/>
+      <c r="V9" s="37"/>
+      <c r="W9" s="38"/>
+      <c r="X9" s="38"/>
+      <c r="Y9" s="38"/>
+      <c r="Z9" s="38"/>
+      <c r="AA9" s="38"/>
+      <c r="AB9" s="38"/>
+      <c r="AC9" s="38"/>
+      <c r="AD9" s="38"/>
+      <c r="AE9" s="38"/>
+      <c r="AF9" s="38"/>
+      <c r="AG9" s="38"/>
+      <c r="AH9" s="38"/>
+      <c r="AI9" s="39"/>
       <c r="AJ9" s="17"/>
       <c r="AK9" s="4"/>
       <c r="AP9" s="10"/>
@@ -5694,36 +5631,36 @@
       <c r="C10" s="11"/>
       <c r="D10" s="10"/>
       <c r="E10" s="17"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="41"/>
-      <c r="S10" s="42"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="39"/>
       <c r="T10" s="17"/>
       <c r="U10" s="17"/>
-      <c r="V10" s="40"/>
-      <c r="W10" s="41"/>
-      <c r="X10" s="41"/>
-      <c r="Y10" s="41"/>
-      <c r="Z10" s="41"/>
-      <c r="AA10" s="41"/>
-      <c r="AB10" s="41"/>
-      <c r="AC10" s="41"/>
-      <c r="AD10" s="41"/>
-      <c r="AE10" s="41"/>
-      <c r="AF10" s="41"/>
-      <c r="AG10" s="41"/>
-      <c r="AH10" s="41"/>
-      <c r="AI10" s="42"/>
+      <c r="V10" s="37"/>
+      <c r="W10" s="38"/>
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="38"/>
+      <c r="AA10" s="38"/>
+      <c r="AB10" s="38"/>
+      <c r="AC10" s="38"/>
+      <c r="AD10" s="38"/>
+      <c r="AE10" s="38"/>
+      <c r="AF10" s="38"/>
+      <c r="AG10" s="38"/>
+      <c r="AH10" s="38"/>
+      <c r="AI10" s="39"/>
       <c r="AJ10" s="17"/>
       <c r="AK10" s="4"/>
       <c r="AP10" s="10"/>
@@ -5739,34 +5676,34 @@
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="10"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
-      <c r="N11" s="41"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="41"/>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="41"/>
-      <c r="S11" s="42"/>
-      <c r="V11" s="40"/>
-      <c r="W11" s="41"/>
-      <c r="X11" s="41"/>
-      <c r="Y11" s="41"/>
-      <c r="Z11" s="41"/>
-      <c r="AA11" s="41"/>
-      <c r="AB11" s="41"/>
-      <c r="AC11" s="41"/>
-      <c r="AD11" s="41"/>
-      <c r="AE11" s="41"/>
-      <c r="AF11" s="41"/>
-      <c r="AG11" s="41"/>
-      <c r="AH11" s="41"/>
-      <c r="AI11" s="42"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="39"/>
+      <c r="V11" s="37"/>
+      <c r="W11" s="38"/>
+      <c r="X11" s="38"/>
+      <c r="Y11" s="38"/>
+      <c r="Z11" s="38"/>
+      <c r="AA11" s="38"/>
+      <c r="AB11" s="38"/>
+      <c r="AC11" s="38"/>
+      <c r="AD11" s="38"/>
+      <c r="AE11" s="38"/>
+      <c r="AF11" s="38"/>
+      <c r="AG11" s="38"/>
+      <c r="AH11" s="38"/>
+      <c r="AI11" s="39"/>
       <c r="AK11" s="4"/>
       <c r="AP11" s="10"/>
       <c r="AQ11" s="11"/>
@@ -5782,36 +5719,36 @@
       <c r="C12" s="11"/>
       <c r="D12" s="10"/>
       <c r="E12" s="17"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="41"/>
-      <c r="S12" s="42"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="39"/>
       <c r="T12" s="17"/>
       <c r="U12" s="17"/>
-      <c r="V12" s="40"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="41"/>
-      <c r="Y12" s="41"/>
-      <c r="Z12" s="41"/>
-      <c r="AA12" s="41"/>
-      <c r="AB12" s="41"/>
-      <c r="AC12" s="41"/>
-      <c r="AD12" s="41"/>
-      <c r="AE12" s="41"/>
-      <c r="AF12" s="41"/>
-      <c r="AG12" s="41"/>
-      <c r="AH12" s="41"/>
-      <c r="AI12" s="42"/>
+      <c r="V12" s="37"/>
+      <c r="W12" s="38"/>
+      <c r="X12" s="38"/>
+      <c r="Y12" s="38"/>
+      <c r="Z12" s="38"/>
+      <c r="AA12" s="38"/>
+      <c r="AB12" s="38"/>
+      <c r="AC12" s="38"/>
+      <c r="AD12" s="38"/>
+      <c r="AE12" s="38"/>
+      <c r="AF12" s="38"/>
+      <c r="AG12" s="38"/>
+      <c r="AH12" s="38"/>
+      <c r="AI12" s="39"/>
       <c r="AJ12" s="17"/>
       <c r="AK12" s="4"/>
       <c r="AP12" s="10"/>
@@ -5828,36 +5765,36 @@
       <c r="C13" s="11"/>
       <c r="D13" s="10"/>
       <c r="E13" s="17"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="41"/>
-      <c r="R13" s="41"/>
-      <c r="S13" s="42"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="38"/>
+      <c r="S13" s="39"/>
       <c r="T13" s="17"/>
       <c r="U13" s="17"/>
-      <c r="V13" s="40"/>
-      <c r="W13" s="41"/>
-      <c r="X13" s="41"/>
-      <c r="Y13" s="41"/>
-      <c r="Z13" s="41"/>
-      <c r="AA13" s="41"/>
-      <c r="AB13" s="41"/>
-      <c r="AC13" s="41"/>
-      <c r="AD13" s="41"/>
-      <c r="AE13" s="41"/>
-      <c r="AF13" s="41"/>
-      <c r="AG13" s="41"/>
-      <c r="AH13" s="41"/>
-      <c r="AI13" s="42"/>
+      <c r="V13" s="37"/>
+      <c r="W13" s="38"/>
+      <c r="X13" s="38"/>
+      <c r="Y13" s="38"/>
+      <c r="Z13" s="38"/>
+      <c r="AA13" s="38"/>
+      <c r="AB13" s="38"/>
+      <c r="AC13" s="38"/>
+      <c r="AD13" s="38"/>
+      <c r="AE13" s="38"/>
+      <c r="AF13" s="38"/>
+      <c r="AG13" s="38"/>
+      <c r="AH13" s="38"/>
+      <c r="AI13" s="39"/>
       <c r="AJ13" s="17"/>
       <c r="AK13" s="4"/>
       <c r="AP13" s="10"/>
@@ -5874,36 +5811,36 @@
       <c r="C14" s="11"/>
       <c r="D14" s="10"/>
       <c r="E14" s="17"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="41"/>
-      <c r="S14" s="42"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="38"/>
+      <c r="S14" s="39"/>
       <c r="T14" s="17"/>
       <c r="U14" s="17"/>
-      <c r="V14" s="40"/>
-      <c r="W14" s="41"/>
-      <c r="X14" s="41"/>
-      <c r="Y14" s="41"/>
-      <c r="Z14" s="41"/>
-      <c r="AA14" s="41"/>
-      <c r="AB14" s="41"/>
-      <c r="AC14" s="41"/>
-      <c r="AD14" s="41"/>
-      <c r="AE14" s="41"/>
-      <c r="AF14" s="41"/>
-      <c r="AG14" s="41"/>
-      <c r="AH14" s="41"/>
-      <c r="AI14" s="42"/>
+      <c r="V14" s="37"/>
+      <c r="W14" s="38"/>
+      <c r="X14" s="38"/>
+      <c r="Y14" s="38"/>
+      <c r="Z14" s="38"/>
+      <c r="AA14" s="38"/>
+      <c r="AB14" s="38"/>
+      <c r="AC14" s="38"/>
+      <c r="AD14" s="38"/>
+      <c r="AE14" s="38"/>
+      <c r="AF14" s="38"/>
+      <c r="AG14" s="38"/>
+      <c r="AH14" s="38"/>
+      <c r="AI14" s="39"/>
       <c r="AJ14" s="17"/>
       <c r="AK14" s="4"/>
       <c r="AP14" s="10"/>
@@ -5919,34 +5856,34 @@
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
       <c r="D15" s="10"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="41"/>
-      <c r="P15" s="41"/>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="41"/>
-      <c r="S15" s="42"/>
-      <c r="V15" s="40"/>
-      <c r="W15" s="41"/>
-      <c r="X15" s="41"/>
-      <c r="Y15" s="41"/>
-      <c r="Z15" s="41"/>
-      <c r="AA15" s="41"/>
-      <c r="AB15" s="41"/>
-      <c r="AC15" s="41"/>
-      <c r="AD15" s="41"/>
-      <c r="AE15" s="41"/>
-      <c r="AF15" s="41"/>
-      <c r="AG15" s="41"/>
-      <c r="AH15" s="41"/>
-      <c r="AI15" s="42"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
+      <c r="S15" s="39"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="38"/>
+      <c r="X15" s="38"/>
+      <c r="Y15" s="38"/>
+      <c r="Z15" s="38"/>
+      <c r="AA15" s="38"/>
+      <c r="AB15" s="38"/>
+      <c r="AC15" s="38"/>
+      <c r="AD15" s="38"/>
+      <c r="AE15" s="38"/>
+      <c r="AF15" s="38"/>
+      <c r="AG15" s="38"/>
+      <c r="AH15" s="38"/>
+      <c r="AI15" s="39"/>
       <c r="AK15" s="4"/>
       <c r="AP15" s="10"/>
       <c r="AQ15" s="11"/>
@@ -5962,36 +5899,36 @@
       <c r="C16" s="11"/>
       <c r="D16" s="10"/>
       <c r="E16" s="17"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="41"/>
-      <c r="P16" s="41"/>
-      <c r="Q16" s="41"/>
-      <c r="R16" s="41"/>
-      <c r="S16" s="42"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="38"/>
+      <c r="S16" s="39"/>
       <c r="T16" s="17"/>
       <c r="U16" s="17"/>
-      <c r="V16" s="40"/>
-      <c r="W16" s="41"/>
-      <c r="X16" s="41"/>
-      <c r="Y16" s="41"/>
-      <c r="Z16" s="41"/>
-      <c r="AA16" s="41"/>
-      <c r="AB16" s="41"/>
-      <c r="AC16" s="41"/>
-      <c r="AD16" s="41"/>
-      <c r="AE16" s="41"/>
-      <c r="AF16" s="41"/>
-      <c r="AG16" s="41"/>
-      <c r="AH16" s="41"/>
-      <c r="AI16" s="42"/>
+      <c r="V16" s="37"/>
+      <c r="W16" s="38"/>
+      <c r="X16" s="38"/>
+      <c r="Y16" s="38"/>
+      <c r="Z16" s="38"/>
+      <c r="AA16" s="38"/>
+      <c r="AB16" s="38"/>
+      <c r="AC16" s="38"/>
+      <c r="AD16" s="38"/>
+      <c r="AE16" s="38"/>
+      <c r="AF16" s="38"/>
+      <c r="AG16" s="38"/>
+      <c r="AH16" s="38"/>
+      <c r="AI16" s="39"/>
       <c r="AJ16" s="17"/>
       <c r="AK16" s="4"/>
       <c r="AP16" s="10"/>
@@ -6008,36 +5945,36 @@
       <c r="C17" s="11"/>
       <c r="D17" s="10"/>
       <c r="E17" s="17"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="41"/>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="41"/>
-      <c r="R17" s="41"/>
-      <c r="S17" s="42"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="39"/>
       <c r="T17" s="17"/>
       <c r="U17" s="17"/>
-      <c r="V17" s="40"/>
-      <c r="W17" s="41"/>
-      <c r="X17" s="41"/>
-      <c r="Y17" s="41"/>
-      <c r="Z17" s="41"/>
-      <c r="AA17" s="41"/>
-      <c r="AB17" s="41"/>
-      <c r="AC17" s="41"/>
-      <c r="AD17" s="41"/>
-      <c r="AE17" s="41"/>
-      <c r="AF17" s="41"/>
-      <c r="AG17" s="41"/>
-      <c r="AH17" s="41"/>
-      <c r="AI17" s="42"/>
+      <c r="V17" s="37"/>
+      <c r="W17" s="38"/>
+      <c r="X17" s="38"/>
+      <c r="Y17" s="38"/>
+      <c r="Z17" s="38"/>
+      <c r="AA17" s="38"/>
+      <c r="AB17" s="38"/>
+      <c r="AC17" s="38"/>
+      <c r="AD17" s="38"/>
+      <c r="AE17" s="38"/>
+      <c r="AF17" s="38"/>
+      <c r="AG17" s="38"/>
+      <c r="AH17" s="38"/>
+      <c r="AI17" s="39"/>
       <c r="AJ17" s="17"/>
       <c r="AK17" s="4"/>
       <c r="AP17" s="10"/>
@@ -6054,36 +5991,36 @@
       <c r="C18" s="11"/>
       <c r="D18" s="10"/>
       <c r="E18" s="17"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="44"/>
-      <c r="N18" s="44"/>
-      <c r="O18" s="44"/>
-      <c r="P18" s="44"/>
-      <c r="Q18" s="44"/>
-      <c r="R18" s="44"/>
-      <c r="S18" s="45"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="41"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="42"/>
       <c r="T18" s="17"/>
       <c r="U18" s="17"/>
-      <c r="V18" s="43"/>
-      <c r="W18" s="44"/>
-      <c r="X18" s="44"/>
-      <c r="Y18" s="44"/>
-      <c r="Z18" s="44"/>
-      <c r="AA18" s="44"/>
-      <c r="AB18" s="44"/>
-      <c r="AC18" s="44"/>
-      <c r="AD18" s="44"/>
-      <c r="AE18" s="44"/>
-      <c r="AF18" s="44"/>
-      <c r="AG18" s="44"/>
-      <c r="AH18" s="44"/>
-      <c r="AI18" s="45"/>
+      <c r="V18" s="40"/>
+      <c r="W18" s="41"/>
+      <c r="X18" s="41"/>
+      <c r="Y18" s="41"/>
+      <c r="Z18" s="41"/>
+      <c r="AA18" s="41"/>
+      <c r="AB18" s="41"/>
+      <c r="AC18" s="41"/>
+      <c r="AD18" s="41"/>
+      <c r="AE18" s="41"/>
+      <c r="AF18" s="41"/>
+      <c r="AG18" s="41"/>
+      <c r="AH18" s="41"/>
+      <c r="AI18" s="42"/>
       <c r="AJ18" s="17"/>
       <c r="AK18" s="4"/>
       <c r="AP18" s="10"/>
@@ -6115,38 +6052,38 @@
       <c r="D20" s="10"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
-      <c r="G20" s="46" t="s">
+      <c r="G20" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="47"/>
-      <c r="P20" s="47"/>
-      <c r="Q20" s="47"/>
-      <c r="R20" s="48"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="44"/>
+      <c r="P20" s="44"/>
+      <c r="Q20" s="44"/>
+      <c r="R20" s="45"/>
       <c r="S20" s="17"/>
       <c r="T20" s="17"/>
       <c r="U20" s="17"/>
       <c r="V20" s="17"/>
-      <c r="W20" s="46" t="s">
+      <c r="W20" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="X20" s="47"/>
-      <c r="Y20" s="47"/>
-      <c r="Z20" s="47"/>
-      <c r="AA20" s="47"/>
-      <c r="AB20" s="47"/>
-      <c r="AC20" s="47"/>
-      <c r="AD20" s="47"/>
-      <c r="AE20" s="47"/>
-      <c r="AF20" s="47"/>
-      <c r="AG20" s="47"/>
-      <c r="AH20" s="48"/>
+      <c r="X20" s="44"/>
+      <c r="Y20" s="44"/>
+      <c r="Z20" s="44"/>
+      <c r="AA20" s="44"/>
+      <c r="AB20" s="44"/>
+      <c r="AC20" s="44"/>
+      <c r="AD20" s="44"/>
+      <c r="AE20" s="44"/>
+      <c r="AF20" s="44"/>
+      <c r="AG20" s="44"/>
+      <c r="AH20" s="45"/>
       <c r="AI20" s="17"/>
       <c r="AJ20" s="17"/>
       <c r="AK20" s="4"/>
@@ -6165,34 +6102,34 @@
       <c r="D21" s="10"/>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="50"/>
-      <c r="O21" s="50"/>
-      <c r="P21" s="50"/>
-      <c r="Q21" s="50"/>
-      <c r="R21" s="51"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="47"/>
+      <c r="R21" s="48"/>
       <c r="S21" s="17"/>
       <c r="T21" s="17"/>
       <c r="U21" s="17"/>
       <c r="V21" s="17"/>
-      <c r="W21" s="49"/>
-      <c r="X21" s="50"/>
-      <c r="Y21" s="50"/>
-      <c r="Z21" s="50"/>
-      <c r="AA21" s="50"/>
-      <c r="AB21" s="50"/>
-      <c r="AC21" s="50"/>
-      <c r="AD21" s="50"/>
-      <c r="AE21" s="50"/>
-      <c r="AF21" s="50"/>
-      <c r="AG21" s="50"/>
-      <c r="AH21" s="51"/>
+      <c r="W21" s="46"/>
+      <c r="X21" s="47"/>
+      <c r="Y21" s="47"/>
+      <c r="Z21" s="47"/>
+      <c r="AA21" s="47"/>
+      <c r="AB21" s="47"/>
+      <c r="AC21" s="47"/>
+      <c r="AD21" s="47"/>
+      <c r="AE21" s="47"/>
+      <c r="AF21" s="47"/>
+      <c r="AG21" s="47"/>
+      <c r="AH21" s="48"/>
       <c r="AI21" s="17"/>
       <c r="AJ21" s="17"/>
       <c r="AK21" s="4"/>
@@ -6483,16 +6420,16 @@
       <c r="AM27" s="11"/>
       <c r="AN27" s="11"/>
       <c r="AO27" s="11"/>
-      <c r="AP27" s="31" t="s">
+      <c r="AP27" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="AQ27" s="31"/>
-      <c r="AR27" s="31"/>
-      <c r="AS27" s="31"/>
-      <c r="AT27" s="31"/>
-      <c r="AU27" s="31"/>
-      <c r="AV27" s="31"/>
-      <c r="AW27" s="32"/>
+      <c r="AQ27" s="29"/>
+      <c r="AR27" s="29"/>
+      <c r="AS27" s="29"/>
+      <c r="AT27" s="29"/>
+      <c r="AU27" s="29"/>
+      <c r="AV27" s="29"/>
+      <c r="AW27" s="30"/>
     </row>
     <row r="28" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="13"/>
@@ -6535,28 +6472,28 @@
       <c r="AM28" s="14"/>
       <c r="AN28" s="14"/>
       <c r="AO28" s="14"/>
-      <c r="AP28" s="33"/>
-      <c r="AQ28" s="33"/>
-      <c r="AR28" s="33"/>
-      <c r="AS28" s="33"/>
-      <c r="AT28" s="33"/>
-      <c r="AU28" s="33"/>
-      <c r="AV28" s="33"/>
-      <c r="AW28" s="34"/>
+      <c r="AP28" s="31"/>
+      <c r="AQ28" s="31"/>
+      <c r="AR28" s="31"/>
+      <c r="AS28" s="31"/>
+      <c r="AT28" s="31"/>
+      <c r="AU28" s="31"/>
+      <c r="AV28" s="31"/>
+      <c r="AW28" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D2:L5"/>
+    <mergeCell ref="AU3:AV4"/>
+    <mergeCell ref="M4:P6"/>
+    <mergeCell ref="N25:S26"/>
+    <mergeCell ref="V25:AA26"/>
     <mergeCell ref="AP27:AW28"/>
     <mergeCell ref="AR7:AU7"/>
     <mergeCell ref="F8:S18"/>
     <mergeCell ref="V8:AI18"/>
     <mergeCell ref="G20:R21"/>
     <mergeCell ref="W20:AH21"/>
-    <mergeCell ref="D2:L5"/>
-    <mergeCell ref="AU3:AV4"/>
-    <mergeCell ref="M4:P6"/>
-    <mergeCell ref="N25:S26"/>
-    <mergeCell ref="V25:AA26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N25:S26" location="Lobby!A1" display="Cancel"/>

</xml_diff>

<commit_message>
Implement Lobby Scene (WIP)
</commit_message>
<xml_diff>
--- a/References/Layout.xlsx
+++ b/References/Layout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="420" windowWidth="21795" windowHeight="6180"/>
+    <workbookView xWindow="480" yWindow="420" windowWidth="21795" windowHeight="6180" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <author>Giang</author>
   </authors>
   <commentList>
-    <comment ref="E8" authorId="0">
+    <comment ref="D8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +46,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P8" authorId="0">
+    <comment ref="O8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA8" authorId="0">
+    <comment ref="Z8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0">
+    <comment ref="D12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -118,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P12" authorId="0">
+    <comment ref="O12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA12" authorId="0">
+    <comment ref="Z12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E16" authorId="0">
+    <comment ref="D16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -190,7 +190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P16" authorId="0">
+    <comment ref="O16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -214,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA16" authorId="0">
+    <comment ref="Z16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -238,7 +238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0">
+    <comment ref="D20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -262,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P20" authorId="0">
+    <comment ref="O20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -286,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA20" authorId="0">
+    <comment ref="Z20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -320,7 +320,7 @@
     <author>Giang</author>
   </authors>
   <commentList>
-    <comment ref="W20" authorId="0">
+    <comment ref="V21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -344,7 +344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V25" authorId="0">
+    <comment ref="U25" authorId="0">
       <text>
         <r>
           <rPr>
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
   <si>
     <t>Login</t>
   </si>
@@ -444,12 +444,15 @@
   <si>
     <t>Back</t>
   </si>
+  <si>
+    <t>VS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,6 +529,14 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="40"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -550,7 +561,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -690,66 +701,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -757,7 +708,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -796,18 +747,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
@@ -823,25 +762,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -887,6 +817,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1195,7 +1141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AW28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AZ24" sqref="AZ24"/>
     </sheetView>
   </sheetViews>
@@ -1324,17 +1270,17 @@
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
-      <c r="S4" s="23" t="s">
+      <c r="S4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="23"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="23"/>
-      <c r="AA4" s="23"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
       <c r="AB4" s="16"/>
       <c r="AC4" s="16"/>
       <c r="AD4" s="16"/>
@@ -1376,15 +1322,15 @@
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="23"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
       <c r="AB5" s="16"/>
       <c r="AC5" s="16"/>
       <c r="AD5" s="16"/>
@@ -1426,21 +1372,21 @@
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="23"/>
-      <c r="AB6" s="22" t="s">
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="19"/>
+      <c r="AB6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="AC6" s="22"/>
-      <c r="AD6" s="22"/>
-      <c r="AE6" s="22"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="18"/>
+      <c r="AE6" s="18"/>
       <c r="AF6" s="11"/>
       <c r="AG6" s="11"/>
       <c r="AH6" s="11"/>
@@ -1478,19 +1424,19 @@
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="23"/>
-      <c r="X7" s="23"/>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="23"/>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="22"/>
-      <c r="AC7" s="22"/>
-      <c r="AD7" s="22"/>
-      <c r="AE7" s="22"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="18"/>
+      <c r="AC7" s="18"/>
+      <c r="AD7" s="18"/>
+      <c r="AE7" s="18"/>
       <c r="AF7" s="11"/>
       <c r="AG7" s="11"/>
       <c r="AH7" s="11"/>
@@ -1537,10 +1483,10 @@
       <c r="Y8" s="11"/>
       <c r="Z8" s="11"/>
       <c r="AA8" s="11"/>
-      <c r="AB8" s="22"/>
-      <c r="AC8" s="22"/>
-      <c r="AD8" s="22"/>
-      <c r="AE8" s="22"/>
+      <c r="AB8" s="18"/>
+      <c r="AC8" s="18"/>
+      <c r="AD8" s="18"/>
+      <c r="AE8" s="18"/>
       <c r="AF8" s="11"/>
       <c r="AG8" s="11"/>
       <c r="AH8" s="11"/>
@@ -2084,22 +2030,22 @@
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
-      <c r="S19" s="24" t="s">
+      <c r="S19" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="T19" s="25"/>
-      <c r="U19" s="25"/>
-      <c r="V19" s="25"/>
-      <c r="W19" s="25"/>
-      <c r="X19" s="25"/>
-      <c r="Y19" s="25"/>
-      <c r="Z19" s="25"/>
-      <c r="AA19" s="25"/>
-      <c r="AB19" s="25"/>
-      <c r="AC19" s="25"/>
-      <c r="AD19" s="25"/>
-      <c r="AE19" s="25"/>
-      <c r="AF19" s="26"/>
+      <c r="T19" s="21"/>
+      <c r="U19" s="21"/>
+      <c r="V19" s="21"/>
+      <c r="W19" s="21"/>
+      <c r="X19" s="21"/>
+      <c r="Y19" s="21"/>
+      <c r="Z19" s="21"/>
+      <c r="AA19" s="21"/>
+      <c r="AB19" s="21"/>
+      <c r="AC19" s="21"/>
+      <c r="AD19" s="21"/>
+      <c r="AE19" s="21"/>
+      <c r="AF19" s="22"/>
       <c r="AG19" s="11"/>
       <c r="AH19" s="11"/>
       <c r="AI19" s="11"/>
@@ -2187,27 +2133,27 @@
       <c r="N21" s="11"/>
       <c r="O21" s="11"/>
       <c r="P21" s="11"/>
-      <c r="Q21" s="21" t="s">
+      <c r="Q21" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
+      <c r="X21" s="23"/>
       <c r="Z21" s="11"/>
-      <c r="AA21" s="21" t="s">
+      <c r="AA21" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AB21" s="21"/>
-      <c r="AC21" s="21"/>
-      <c r="AD21" s="21"/>
-      <c r="AE21" s="21"/>
-      <c r="AF21" s="21"/>
-      <c r="AG21" s="21"/>
-      <c r="AH21" s="21"/>
+      <c r="AB21" s="23"/>
+      <c r="AC21" s="23"/>
+      <c r="AD21" s="23"/>
+      <c r="AE21" s="23"/>
+      <c r="AF21" s="23"/>
+      <c r="AG21" s="23"/>
+      <c r="AH21" s="23"/>
       <c r="AI21" s="11"/>
       <c r="AJ21" s="11"/>
       <c r="AK21" s="11"/>
@@ -2240,23 +2186,23 @@
       <c r="N22" s="11"/>
       <c r="O22" s="11"/>
       <c r="P22" s="11"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="21"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="23"/>
+      <c r="W22" s="23"/>
+      <c r="X22" s="23"/>
       <c r="Z22" s="11"/>
-      <c r="AA22" s="21"/>
-      <c r="AB22" s="21"/>
-      <c r="AC22" s="21"/>
-      <c r="AD22" s="21"/>
-      <c r="AE22" s="21"/>
-      <c r="AF22" s="21"/>
-      <c r="AG22" s="21"/>
-      <c r="AH22" s="21"/>
+      <c r="AA22" s="23"/>
+      <c r="AB22" s="23"/>
+      <c r="AC22" s="23"/>
+      <c r="AD22" s="23"/>
+      <c r="AE22" s="23"/>
+      <c r="AF22" s="23"/>
+      <c r="AG22" s="23"/>
+      <c r="AH22" s="23"/>
       <c r="AI22" s="11"/>
       <c r="AJ22" s="11"/>
       <c r="AK22" s="11"/>
@@ -2289,24 +2235,24 @@
       <c r="N23" s="11"/>
       <c r="O23" s="11"/>
       <c r="P23" s="11"/>
-      <c r="Q23" s="21"/>
-      <c r="R23" s="21"/>
-      <c r="S23" s="21"/>
-      <c r="T23" s="21"/>
-      <c r="U23" s="21"/>
-      <c r="V23" s="21"/>
-      <c r="W23" s="21"/>
-      <c r="X23" s="21"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="23"/>
+      <c r="W23" s="23"/>
+      <c r="X23" s="23"/>
       <c r="Y23" s="11"/>
       <c r="Z23" s="11"/>
-      <c r="AA23" s="21"/>
-      <c r="AB23" s="21"/>
-      <c r="AC23" s="21"/>
-      <c r="AD23" s="21"/>
-      <c r="AE23" s="21"/>
-      <c r="AF23" s="21"/>
-      <c r="AG23" s="21"/>
-      <c r="AH23" s="21"/>
+      <c r="AA23" s="23"/>
+      <c r="AB23" s="23"/>
+      <c r="AC23" s="23"/>
+      <c r="AD23" s="23"/>
+      <c r="AE23" s="23"/>
+      <c r="AF23" s="23"/>
+      <c r="AG23" s="23"/>
+      <c r="AH23" s="23"/>
       <c r="AI23" s="11"/>
       <c r="AJ23" s="11"/>
       <c r="AK23" s="11"/>
@@ -2339,24 +2285,24 @@
       <c r="N24" s="11"/>
       <c r="O24" s="11"/>
       <c r="P24" s="11"/>
-      <c r="Q24" s="21"/>
-      <c r="R24" s="21"/>
-      <c r="S24" s="21"/>
-      <c r="T24" s="21"/>
-      <c r="U24" s="21"/>
-      <c r="V24" s="21"/>
-      <c r="W24" s="21"/>
-      <c r="X24" s="21"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
+      <c r="V24" s="23"/>
+      <c r="W24" s="23"/>
+      <c r="X24" s="23"/>
       <c r="Y24" s="11"/>
       <c r="Z24" s="11"/>
-      <c r="AA24" s="21"/>
-      <c r="AB24" s="21"/>
-      <c r="AC24" s="21"/>
-      <c r="AD24" s="21"/>
-      <c r="AE24" s="21"/>
-      <c r="AF24" s="21"/>
-      <c r="AG24" s="21"/>
-      <c r="AH24" s="21"/>
+      <c r="AA24" s="23"/>
+      <c r="AB24" s="23"/>
+      <c r="AC24" s="23"/>
+      <c r="AD24" s="23"/>
+      <c r="AE24" s="23"/>
+      <c r="AF24" s="23"/>
+      <c r="AG24" s="23"/>
+      <c r="AH24" s="23"/>
       <c r="AI24" s="11"/>
       <c r="AJ24" s="11"/>
       <c r="AK24" s="11"/>
@@ -2594,7 +2540,7 @@
   <dimension ref="B1:AW28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21:X24"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2722,17 +2668,17 @@
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
-      <c r="S4" s="23" t="s">
+      <c r="S4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="23"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="23"/>
-      <c r="AA4" s="23"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
       <c r="AB4" s="16"/>
       <c r="AC4" s="16"/>
       <c r="AD4" s="16"/>
@@ -2774,15 +2720,15 @@
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="23"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
       <c r="AB5" s="16"/>
       <c r="AC5" s="16"/>
       <c r="AD5" s="16"/>
@@ -2824,21 +2770,21 @@
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="23"/>
-      <c r="AB6" s="22" t="s">
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="19"/>
+      <c r="AB6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="AC6" s="22"/>
-      <c r="AD6" s="22"/>
-      <c r="AE6" s="22"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="18"/>
+      <c r="AE6" s="18"/>
       <c r="AF6" s="11"/>
       <c r="AG6" s="11"/>
       <c r="AH6" s="11"/>
@@ -2876,19 +2822,19 @@
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="23"/>
-      <c r="X7" s="23"/>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="23"/>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="22"/>
-      <c r="AC7" s="22"/>
-      <c r="AD7" s="22"/>
-      <c r="AE7" s="22"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="18"/>
+      <c r="AC7" s="18"/>
+      <c r="AD7" s="18"/>
+      <c r="AE7" s="18"/>
       <c r="AF7" s="11"/>
       <c r="AG7" s="11"/>
       <c r="AH7" s="11"/>
@@ -2935,10 +2881,10 @@
       <c r="Y8" s="11"/>
       <c r="Z8" s="11"/>
       <c r="AA8" s="11"/>
-      <c r="AB8" s="22"/>
-      <c r="AC8" s="22"/>
-      <c r="AD8" s="22"/>
-      <c r="AE8" s="22"/>
+      <c r="AB8" s="18"/>
+      <c r="AC8" s="18"/>
+      <c r="AD8" s="18"/>
+      <c r="AE8" s="18"/>
       <c r="AF8" s="11"/>
       <c r="AG8" s="11"/>
       <c r="AH8" s="11"/>
@@ -3502,27 +3448,27 @@
       <c r="N21" s="11"/>
       <c r="O21" s="11"/>
       <c r="P21" s="11"/>
-      <c r="Q21" s="21" t="s">
+      <c r="Q21" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
+      <c r="X21" s="23"/>
       <c r="Z21" s="11"/>
-      <c r="AA21" s="21" t="s">
+      <c r="AA21" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AB21" s="21"/>
-      <c r="AC21" s="21"/>
-      <c r="AD21" s="21"/>
-      <c r="AE21" s="21"/>
-      <c r="AF21" s="21"/>
-      <c r="AG21" s="21"/>
-      <c r="AH21" s="21"/>
+      <c r="AB21" s="23"/>
+      <c r="AC21" s="23"/>
+      <c r="AD21" s="23"/>
+      <c r="AE21" s="23"/>
+      <c r="AF21" s="23"/>
+      <c r="AG21" s="23"/>
+      <c r="AH21" s="23"/>
       <c r="AI21" s="11"/>
       <c r="AJ21" s="11"/>
       <c r="AK21" s="11"/>
@@ -3555,23 +3501,23 @@
       <c r="N22" s="11"/>
       <c r="O22" s="11"/>
       <c r="P22" s="11"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="21"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="23"/>
+      <c r="W22" s="23"/>
+      <c r="X22" s="23"/>
       <c r="Z22" s="11"/>
-      <c r="AA22" s="21"/>
-      <c r="AB22" s="21"/>
-      <c r="AC22" s="21"/>
-      <c r="AD22" s="21"/>
-      <c r="AE22" s="21"/>
-      <c r="AF22" s="21"/>
-      <c r="AG22" s="21"/>
-      <c r="AH22" s="21"/>
+      <c r="AA22" s="23"/>
+      <c r="AB22" s="23"/>
+      <c r="AC22" s="23"/>
+      <c r="AD22" s="23"/>
+      <c r="AE22" s="23"/>
+      <c r="AF22" s="23"/>
+      <c r="AG22" s="23"/>
+      <c r="AH22" s="23"/>
       <c r="AI22" s="11"/>
       <c r="AJ22" s="11"/>
       <c r="AK22" s="11"/>
@@ -3604,24 +3550,24 @@
       <c r="N23" s="11"/>
       <c r="O23" s="11"/>
       <c r="P23" s="11"/>
-      <c r="Q23" s="21"/>
-      <c r="R23" s="21"/>
-      <c r="S23" s="21"/>
-      <c r="T23" s="21"/>
-      <c r="U23" s="21"/>
-      <c r="V23" s="21"/>
-      <c r="W23" s="21"/>
-      <c r="X23" s="21"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="23"/>
+      <c r="W23" s="23"/>
+      <c r="X23" s="23"/>
       <c r="Y23" s="11"/>
       <c r="Z23" s="11"/>
-      <c r="AA23" s="21"/>
-      <c r="AB23" s="21"/>
-      <c r="AC23" s="21"/>
-      <c r="AD23" s="21"/>
-      <c r="AE23" s="21"/>
-      <c r="AF23" s="21"/>
-      <c r="AG23" s="21"/>
-      <c r="AH23" s="21"/>
+      <c r="AA23" s="23"/>
+      <c r="AB23" s="23"/>
+      <c r="AC23" s="23"/>
+      <c r="AD23" s="23"/>
+      <c r="AE23" s="23"/>
+      <c r="AF23" s="23"/>
+      <c r="AG23" s="23"/>
+      <c r="AH23" s="23"/>
       <c r="AI23" s="11"/>
       <c r="AJ23" s="11"/>
       <c r="AK23" s="11"/>
@@ -3654,24 +3600,24 @@
       <c r="N24" s="11"/>
       <c r="O24" s="11"/>
       <c r="P24" s="11"/>
-      <c r="Q24" s="21"/>
-      <c r="R24" s="21"/>
-      <c r="S24" s="21"/>
-      <c r="T24" s="21"/>
-      <c r="U24" s="21"/>
-      <c r="V24" s="21"/>
-      <c r="W24" s="21"/>
-      <c r="X24" s="21"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
+      <c r="V24" s="23"/>
+      <c r="W24" s="23"/>
+      <c r="X24" s="23"/>
       <c r="Y24" s="11"/>
       <c r="Z24" s="11"/>
-      <c r="AA24" s="21"/>
-      <c r="AB24" s="21"/>
-      <c r="AC24" s="21"/>
-      <c r="AD24" s="21"/>
-      <c r="AE24" s="21"/>
-      <c r="AF24" s="21"/>
-      <c r="AG24" s="21"/>
-      <c r="AH24" s="21"/>
+      <c r="AA24" s="23"/>
+      <c r="AB24" s="23"/>
+      <c r="AC24" s="23"/>
+      <c r="AD24" s="23"/>
+      <c r="AE24" s="23"/>
+      <c r="AF24" s="23"/>
+      <c r="AG24" s="23"/>
+      <c r="AH24" s="23"/>
       <c r="AI24" s="11"/>
       <c r="AJ24" s="11"/>
       <c r="AK24" s="11"/>
@@ -3896,7 +3842,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF34" sqref="AF34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3905,22 +3853,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-    </row>
-    <row r="2" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+    </row>
+    <row r="2" spans="1:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -3962,15 +3910,15 @@
     <row r="3" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
       <c r="M3" s="16"/>
       <c r="N3" s="16"/>
       <c r="O3" s="16"/>
@@ -3979,16 +3927,16 @@
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="11"/>
-      <c r="AC3" s="11"/>
-      <c r="AD3" s="11"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="9"/>
       <c r="AE3" s="11"/>
       <c r="AF3" s="11"/>
       <c r="AG3" s="11"/>
@@ -3997,42 +3945,55 @@
       <c r="AJ3" s="11"/>
       <c r="AK3" s="11"/>
       <c r="AL3" s="11"/>
-      <c r="AM3" s="11"/>
-      <c r="AN3" s="11"/>
-      <c r="AO3" s="11" t="s">
+      <c r="AM3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AP3" s="11"/>
-      <c r="AQ3" s="11"/>
+      <c r="AN3" s="11"/>
+      <c r="AO3" s="11"/>
+      <c r="AP3" s="3"/>
+      <c r="AQ3" s="3"/>
       <c r="AR3" s="11"/>
       <c r="AS3" s="11"/>
-      <c r="AT3" s="11"/>
-      <c r="AU3" s="21" t="s">
+      <c r="AT3" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="AV3" s="21"/>
+      <c r="AU3" s="44"/>
+      <c r="AV3" s="44"/>
       <c r="AW3" s="12"/>
     </row>
-    <row r="4" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
       <c r="C4" s="11"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="22" t="s">
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="43"/>
+      <c r="X4" s="43"/>
+      <c r="Y4" s="43"/>
+      <c r="Z4" s="43"/>
+      <c r="AA4" s="43"/>
+      <c r="AB4" s="43"/>
+      <c r="AC4" s="43"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="3"/>
       <c r="AF4" s="11"/>
       <c r="AG4" s="11"/>
       <c r="AH4" s="11"/>
@@ -4040,38 +4001,51 @@
       <c r="AJ4" s="11"/>
       <c r="AK4" s="11"/>
       <c r="AL4" s="11"/>
-      <c r="AM4" s="11"/>
-      <c r="AN4" s="11"/>
-      <c r="AO4" s="11" t="s">
+      <c r="AM4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="AP4" s="11"/>
-      <c r="AQ4" s="11"/>
+      <c r="AN4" s="11"/>
+      <c r="AO4" s="11"/>
+      <c r="AP4" s="3"/>
+      <c r="AQ4" s="3"/>
       <c r="AR4" s="11"/>
       <c r="AS4" s="11"/>
-      <c r="AT4" s="11"/>
-      <c r="AU4" s="21"/>
-      <c r="AV4" s="21"/>
+      <c r="AT4" s="44"/>
+      <c r="AU4" s="44"/>
+      <c r="AV4" s="44"/>
       <c r="AW4" s="12"/>
     </row>
     <row r="5" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
       <c r="AF5" s="11"/>
       <c r="AG5" s="11"/>
       <c r="AH5" s="11"/>
@@ -4086,9 +4060,9 @@
       <c r="AQ5" s="11"/>
       <c r="AR5" s="11"/>
       <c r="AS5" s="11"/>
-      <c r="AT5" s="11"/>
-      <c r="AU5" s="11"/>
-      <c r="AV5" s="11"/>
+      <c r="AT5" s="44"/>
+      <c r="AU5" s="44"/>
+      <c r="AV5" s="44"/>
       <c r="AW5" s="12"/>
     </row>
     <row r="6" spans="1:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4103,12 +4077,25 @@
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
       <c r="AF6" s="11"/>
       <c r="AG6" s="11"/>
       <c r="AH6" s="11"/>
@@ -4130,8 +4117,8 @@
     </row>
     <row r="7" spans="1:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -4143,9 +4130,9 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
+      <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
@@ -4158,180 +4145,188 @@
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
+      <c r="AE7" s="8"/>
       <c r="AF7" s="8"/>
       <c r="AG7" s="8"/>
       <c r="AH7" s="8"/>
       <c r="AI7" s="8"/>
-      <c r="AJ7" s="8"/>
-      <c r="AK7" s="9"/>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="11"/>
       <c r="AL7" s="11"/>
-      <c r="AM7" s="11"/>
-      <c r="AN7" s="11"/>
-      <c r="AO7" s="11"/>
-      <c r="AP7" s="18"/>
-      <c r="AQ7" s="19"/>
-      <c r="AR7" s="33" t="s">
+      <c r="AM7" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="AS7" s="33"/>
-      <c r="AT7" s="33"/>
-      <c r="AU7" s="33"/>
-      <c r="AV7" s="19"/>
-      <c r="AW7" s="20"/>
+      <c r="AN7" s="25"/>
+      <c r="AO7" s="25"/>
+      <c r="AP7" s="25"/>
+      <c r="AQ7" s="25"/>
+      <c r="AR7" s="25"/>
+      <c r="AS7" s="25"/>
+      <c r="AT7" s="25"/>
+      <c r="AU7" s="25"/>
+      <c r="AV7" s="46"/>
+      <c r="AW7" s="4"/>
     </row>
     <row r="8" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="27" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="27" t="s">
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="27"/>
-      <c r="V8" s="27"/>
-      <c r="W8" s="27"/>
-      <c r="X8" s="27"/>
-      <c r="Y8" s="27"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="27" t="s">
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="AB8" s="27"/>
-      <c r="AC8" s="27"/>
-      <c r="AD8" s="27"/>
-      <c r="AE8" s="27"/>
-      <c r="AF8" s="27"/>
-      <c r="AG8" s="27"/>
-      <c r="AH8" s="27"/>
-      <c r="AI8" s="27"/>
-      <c r="AJ8" s="27"/>
-      <c r="AK8" s="12"/>
+      <c r="AA8" s="24"/>
+      <c r="AB8" s="24"/>
+      <c r="AC8" s="24"/>
+      <c r="AD8" s="24"/>
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="24"/>
+      <c r="AG8" s="24"/>
+      <c r="AH8" s="24"/>
+      <c r="AI8" s="24"/>
+      <c r="AJ8" s="12"/>
+      <c r="AK8" s="11"/>
       <c r="AL8" s="11"/>
-      <c r="AM8" s="11"/>
-      <c r="AN8" s="11"/>
-      <c r="AO8" s="11"/>
-      <c r="AP8" s="10"/>
-      <c r="AQ8" s="11"/>
-      <c r="AR8" s="11"/>
-      <c r="AS8" s="11"/>
-      <c r="AT8" s="11"/>
-      <c r="AU8" s="11"/>
-      <c r="AV8" s="11"/>
-      <c r="AW8" s="12"/>
+      <c r="AM8" s="7"/>
+      <c r="AN8" s="8"/>
+      <c r="AO8" s="8"/>
+      <c r="AP8" s="8"/>
+      <c r="AQ8" s="8"/>
+      <c r="AR8" s="8"/>
+      <c r="AS8" s="8"/>
+      <c r="AT8" s="8"/>
+      <c r="AU8" s="8"/>
+      <c r="AV8" s="9"/>
+      <c r="AW8" s="4"/>
     </row>
     <row r="9" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="27"/>
-      <c r="V9" s="27"/>
-      <c r="W9" s="27"/>
-      <c r="X9" s="27"/>
-      <c r="Y9" s="27"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="27"/>
-      <c r="AB9" s="27"/>
-      <c r="AC9" s="27"/>
-      <c r="AD9" s="27"/>
-      <c r="AE9" s="27"/>
-      <c r="AF9" s="27"/>
-      <c r="AG9" s="27"/>
-      <c r="AH9" s="27"/>
-      <c r="AI9" s="27"/>
-      <c r="AJ9" s="27"/>
-      <c r="AK9" s="4"/>
-      <c r="AP9" s="10"/>
-      <c r="AQ9" s="3"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="24"/>
+      <c r="AA9" s="24"/>
+      <c r="AB9" s="24"/>
+      <c r="AC9" s="24"/>
+      <c r="AD9" s="24"/>
+      <c r="AE9" s="24"/>
+      <c r="AF9" s="24"/>
+      <c r="AG9" s="24"/>
+      <c r="AH9" s="24"/>
+      <c r="AI9" s="24"/>
+      <c r="AJ9" s="4"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="10"/>
+      <c r="AN9" s="11"/>
+      <c r="AO9" s="11"/>
+      <c r="AP9" s="11"/>
+      <c r="AQ9" s="11"/>
       <c r="AR9" s="11"/>
       <c r="AS9" s="11"/>
       <c r="AT9" s="11"/>
       <c r="AU9" s="11"/>
-      <c r="AV9" s="11"/>
-      <c r="AW9" s="12"/>
+      <c r="AV9" s="12"/>
+      <c r="AW9" s="4"/>
     </row>
     <row r="10" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
-      <c r="U10" s="27"/>
-      <c r="V10" s="27"/>
-      <c r="W10" s="27"/>
-      <c r="X10" s="27"/>
-      <c r="Y10" s="27"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="27"/>
-      <c r="AB10" s="27"/>
-      <c r="AC10" s="27"/>
-      <c r="AD10" s="27"/>
-      <c r="AE10" s="27"/>
-      <c r="AF10" s="27"/>
-      <c r="AG10" s="27"/>
-      <c r="AH10" s="27"/>
-      <c r="AI10" s="27"/>
-      <c r="AJ10" s="27"/>
-      <c r="AK10" s="4"/>
-      <c r="AP10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="24"/>
+      <c r="AA10" s="24"/>
+      <c r="AB10" s="24"/>
+      <c r="AC10" s="24"/>
+      <c r="AD10" s="24"/>
+      <c r="AE10" s="24"/>
+      <c r="AF10" s="24"/>
+      <c r="AG10" s="24"/>
+      <c r="AH10" s="24"/>
+      <c r="AI10" s="24"/>
+      <c r="AJ10" s="4"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="3"/>
+      <c r="AM10" s="10"/>
+      <c r="AN10" s="11"/>
+      <c r="AO10" s="11"/>
+      <c r="AP10" s="11"/>
       <c r="AQ10" s="11"/>
       <c r="AR10" s="11"/>
       <c r="AS10" s="11"/>
       <c r="AT10" s="11"/>
       <c r="AU10" s="11"/>
-      <c r="AV10" s="11"/>
-      <c r="AW10" s="12"/>
+      <c r="AV10" s="12"/>
+      <c r="AW10" s="4"/>
     </row>
     <row r="11" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -4352,8 +4347,8 @@
       <c r="V11" s="11"/>
       <c r="W11" s="11"/>
       <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="11"/>
       <c r="AA11" s="11"/>
       <c r="AB11" s="11"/>
       <c r="AC11" s="11"/>
@@ -4363,355 +4358,387 @@
       <c r="AG11" s="11"/>
       <c r="AH11" s="11"/>
       <c r="AI11" s="11"/>
-      <c r="AJ11" s="11"/>
-      <c r="AK11" s="4"/>
-      <c r="AP11" s="10"/>
+      <c r="AJ11" s="4"/>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="10"/>
+      <c r="AN11" s="11"/>
+      <c r="AO11" s="11"/>
+      <c r="AP11" s="11"/>
       <c r="AQ11" s="11"/>
       <c r="AR11" s="11"/>
       <c r="AS11" s="11"/>
       <c r="AT11" s="11"/>
       <c r="AU11" s="11"/>
-      <c r="AV11" s="11"/>
-      <c r="AW11" s="12"/>
+      <c r="AV11" s="12"/>
+      <c r="AW11" s="4"/>
     </row>
     <row r="12" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="27" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="27" t="s">
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="27"/>
-      <c r="T12" s="27"/>
-      <c r="U12" s="27"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="27"/>
-      <c r="X12" s="27"/>
-      <c r="Y12" s="27"/>
-      <c r="Z12" s="3"/>
-      <c r="AA12" s="27" t="s">
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="24"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="AB12" s="27"/>
-      <c r="AC12" s="27"/>
-      <c r="AD12" s="27"/>
-      <c r="AE12" s="27"/>
-      <c r="AF12" s="27"/>
-      <c r="AG12" s="27"/>
-      <c r="AH12" s="27"/>
-      <c r="AI12" s="27"/>
-      <c r="AJ12" s="27"/>
-      <c r="AK12" s="4"/>
-      <c r="AP12" s="10"/>
+      <c r="AA12" s="24"/>
+      <c r="AB12" s="24"/>
+      <c r="AC12" s="24"/>
+      <c r="AD12" s="24"/>
+      <c r="AE12" s="24"/>
+      <c r="AF12" s="24"/>
+      <c r="AG12" s="24"/>
+      <c r="AH12" s="24"/>
+      <c r="AI12" s="24"/>
+      <c r="AJ12" s="4"/>
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="10"/>
+      <c r="AN12" s="11"/>
+      <c r="AO12" s="11"/>
+      <c r="AP12" s="11"/>
       <c r="AQ12" s="11"/>
       <c r="AR12" s="11"/>
       <c r="AS12" s="11"/>
       <c r="AT12" s="11"/>
       <c r="AU12" s="11"/>
-      <c r="AV12" s="11"/>
-      <c r="AW12" s="12"/>
+      <c r="AV12" s="12"/>
+      <c r="AW12" s="4"/>
     </row>
     <row r="13" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="27"/>
-      <c r="U13" s="27"/>
-      <c r="V13" s="27"/>
-      <c r="W13" s="27"/>
-      <c r="X13" s="27"/>
-      <c r="Y13" s="27"/>
-      <c r="Z13" s="3"/>
-      <c r="AA13" s="27"/>
-      <c r="AB13" s="27"/>
-      <c r="AC13" s="27"/>
-      <c r="AD13" s="27"/>
-      <c r="AE13" s="27"/>
-      <c r="AF13" s="27"/>
-      <c r="AG13" s="27"/>
-      <c r="AH13" s="27"/>
-      <c r="AI13" s="27"/>
-      <c r="AJ13" s="27"/>
-      <c r="AK13" s="4"/>
-      <c r="AP13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="24"/>
+      <c r="T13" s="24"/>
+      <c r="U13" s="24"/>
+      <c r="V13" s="24"/>
+      <c r="W13" s="24"/>
+      <c r="X13" s="24"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="24"/>
+      <c r="AA13" s="24"/>
+      <c r="AB13" s="24"/>
+      <c r="AC13" s="24"/>
+      <c r="AD13" s="24"/>
+      <c r="AE13" s="24"/>
+      <c r="AF13" s="24"/>
+      <c r="AG13" s="24"/>
+      <c r="AH13" s="24"/>
+      <c r="AI13" s="24"/>
+      <c r="AJ13" s="4"/>
+      <c r="AK13" s="3"/>
+      <c r="AL13" s="3"/>
+      <c r="AM13" s="10"/>
+      <c r="AN13" s="11"/>
+      <c r="AO13" s="11"/>
+      <c r="AP13" s="11"/>
       <c r="AQ13" s="11"/>
       <c r="AR13" s="11"/>
       <c r="AS13" s="11"/>
       <c r="AT13" s="11"/>
       <c r="AU13" s="11"/>
-      <c r="AV13" s="11"/>
-      <c r="AW13" s="12"/>
+      <c r="AV13" s="12"/>
+      <c r="AW13" s="4"/>
     </row>
     <row r="14" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
-      <c r="R14" s="27"/>
-      <c r="S14" s="27"/>
-      <c r="T14" s="27"/>
-      <c r="U14" s="27"/>
-      <c r="V14" s="27"/>
-      <c r="W14" s="27"/>
-      <c r="X14" s="27"/>
-      <c r="Y14" s="27"/>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="27"/>
-      <c r="AB14" s="27"/>
-      <c r="AC14" s="27"/>
-      <c r="AD14" s="27"/>
-      <c r="AE14" s="27"/>
-      <c r="AF14" s="27"/>
-      <c r="AG14" s="27"/>
-      <c r="AH14" s="27"/>
-      <c r="AI14" s="27"/>
-      <c r="AJ14" s="27"/>
-      <c r="AK14" s="4"/>
-      <c r="AP14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="24"/>
+      <c r="AA14" s="24"/>
+      <c r="AB14" s="24"/>
+      <c r="AC14" s="24"/>
+      <c r="AD14" s="24"/>
+      <c r="AE14" s="24"/>
+      <c r="AF14" s="24"/>
+      <c r="AG14" s="24"/>
+      <c r="AH14" s="24"/>
+      <c r="AI14" s="24"/>
+      <c r="AJ14" s="4"/>
+      <c r="AK14" s="3"/>
+      <c r="AL14" s="3"/>
+      <c r="AM14" s="10"/>
+      <c r="AN14" s="11"/>
+      <c r="AO14" s="11"/>
+      <c r="AP14" s="11"/>
       <c r="AQ14" s="11"/>
       <c r="AR14" s="11"/>
       <c r="AS14" s="11"/>
       <c r="AT14" s="11"/>
       <c r="AU14" s="11"/>
-      <c r="AV14" s="11"/>
-      <c r="AW14" s="12"/>
+      <c r="AV14" s="12"/>
+      <c r="AW14" s="4"/>
     </row>
     <row r="15" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
+      <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
+      <c r="O15" s="11"/>
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
       <c r="R15" s="11"/>
       <c r="S15" s="11"/>
       <c r="T15" s="11"/>
       <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
+      <c r="V15" s="3"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
       <c r="Y15" s="3"/>
-      <c r="Z15" s="3"/>
+      <c r="Z15" s="11"/>
       <c r="AA15" s="11"/>
       <c r="AB15" s="11"/>
       <c r="AC15" s="11"/>
       <c r="AD15" s="11"/>
       <c r="AE15" s="11"/>
       <c r="AF15" s="11"/>
-      <c r="AG15" s="11"/>
+      <c r="AG15" s="3"/>
       <c r="AH15" s="3"/>
       <c r="AI15" s="3"/>
-      <c r="AJ15" s="3"/>
-      <c r="AK15" s="4"/>
-      <c r="AP15" s="10"/>
+      <c r="AJ15" s="4"/>
+      <c r="AK15" s="3"/>
+      <c r="AL15" s="3"/>
+      <c r="AM15" s="10"/>
+      <c r="AN15" s="11"/>
+      <c r="AO15" s="11"/>
+      <c r="AP15" s="11"/>
       <c r="AQ15" s="11"/>
       <c r="AR15" s="11"/>
       <c r="AS15" s="11"/>
       <c r="AT15" s="11"/>
       <c r="AU15" s="11"/>
-      <c r="AV15" s="11"/>
-      <c r="AW15" s="12"/>
+      <c r="AV15" s="12"/>
+      <c r="AW15" s="4"/>
     </row>
     <row r="16" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="27" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="27" t="s">
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="27"/>
-      <c r="T16" s="27"/>
-      <c r="U16" s="27"/>
-      <c r="V16" s="27"/>
-      <c r="W16" s="27"/>
-      <c r="X16" s="27"/>
-      <c r="Y16" s="27"/>
-      <c r="Z16" s="3"/>
-      <c r="AA16" s="27" t="s">
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="24"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="24"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="AB16" s="27"/>
-      <c r="AC16" s="27"/>
-      <c r="AD16" s="27"/>
-      <c r="AE16" s="27"/>
-      <c r="AF16" s="27"/>
-      <c r="AG16" s="27"/>
-      <c r="AH16" s="27"/>
-      <c r="AI16" s="27"/>
-      <c r="AJ16" s="27"/>
-      <c r="AK16" s="4"/>
-      <c r="AP16" s="10"/>
+      <c r="AA16" s="24"/>
+      <c r="AB16" s="24"/>
+      <c r="AC16" s="24"/>
+      <c r="AD16" s="24"/>
+      <c r="AE16" s="24"/>
+      <c r="AF16" s="24"/>
+      <c r="AG16" s="24"/>
+      <c r="AH16" s="24"/>
+      <c r="AI16" s="24"/>
+      <c r="AJ16" s="4"/>
+      <c r="AK16" s="3"/>
+      <c r="AL16" s="3"/>
+      <c r="AM16" s="10"/>
+      <c r="AN16" s="11"/>
+      <c r="AO16" s="11"/>
+      <c r="AP16" s="11"/>
       <c r="AQ16" s="11"/>
       <c r="AR16" s="11"/>
       <c r="AS16" s="11"/>
       <c r="AT16" s="11"/>
       <c r="AU16" s="11"/>
-      <c r="AV16" s="11"/>
-      <c r="AW16" s="12"/>
+      <c r="AV16" s="12"/>
+      <c r="AW16" s="4"/>
     </row>
     <row r="17" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
-      <c r="U17" s="27"/>
-      <c r="V17" s="27"/>
-      <c r="W17" s="27"/>
-      <c r="X17" s="27"/>
-      <c r="Y17" s="27"/>
-      <c r="Z17" s="3"/>
-      <c r="AA17" s="27"/>
-      <c r="AB17" s="27"/>
-      <c r="AC17" s="27"/>
-      <c r="AD17" s="27"/>
-      <c r="AE17" s="27"/>
-      <c r="AF17" s="27"/>
-      <c r="AG17" s="27"/>
-      <c r="AH17" s="27"/>
-      <c r="AI17" s="27"/>
-      <c r="AJ17" s="27"/>
-      <c r="AK17" s="4"/>
-      <c r="AP17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="24"/>
+      <c r="U17" s="24"/>
+      <c r="V17" s="24"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="24"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="24"/>
+      <c r="AA17" s="24"/>
+      <c r="AB17" s="24"/>
+      <c r="AC17" s="24"/>
+      <c r="AD17" s="24"/>
+      <c r="AE17" s="24"/>
+      <c r="AF17" s="24"/>
+      <c r="AG17" s="24"/>
+      <c r="AH17" s="24"/>
+      <c r="AI17" s="24"/>
+      <c r="AJ17" s="4"/>
+      <c r="AK17" s="3"/>
+      <c r="AL17" s="3"/>
+      <c r="AM17" s="10"/>
+      <c r="AN17" s="11"/>
+      <c r="AO17" s="11"/>
+      <c r="AP17" s="11"/>
       <c r="AQ17" s="11"/>
       <c r="AR17" s="11"/>
       <c r="AS17" s="11"/>
       <c r="AT17" s="11"/>
       <c r="AU17" s="11"/>
-      <c r="AV17" s="11"/>
-      <c r="AW17" s="12"/>
+      <c r="AV17" s="12"/>
+      <c r="AW17" s="4"/>
     </row>
     <row r="18" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="27"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="27"/>
-      <c r="T18" s="27"/>
-      <c r="U18" s="27"/>
-      <c r="V18" s="27"/>
-      <c r="W18" s="27"/>
-      <c r="X18" s="27"/>
-      <c r="Y18" s="27"/>
-      <c r="Z18" s="3"/>
-      <c r="AA18" s="27"/>
-      <c r="AB18" s="27"/>
-      <c r="AC18" s="27"/>
-      <c r="AD18" s="27"/>
-      <c r="AE18" s="27"/>
-      <c r="AF18" s="27"/>
-      <c r="AG18" s="27"/>
-      <c r="AH18" s="27"/>
-      <c r="AI18" s="27"/>
-      <c r="AJ18" s="27"/>
-      <c r="AK18" s="4"/>
-      <c r="AP18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24"/>
+      <c r="X18" s="24"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="24"/>
+      <c r="AA18" s="24"/>
+      <c r="AB18" s="24"/>
+      <c r="AC18" s="24"/>
+      <c r="AD18" s="24"/>
+      <c r="AE18" s="24"/>
+      <c r="AF18" s="24"/>
+      <c r="AG18" s="24"/>
+      <c r="AH18" s="24"/>
+      <c r="AI18" s="24"/>
+      <c r="AJ18" s="4"/>
+      <c r="AK18" s="3"/>
+      <c r="AL18" s="3"/>
+      <c r="AM18" s="10"/>
+      <c r="AN18" s="11"/>
+      <c r="AO18" s="11"/>
+      <c r="AP18" s="11"/>
       <c r="AQ18" s="11"/>
       <c r="AR18" s="11"/>
       <c r="AS18" s="11"/>
       <c r="AT18" s="11"/>
       <c r="AU18" s="11"/>
-      <c r="AV18" s="11"/>
-      <c r="AW18" s="12"/>
+      <c r="AV18" s="12"/>
+      <c r="AW18" s="4"/>
     </row>
     <row r="19" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
@@ -4732,8 +4759,8 @@
       <c r="V19" s="11"/>
       <c r="W19" s="11"/>
       <c r="X19" s="11"/>
-      <c r="Y19" s="11"/>
-      <c r="Z19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="11"/>
       <c r="AA19" s="11"/>
       <c r="AB19" s="11"/>
       <c r="AC19" s="11"/>
@@ -4743,165 +4770,181 @@
       <c r="AG19" s="11"/>
       <c r="AH19" s="11"/>
       <c r="AI19" s="11"/>
-      <c r="AJ19" s="11"/>
-      <c r="AK19" s="4"/>
-      <c r="AP19" s="10"/>
+      <c r="AJ19" s="4"/>
+      <c r="AK19" s="3"/>
+      <c r="AL19" s="3"/>
+      <c r="AM19" s="10"/>
+      <c r="AN19" s="11"/>
+      <c r="AO19" s="11"/>
+      <c r="AP19" s="11"/>
       <c r="AQ19" s="11"/>
       <c r="AR19" s="11"/>
       <c r="AS19" s="11"/>
       <c r="AT19" s="11"/>
       <c r="AU19" s="11"/>
-      <c r="AV19" s="11"/>
-      <c r="AW19" s="12"/>
+      <c r="AV19" s="12"/>
+      <c r="AW19" s="4"/>
     </row>
     <row r="20" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="27" t="s">
+      <c r="C20" s="10"/>
+      <c r="D20" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="27" t="s">
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="Q20" s="27"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="27"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="27"/>
-      <c r="V20" s="27"/>
-      <c r="W20" s="27"/>
-      <c r="X20" s="27"/>
-      <c r="Y20" s="27"/>
-      <c r="Z20" s="3"/>
-      <c r="AA20" s="27" t="s">
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
+      <c r="V20" s="24"/>
+      <c r="W20" s="24"/>
+      <c r="X20" s="24"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="AB20" s="27"/>
-      <c r="AC20" s="27"/>
-      <c r="AD20" s="27"/>
-      <c r="AE20" s="27"/>
-      <c r="AF20" s="27"/>
-      <c r="AG20" s="27"/>
-      <c r="AH20" s="27"/>
-      <c r="AI20" s="27"/>
-      <c r="AJ20" s="27"/>
-      <c r="AK20" s="4"/>
-      <c r="AP20" s="10"/>
+      <c r="AA20" s="24"/>
+      <c r="AB20" s="24"/>
+      <c r="AC20" s="24"/>
+      <c r="AD20" s="24"/>
+      <c r="AE20" s="24"/>
+      <c r="AF20" s="24"/>
+      <c r="AG20" s="24"/>
+      <c r="AH20" s="24"/>
+      <c r="AI20" s="24"/>
+      <c r="AJ20" s="4"/>
+      <c r="AK20" s="3"/>
+      <c r="AL20" s="3"/>
+      <c r="AM20" s="10"/>
+      <c r="AN20" s="11"/>
+      <c r="AO20" s="11"/>
+      <c r="AP20" s="11"/>
       <c r="AQ20" s="11"/>
       <c r="AR20" s="11"/>
       <c r="AS20" s="11"/>
       <c r="AT20" s="11"/>
       <c r="AU20" s="11"/>
-      <c r="AV20" s="11"/>
-      <c r="AW20" s="12"/>
+      <c r="AV20" s="12"/>
+      <c r="AW20" s="4"/>
     </row>
     <row r="21" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="U21" s="27"/>
-      <c r="V21" s="27"/>
-      <c r="W21" s="27"/>
-      <c r="X21" s="27"/>
-      <c r="Y21" s="27"/>
-      <c r="Z21" s="3"/>
-      <c r="AA21" s="27"/>
-      <c r="AB21" s="27"/>
-      <c r="AC21" s="27"/>
-      <c r="AD21" s="27"/>
-      <c r="AE21" s="27"/>
-      <c r="AF21" s="27"/>
-      <c r="AG21" s="27"/>
-      <c r="AH21" s="27"/>
-      <c r="AI21" s="27"/>
-      <c r="AJ21" s="27"/>
-      <c r="AK21" s="4"/>
-      <c r="AP21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
+      <c r="W21" s="24"/>
+      <c r="X21" s="24"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="24"/>
+      <c r="AA21" s="24"/>
+      <c r="AB21" s="24"/>
+      <c r="AC21" s="24"/>
+      <c r="AD21" s="24"/>
+      <c r="AE21" s="24"/>
+      <c r="AF21" s="24"/>
+      <c r="AG21" s="24"/>
+      <c r="AH21" s="24"/>
+      <c r="AI21" s="24"/>
+      <c r="AJ21" s="4"/>
+      <c r="AK21" s="3"/>
+      <c r="AL21" s="3"/>
+      <c r="AM21" s="10"/>
+      <c r="AN21" s="11"/>
+      <c r="AO21" s="11"/>
+      <c r="AP21" s="11"/>
       <c r="AQ21" s="11"/>
       <c r="AR21" s="11"/>
       <c r="AS21" s="11"/>
       <c r="AT21" s="11"/>
       <c r="AU21" s="11"/>
-      <c r="AV21" s="11"/>
-      <c r="AW21" s="12"/>
+      <c r="AV21" s="12"/>
+      <c r="AW21" s="4"/>
     </row>
     <row r="22" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
-      <c r="R22" s="27"/>
-      <c r="S22" s="27"/>
-      <c r="T22" s="27"/>
-      <c r="U22" s="27"/>
-      <c r="V22" s="27"/>
-      <c r="W22" s="27"/>
-      <c r="X22" s="27"/>
-      <c r="Y22" s="27"/>
-      <c r="Z22" s="3"/>
-      <c r="AA22" s="27"/>
-      <c r="AB22" s="27"/>
-      <c r="AC22" s="27"/>
-      <c r="AD22" s="27"/>
-      <c r="AE22" s="27"/>
-      <c r="AF22" s="27"/>
-      <c r="AG22" s="27"/>
-      <c r="AH22" s="27"/>
-      <c r="AI22" s="27"/>
-      <c r="AJ22" s="27"/>
-      <c r="AK22" s="4"/>
-      <c r="AP22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="24"/>
+      <c r="V22" s="24"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="24"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="24"/>
+      <c r="AA22" s="24"/>
+      <c r="AB22" s="24"/>
+      <c r="AC22" s="24"/>
+      <c r="AD22" s="24"/>
+      <c r="AE22" s="24"/>
+      <c r="AF22" s="24"/>
+      <c r="AG22" s="24"/>
+      <c r="AH22" s="24"/>
+      <c r="AI22" s="24"/>
+      <c r="AJ22" s="4"/>
+      <c r="AK22" s="3"/>
+      <c r="AL22" s="3"/>
+      <c r="AM22" s="10"/>
+      <c r="AN22" s="11"/>
+      <c r="AO22" s="11"/>
+      <c r="AP22" s="11"/>
       <c r="AQ22" s="11"/>
       <c r="AR22" s="11"/>
       <c r="AS22" s="11"/>
       <c r="AT22" s="11"/>
       <c r="AU22" s="11"/>
-      <c r="AV22" s="11"/>
-      <c r="AW22" s="12"/>
+      <c r="AV22" s="12"/>
+      <c r="AW22" s="4"/>
     </row>
     <row r="23" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="10"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
@@ -4933,20 +4976,20 @@
       <c r="AG23" s="14"/>
       <c r="AH23" s="14"/>
       <c r="AI23" s="14"/>
-      <c r="AJ23" s="14"/>
-      <c r="AK23" s="15"/>
+      <c r="AJ23" s="15"/>
+      <c r="AK23" s="11"/>
       <c r="AL23" s="11"/>
-      <c r="AM23" s="11"/>
-      <c r="AN23" s="11"/>
-      <c r="AO23" s="11"/>
-      <c r="AP23" s="10"/>
-      <c r="AQ23" s="11"/>
-      <c r="AR23" s="11"/>
-      <c r="AS23" s="11"/>
-      <c r="AT23" s="11"/>
-      <c r="AU23" s="11"/>
-      <c r="AV23" s="11"/>
-      <c r="AW23" s="12"/>
+      <c r="AM23" s="13"/>
+      <c r="AN23" s="14"/>
+      <c r="AO23" s="14"/>
+      <c r="AP23" s="14"/>
+      <c r="AQ23" s="14"/>
+      <c r="AR23" s="14"/>
+      <c r="AS23" s="14"/>
+      <c r="AT23" s="14"/>
+      <c r="AU23" s="14"/>
+      <c r="AV23" s="15"/>
+      <c r="AW23" s="4"/>
     </row>
     <row r="24" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
@@ -4989,41 +5032,46 @@
       <c r="AM24" s="11"/>
       <c r="AN24" s="11"/>
       <c r="AO24" s="11"/>
-      <c r="AP24" s="10"/>
-      <c r="AQ24" s="11"/>
-      <c r="AR24" s="11"/>
-      <c r="AS24" s="11"/>
-      <c r="AT24" s="11"/>
-      <c r="AU24" s="11"/>
-      <c r="AV24" s="11"/>
-      <c r="AW24" s="12"/>
+      <c r="AP24" s="3"/>
+      <c r="AQ24" s="3"/>
+      <c r="AR24" s="3"/>
+      <c r="AS24" s="3"/>
+      <c r="AT24" s="3"/>
+      <c r="AU24" s="3"/>
+      <c r="AV24" s="3"/>
+      <c r="AW24" s="4"/>
     </row>
     <row r="25" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="C25" s="11"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
       <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="21" t="s">
+      <c r="K25" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="O25" s="21"/>
-      <c r="P25" s="21"/>
-      <c r="Q25" s="21"/>
-      <c r="R25" s="21"/>
-      <c r="S25" s="21"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="21" t="s">
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="42"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="W25" s="21"/>
-      <c r="X25" s="21"/>
-      <c r="Y25" s="21"/>
-      <c r="Z25" s="21"/>
-      <c r="AA25" s="21"/>
-      <c r="AB25" s="11"/>
-      <c r="AC25" s="11"/>
+      <c r="V25" s="42"/>
+      <c r="W25" s="42"/>
+      <c r="X25" s="42"/>
+      <c r="Y25" s="42"/>
+      <c r="Z25" s="42"/>
+      <c r="AA25" s="42"/>
+      <c r="AB25" s="42"/>
       <c r="AD25" s="11"/>
       <c r="AE25" s="11"/>
       <c r="AF25" s="11"/>
@@ -5034,42 +5082,47 @@
       <c r="AK25" s="11"/>
       <c r="AL25" s="11"/>
       <c r="AM25" s="11"/>
-      <c r="AN25" s="11"/>
-      <c r="AO25" s="11"/>
-      <c r="AP25" s="10"/>
-      <c r="AQ25" s="11"/>
-      <c r="AR25" s="11"/>
-      <c r="AS25" s="11"/>
-      <c r="AT25" s="11"/>
-      <c r="AU25" s="11"/>
-      <c r="AV25" s="11"/>
-      <c r="AW25" s="12"/>
-    </row>
-    <row r="26" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AN25" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO25" s="42"/>
+      <c r="AP25" s="42"/>
+      <c r="AQ25" s="42"/>
+      <c r="AR25" s="42"/>
+      <c r="AS25" s="42"/>
+      <c r="AT25" s="42"/>
+      <c r="AU25" s="42"/>
+      <c r="AW25" s="4"/>
+    </row>
+    <row r="26" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
-      <c r="D26" t="s">
+      <c r="D26" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
       <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21"/>
-      <c r="P26" s="21"/>
-      <c r="Q26" s="21"/>
-      <c r="R26" s="21"/>
-      <c r="S26" s="21"/>
-      <c r="U26" s="11"/>
-      <c r="V26" s="21"/>
-      <c r="W26" s="21"/>
-      <c r="X26" s="21"/>
-      <c r="Y26" s="21"/>
-      <c r="Z26" s="21"/>
-      <c r="AA26" s="21"/>
-      <c r="AB26" s="11"/>
-      <c r="AC26" s="11"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="42"/>
+      <c r="Q26" s="42"/>
+      <c r="R26" s="42"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="42"/>
+      <c r="V26" s="42"/>
+      <c r="W26" s="42"/>
+      <c r="X26" s="42"/>
+      <c r="Y26" s="42"/>
+      <c r="Z26" s="42"/>
+      <c r="AA26" s="42"/>
+      <c r="AB26" s="42"/>
       <c r="AD26" s="11"/>
       <c r="AE26" s="11"/>
       <c r="AF26" s="11"/>
@@ -5080,16 +5133,15 @@
       <c r="AK26" s="11"/>
       <c r="AL26" s="11"/>
       <c r="AM26" s="11"/>
-      <c r="AN26" s="11"/>
-      <c r="AO26" s="11"/>
-      <c r="AP26" s="13"/>
-      <c r="AQ26" s="14"/>
-      <c r="AR26" s="14"/>
-      <c r="AS26" s="14"/>
-      <c r="AT26" s="14"/>
-      <c r="AU26" s="14"/>
-      <c r="AV26" s="14"/>
-      <c r="AW26" s="15"/>
+      <c r="AN26" s="42"/>
+      <c r="AO26" s="42"/>
+      <c r="AP26" s="42"/>
+      <c r="AQ26" s="42"/>
+      <c r="AR26" s="42"/>
+      <c r="AS26" s="42"/>
+      <c r="AT26" s="42"/>
+      <c r="AU26" s="42"/>
+      <c r="AW26" s="4"/>
     </row>
     <row r="27" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
@@ -5101,25 +5153,23 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="11"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="42"/>
+      <c r="Q27" s="42"/>
+      <c r="R27" s="42"/>
       <c r="T27" s="11"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
-      <c r="Z27" s="11"/>
-      <c r="AA27" s="11"/>
-      <c r="AB27" s="11"/>
-      <c r="AC27" s="11"/>
+      <c r="U27" s="42"/>
+      <c r="V27" s="42"/>
+      <c r="W27" s="42"/>
+      <c r="X27" s="42"/>
+      <c r="Y27" s="42"/>
+      <c r="Z27" s="42"/>
+      <c r="AA27" s="42"/>
+      <c r="AB27" s="42"/>
       <c r="AD27" s="11"/>
       <c r="AE27" s="11"/>
       <c r="AF27" s="11"/>
@@ -5130,18 +5180,15 @@
       <c r="AK27" s="11"/>
       <c r="AL27" s="11"/>
       <c r="AM27" s="11"/>
-      <c r="AN27" s="11"/>
-      <c r="AO27" s="11"/>
-      <c r="AP27" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AQ27" s="29"/>
-      <c r="AR27" s="29"/>
-      <c r="AS27" s="29"/>
-      <c r="AT27" s="29"/>
-      <c r="AU27" s="29"/>
-      <c r="AV27" s="29"/>
-      <c r="AW27" s="30"/>
+      <c r="AN27" s="42"/>
+      <c r="AO27" s="42"/>
+      <c r="AP27" s="42"/>
+      <c r="AQ27" s="42"/>
+      <c r="AR27" s="42"/>
+      <c r="AS27" s="42"/>
+      <c r="AT27" s="42"/>
+      <c r="AU27" s="42"/>
+      <c r="AW27" s="4"/>
     </row>
     <row r="28" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="13"/>
@@ -5184,54 +5231,53 @@
       <c r="AM28" s="14"/>
       <c r="AN28" s="14"/>
       <c r="AO28" s="14"/>
-      <c r="AP28" s="31"/>
-      <c r="AQ28" s="31"/>
-      <c r="AR28" s="31"/>
-      <c r="AS28" s="31"/>
-      <c r="AT28" s="31"/>
-      <c r="AU28" s="31"/>
-      <c r="AV28" s="31"/>
-      <c r="AW28" s="32"/>
+      <c r="AP28" s="43"/>
+      <c r="AQ28" s="43"/>
+      <c r="AR28" s="43"/>
+      <c r="AS28" s="43"/>
+      <c r="AT28" s="43"/>
+      <c r="AU28" s="43"/>
+      <c r="AV28" s="43"/>
+      <c r="AW28" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="AP27:AW28"/>
-    <mergeCell ref="AU3:AV4"/>
-    <mergeCell ref="E8:N10"/>
-    <mergeCell ref="E12:N14"/>
-    <mergeCell ref="E16:N18"/>
-    <mergeCell ref="N25:S26"/>
-    <mergeCell ref="V25:AA26"/>
-    <mergeCell ref="AR7:AU7"/>
-    <mergeCell ref="E20:N22"/>
-    <mergeCell ref="P8:Y10"/>
-    <mergeCell ref="P12:Y14"/>
-    <mergeCell ref="P16:Y18"/>
-    <mergeCell ref="P20:Y22"/>
-    <mergeCell ref="AA8:AJ10"/>
-    <mergeCell ref="AA12:AJ14"/>
-    <mergeCell ref="AA16:AJ18"/>
-    <mergeCell ref="AA20:AJ22"/>
+    <mergeCell ref="K25:R27"/>
+    <mergeCell ref="U25:AB27"/>
+    <mergeCell ref="AN25:AU27"/>
+    <mergeCell ref="Z20:AI22"/>
     <mergeCell ref="D2:L5"/>
     <mergeCell ref="M4:P6"/>
+    <mergeCell ref="AT3:AV5"/>
+    <mergeCell ref="AM7:AV7"/>
+    <mergeCell ref="D8:M10"/>
+    <mergeCell ref="D12:M14"/>
+    <mergeCell ref="D16:M18"/>
+    <mergeCell ref="D20:M22"/>
+    <mergeCell ref="O8:X10"/>
+    <mergeCell ref="O12:X14"/>
+    <mergeCell ref="O16:X18"/>
+    <mergeCell ref="O20:X22"/>
+    <mergeCell ref="Z8:AI10"/>
+    <mergeCell ref="Z12:AI14"/>
+    <mergeCell ref="Z16:AI18"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="V25:AA26" location="CreateRoom!A1" display="Create Room"/>
-    <hyperlink ref="N25:S26" location="Lobby!A1" display="Refresh Room"/>
-    <hyperlink ref="AU3:AV4" location="Login!A1" display="Logout"/>
-    <hyperlink ref="AP27:AW28" location="Lobby!A1" display="Refresh List"/>
-    <hyperlink ref="E8:N10" location="CreateRoom!A1" display="Room"/>
-    <hyperlink ref="P8:Y10" location="CreateRoom!A1" display="Room"/>
-    <hyperlink ref="E12:N14" location="CreateRoom!A1" display="Room"/>
-    <hyperlink ref="P12:Y14" location="CreateRoom!A1" display="Room"/>
-    <hyperlink ref="AA12:AJ14" location="CreateRoom!A1" display="Room"/>
-    <hyperlink ref="AA8:AJ10" location="CreateRoom!A1" display="Room"/>
-    <hyperlink ref="E16:N18" location="CreateRoom!A1" display="Room"/>
-    <hyperlink ref="P16:Y18" location="CreateRoom!A1" display="Room"/>
-    <hyperlink ref="E20:N22" location="CreateRoom!A1" display="Room"/>
-    <hyperlink ref="P20:Y22" location="CreateRoom!A1" display="Room"/>
-    <hyperlink ref="AA20:AJ22" location="CreateRoom!A1" display="Room"/>
-    <hyperlink ref="AA16:AJ18" location="CreateRoom!A1" display="Room"/>
+    <hyperlink ref="U25:Z26" location="CreateRoom!A1" display="Create Room"/>
+    <hyperlink ref="M25:R26" location="Lobby!A1" display="Refresh Room"/>
+    <hyperlink ref="D8:M10" location="CreateRoom!A1" display="Room"/>
+    <hyperlink ref="O8:X10" location="CreateRoom!A1" display="Room"/>
+    <hyperlink ref="D12:M14" location="CreateRoom!A1" display="Room"/>
+    <hyperlink ref="O12:X14" location="CreateRoom!A1" display="Room"/>
+    <hyperlink ref="Z12:AI14" location="CreateRoom!A1" display="Room"/>
+    <hyperlink ref="Z8:AI10" location="CreateRoom!A1" display="Room"/>
+    <hyperlink ref="D16:M18" location="CreateRoom!A1" display="Room"/>
+    <hyperlink ref="O16:X18" location="CreateRoom!A1" display="Room"/>
+    <hyperlink ref="D20:M22" location="CreateRoom!A1" display="Room"/>
+    <hyperlink ref="O20:X22" location="CreateRoom!A1" display="Room"/>
+    <hyperlink ref="Z20:AI22" location="CreateRoom!A1" display="Room"/>
+    <hyperlink ref="Z16:AI18" location="CreateRoom!A1" display="Room"/>
+    <hyperlink ref="AP25:AU26" location="Lobby!A1" display="Refresh List"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5242,8 +5288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AW28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BD24" sqref="BD24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5256,17 +5302,17 @@
     <row r="2" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -5308,15 +5354,15 @@
     <row r="3" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
       <c r="M3" s="16"/>
       <c r="N3" s="16"/>
       <c r="O3" s="16"/>
@@ -5343,40 +5389,40 @@
       <c r="AJ3" s="11"/>
       <c r="AK3" s="11"/>
       <c r="AL3" s="11"/>
-      <c r="AM3" s="11"/>
-      <c r="AN3" s="11"/>
-      <c r="AO3" s="11" t="s">
+      <c r="AM3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AP3" s="11"/>
-      <c r="AQ3" s="11"/>
+      <c r="AN3" s="11"/>
+      <c r="AO3" s="11"/>
+      <c r="AP3" s="3"/>
+      <c r="AQ3" s="3"/>
       <c r="AR3" s="11"/>
       <c r="AS3" s="11"/>
-      <c r="AT3" s="11"/>
-      <c r="AU3" s="21" t="s">
+      <c r="AT3" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="AV3" s="21"/>
+      <c r="AU3" s="44"/>
+      <c r="AV3" s="44"/>
       <c r="AW3" s="12"/>
     </row>
     <row r="4" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
       <c r="C4" s="11"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="22" t="s">
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
       <c r="AF4" s="11"/>
@@ -5386,36 +5432,36 @@
       <c r="AJ4" s="11"/>
       <c r="AK4" s="11"/>
       <c r="AL4" s="11"/>
-      <c r="AM4" s="11"/>
-      <c r="AN4" s="11"/>
-      <c r="AO4" s="11" t="s">
+      <c r="AM4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="AP4" s="11"/>
-      <c r="AQ4" s="11"/>
+      <c r="AN4" s="11"/>
+      <c r="AO4" s="11"/>
+      <c r="AP4" s="3"/>
+      <c r="AQ4" s="3"/>
       <c r="AR4" s="11"/>
       <c r="AS4" s="11"/>
-      <c r="AT4" s="11"/>
-      <c r="AU4" s="21"/>
-      <c r="AV4" s="21"/>
+      <c r="AT4" s="44"/>
+      <c r="AU4" s="44"/>
+      <c r="AV4" s="44"/>
       <c r="AW4" s="12"/>
     </row>
     <row r="5" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
       <c r="AF5" s="11"/>
@@ -5432,9 +5478,9 @@
       <c r="AQ5" s="11"/>
       <c r="AR5" s="11"/>
       <c r="AS5" s="11"/>
-      <c r="AT5" s="11"/>
-      <c r="AU5" s="11"/>
-      <c r="AV5" s="11"/>
+      <c r="AT5" s="44"/>
+      <c r="AU5" s="44"/>
+      <c r="AV5" s="44"/>
       <c r="AW5" s="12"/>
     </row>
     <row r="6" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5449,10 +5495,10 @@
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
       <c r="AF6" s="11"/>
@@ -5476,8 +5522,8 @@
     </row>
     <row r="7" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -5489,9 +5535,9 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
+      <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
@@ -5504,692 +5550,706 @@
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
+      <c r="AE7" s="8"/>
       <c r="AF7" s="8"/>
       <c r="AG7" s="8"/>
       <c r="AH7" s="8"/>
       <c r="AI7" s="8"/>
-      <c r="AJ7" s="8"/>
-      <c r="AK7" s="9"/>
+      <c r="AJ7" s="9"/>
       <c r="AL7" s="11"/>
-      <c r="AM7" s="11"/>
-      <c r="AN7" s="11"/>
-      <c r="AO7" s="11"/>
-      <c r="AP7" s="18"/>
-      <c r="AQ7" s="19"/>
-      <c r="AR7" s="33" t="s">
+      <c r="AM7" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="AS7" s="33"/>
-      <c r="AT7" s="33"/>
-      <c r="AU7" s="33"/>
-      <c r="AV7" s="19"/>
-      <c r="AW7" s="20"/>
-    </row>
-    <row r="8" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN7" s="25"/>
+      <c r="AO7" s="25"/>
+      <c r="AP7" s="25"/>
+      <c r="AQ7" s="25"/>
+      <c r="AR7" s="25"/>
+      <c r="AS7" s="25"/>
+      <c r="AT7" s="25"/>
+      <c r="AU7" s="25"/>
+      <c r="AV7" s="46"/>
+      <c r="AW7" s="4"/>
+    </row>
+    <row r="8" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="34" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="17"/>
+      <c r="AI8" s="17"/>
+      <c r="AJ8" s="12"/>
+      <c r="AL8" s="11"/>
+      <c r="AM8" s="7"/>
+      <c r="AN8" s="8"/>
+      <c r="AO8" s="8"/>
+      <c r="AP8" s="8"/>
+      <c r="AQ8" s="8"/>
+      <c r="AR8" s="8"/>
+      <c r="AS8" s="8"/>
+      <c r="AT8" s="8"/>
+      <c r="AU8" s="8"/>
+      <c r="AV8" s="9"/>
+      <c r="AW8" s="4"/>
+    </row>
+    <row r="9" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="35"/>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="36"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="34" t="s">
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="W8" s="35"/>
-      <c r="X8" s="35"/>
-      <c r="Y8" s="35"/>
-      <c r="Z8" s="35"/>
-      <c r="AA8" s="35"/>
-      <c r="AB8" s="35"/>
-      <c r="AC8" s="35"/>
-      <c r="AD8" s="35"/>
-      <c r="AE8" s="35"/>
-      <c r="AF8" s="35"/>
-      <c r="AG8" s="35"/>
-      <c r="AH8" s="35"/>
-      <c r="AI8" s="36"/>
-      <c r="AJ8" s="17"/>
-      <c r="AK8" s="12"/>
-      <c r="AL8" s="11"/>
-      <c r="AM8" s="11"/>
-      <c r="AN8" s="11"/>
-      <c r="AO8" s="11"/>
-      <c r="AP8" s="10"/>
-      <c r="AQ8" s="11"/>
-      <c r="AR8" s="11"/>
-      <c r="AS8" s="11"/>
-      <c r="AT8" s="11"/>
-      <c r="AU8" s="11"/>
-      <c r="AV8" s="11"/>
-      <c r="AW8" s="12"/>
-    </row>
-    <row r="9" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="38"/>
-      <c r="R9" s="38"/>
-      <c r="S9" s="39"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
-      <c r="V9" s="37"/>
-      <c r="W9" s="38"/>
-      <c r="X9" s="38"/>
-      <c r="Y9" s="38"/>
-      <c r="Z9" s="38"/>
-      <c r="AA9" s="38"/>
-      <c r="AB9" s="38"/>
-      <c r="AC9" s="38"/>
-      <c r="AD9" s="38"/>
-      <c r="AE9" s="38"/>
-      <c r="AF9" s="38"/>
-      <c r="AG9" s="38"/>
-      <c r="AH9" s="38"/>
-      <c r="AI9" s="39"/>
-      <c r="AJ9" s="17"/>
-      <c r="AK9" s="4"/>
-      <c r="AP9" s="10"/>
-      <c r="AQ9" s="3"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28"/>
+      <c r="X9" s="28"/>
+      <c r="Y9" s="28"/>
+      <c r="Z9" s="28"/>
+      <c r="AA9" s="28"/>
+      <c r="AB9" s="28"/>
+      <c r="AC9" s="28"/>
+      <c r="AD9" s="28"/>
+      <c r="AE9" s="28"/>
+      <c r="AF9" s="28"/>
+      <c r="AG9" s="28"/>
+      <c r="AH9" s="29"/>
+      <c r="AI9" s="17"/>
+      <c r="AJ9" s="4"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="10"/>
+      <c r="AN9" s="11"/>
+      <c r="AO9" s="11"/>
+      <c r="AP9" s="11"/>
+      <c r="AQ9" s="11"/>
       <c r="AR9" s="11"/>
       <c r="AS9" s="11"/>
       <c r="AT9" s="11"/>
       <c r="AU9" s="11"/>
-      <c r="AV9" s="11"/>
-      <c r="AW9" s="12"/>
+      <c r="AV9" s="12"/>
+      <c r="AW9" s="4"/>
     </row>
     <row r="10" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="38"/>
-      <c r="S10" s="39"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="17"/>
       <c r="T10" s="17"/>
-      <c r="U10" s="17"/>
-      <c r="V10" s="37"/>
-      <c r="W10" s="38"/>
-      <c r="X10" s="38"/>
-      <c r="Y10" s="38"/>
-      <c r="Z10" s="38"/>
-      <c r="AA10" s="38"/>
-      <c r="AB10" s="38"/>
-      <c r="AC10" s="38"/>
-      <c r="AD10" s="38"/>
-      <c r="AE10" s="38"/>
-      <c r="AF10" s="38"/>
-      <c r="AG10" s="38"/>
-      <c r="AH10" s="38"/>
-      <c r="AI10" s="39"/>
-      <c r="AJ10" s="17"/>
-      <c r="AK10" s="4"/>
-      <c r="AP10" s="10"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="31"/>
+      <c r="W10" s="31"/>
+      <c r="X10" s="31"/>
+      <c r="Y10" s="31"/>
+      <c r="Z10" s="31"/>
+      <c r="AA10" s="31"/>
+      <c r="AB10" s="31"/>
+      <c r="AC10" s="31"/>
+      <c r="AD10" s="31"/>
+      <c r="AE10" s="31"/>
+      <c r="AF10" s="31"/>
+      <c r="AG10" s="31"/>
+      <c r="AH10" s="32"/>
+      <c r="AI10" s="17"/>
+      <c r="AJ10" s="4"/>
+      <c r="AL10" s="3"/>
+      <c r="AM10" s="10"/>
+      <c r="AN10" s="11"/>
+      <c r="AO10" s="11"/>
+      <c r="AP10" s="11"/>
       <c r="AQ10" s="11"/>
       <c r="AR10" s="11"/>
       <c r="AS10" s="11"/>
       <c r="AT10" s="11"/>
       <c r="AU10" s="11"/>
-      <c r="AV10" s="11"/>
-      <c r="AW10" s="12"/>
+      <c r="AV10" s="12"/>
+      <c r="AW10" s="4"/>
     </row>
     <row r="11" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="10"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="39"/>
-      <c r="V11" s="37"/>
-      <c r="W11" s="38"/>
-      <c r="X11" s="38"/>
-      <c r="Y11" s="38"/>
-      <c r="Z11" s="38"/>
-      <c r="AA11" s="38"/>
-      <c r="AB11" s="38"/>
-      <c r="AC11" s="38"/>
-      <c r="AD11" s="38"/>
-      <c r="AE11" s="38"/>
-      <c r="AF11" s="38"/>
-      <c r="AG11" s="38"/>
-      <c r="AH11" s="38"/>
-      <c r="AI11" s="39"/>
-      <c r="AK11" s="4"/>
-      <c r="AP11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="30"/>
+      <c r="V11" s="31"/>
+      <c r="W11" s="31"/>
+      <c r="X11" s="31"/>
+      <c r="Y11" s="31"/>
+      <c r="Z11" s="31"/>
+      <c r="AA11" s="31"/>
+      <c r="AB11" s="31"/>
+      <c r="AC11" s="31"/>
+      <c r="AD11" s="31"/>
+      <c r="AE11" s="31"/>
+      <c r="AF11" s="31"/>
+      <c r="AG11" s="31"/>
+      <c r="AH11" s="32"/>
+      <c r="AJ11" s="4"/>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="10"/>
+      <c r="AN11" s="11"/>
+      <c r="AO11" s="11"/>
+      <c r="AP11" s="11"/>
       <c r="AQ11" s="11"/>
       <c r="AR11" s="11"/>
       <c r="AS11" s="11"/>
       <c r="AT11" s="11"/>
       <c r="AU11" s="11"/>
-      <c r="AV11" s="11"/>
-      <c r="AW11" s="12"/>
+      <c r="AV11" s="12"/>
+      <c r="AW11" s="4"/>
     </row>
     <row r="12" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="38"/>
-      <c r="S12" s="39"/>
-      <c r="T12" s="17"/>
-      <c r="U12" s="17"/>
-      <c r="V12" s="37"/>
-      <c r="W12" s="38"/>
-      <c r="X12" s="38"/>
-      <c r="Y12" s="38"/>
-      <c r="Z12" s="38"/>
-      <c r="AA12" s="38"/>
-      <c r="AB12" s="38"/>
-      <c r="AC12" s="38"/>
-      <c r="AD12" s="38"/>
-      <c r="AE12" s="38"/>
-      <c r="AF12" s="38"/>
-      <c r="AG12" s="38"/>
-      <c r="AH12" s="38"/>
-      <c r="AI12" s="39"/>
-      <c r="AJ12" s="17"/>
-      <c r="AK12" s="4"/>
-      <c r="AP12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="32"/>
+      <c r="U12" s="30"/>
+      <c r="V12" s="31"/>
+      <c r="W12" s="31"/>
+      <c r="X12" s="31"/>
+      <c r="Y12" s="31"/>
+      <c r="Z12" s="31"/>
+      <c r="AA12" s="31"/>
+      <c r="AB12" s="31"/>
+      <c r="AC12" s="31"/>
+      <c r="AD12" s="31"/>
+      <c r="AE12" s="31"/>
+      <c r="AF12" s="31"/>
+      <c r="AG12" s="31"/>
+      <c r="AH12" s="32"/>
+      <c r="AI12" s="17"/>
+      <c r="AJ12" s="4"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="10"/>
+      <c r="AN12" s="11"/>
+      <c r="AO12" s="11"/>
+      <c r="AP12" s="11"/>
       <c r="AQ12" s="11"/>
       <c r="AR12" s="11"/>
       <c r="AS12" s="11"/>
       <c r="AT12" s="11"/>
       <c r="AU12" s="11"/>
-      <c r="AV12" s="11"/>
-      <c r="AW12" s="12"/>
+      <c r="AV12" s="12"/>
+      <c r="AW12" s="4"/>
     </row>
     <row r="13" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="38"/>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="38"/>
-      <c r="S13" s="39"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="17"/>
       <c r="T13" s="17"/>
-      <c r="U13" s="17"/>
-      <c r="V13" s="37"/>
-      <c r="W13" s="38"/>
-      <c r="X13" s="38"/>
-      <c r="Y13" s="38"/>
-      <c r="Z13" s="38"/>
-      <c r="AA13" s="38"/>
-      <c r="AB13" s="38"/>
-      <c r="AC13" s="38"/>
-      <c r="AD13" s="38"/>
-      <c r="AE13" s="38"/>
-      <c r="AF13" s="38"/>
-      <c r="AG13" s="38"/>
-      <c r="AH13" s="38"/>
-      <c r="AI13" s="39"/>
-      <c r="AJ13" s="17"/>
-      <c r="AK13" s="4"/>
-      <c r="AP13" s="10"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="31"/>
+      <c r="W13" s="31"/>
+      <c r="X13" s="31"/>
+      <c r="Y13" s="31"/>
+      <c r="Z13" s="31"/>
+      <c r="AA13" s="31"/>
+      <c r="AB13" s="31"/>
+      <c r="AC13" s="31"/>
+      <c r="AD13" s="31"/>
+      <c r="AE13" s="31"/>
+      <c r="AF13" s="31"/>
+      <c r="AG13" s="31"/>
+      <c r="AH13" s="32"/>
+      <c r="AI13" s="17"/>
+      <c r="AJ13" s="4"/>
+      <c r="AL13" s="3"/>
+      <c r="AM13" s="10"/>
+      <c r="AN13" s="11"/>
+      <c r="AO13" s="11"/>
+      <c r="AP13" s="11"/>
       <c r="AQ13" s="11"/>
       <c r="AR13" s="11"/>
       <c r="AS13" s="11"/>
       <c r="AT13" s="11"/>
       <c r="AU13" s="11"/>
-      <c r="AV13" s="11"/>
-      <c r="AW13" s="12"/>
+      <c r="AV13" s="12"/>
+      <c r="AW13" s="4"/>
     </row>
     <row r="14" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="38"/>
-      <c r="Q14" s="38"/>
-      <c r="R14" s="38"/>
-      <c r="S14" s="39"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="17"/>
       <c r="T14" s="17"/>
-      <c r="U14" s="17"/>
-      <c r="V14" s="37"/>
-      <c r="W14" s="38"/>
-      <c r="X14" s="38"/>
-      <c r="Y14" s="38"/>
-      <c r="Z14" s="38"/>
-      <c r="AA14" s="38"/>
-      <c r="AB14" s="38"/>
-      <c r="AC14" s="38"/>
-      <c r="AD14" s="38"/>
-      <c r="AE14" s="38"/>
-      <c r="AF14" s="38"/>
-      <c r="AG14" s="38"/>
-      <c r="AH14" s="38"/>
-      <c r="AI14" s="39"/>
-      <c r="AJ14" s="17"/>
-      <c r="AK14" s="4"/>
-      <c r="AP14" s="10"/>
+      <c r="U14" s="30"/>
+      <c r="V14" s="31"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="31"/>
+      <c r="Y14" s="31"/>
+      <c r="Z14" s="31"/>
+      <c r="AA14" s="31"/>
+      <c r="AB14" s="31"/>
+      <c r="AC14" s="31"/>
+      <c r="AD14" s="31"/>
+      <c r="AE14" s="31"/>
+      <c r="AF14" s="31"/>
+      <c r="AG14" s="31"/>
+      <c r="AH14" s="32"/>
+      <c r="AI14" s="17"/>
+      <c r="AJ14" s="4"/>
+      <c r="AL14" s="3"/>
+      <c r="AM14" s="10"/>
+      <c r="AN14" s="11"/>
+      <c r="AO14" s="11"/>
+      <c r="AP14" s="11"/>
       <c r="AQ14" s="11"/>
       <c r="AR14" s="11"/>
       <c r="AS14" s="11"/>
       <c r="AT14" s="11"/>
       <c r="AU14" s="11"/>
-      <c r="AV14" s="11"/>
-      <c r="AW14" s="12"/>
+      <c r="AV14" s="12"/>
+      <c r="AW14" s="4"/>
     </row>
     <row r="15" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="10"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="38"/>
-      <c r="P15" s="38"/>
-      <c r="Q15" s="38"/>
-      <c r="R15" s="38"/>
-      <c r="S15" s="39"/>
-      <c r="V15" s="37"/>
-      <c r="W15" s="38"/>
-      <c r="X15" s="38"/>
-      <c r="Y15" s="38"/>
-      <c r="Z15" s="38"/>
-      <c r="AA15" s="38"/>
-      <c r="AB15" s="38"/>
-      <c r="AC15" s="38"/>
-      <c r="AD15" s="38"/>
-      <c r="AE15" s="38"/>
-      <c r="AF15" s="38"/>
-      <c r="AG15" s="38"/>
-      <c r="AH15" s="38"/>
-      <c r="AI15" s="39"/>
-      <c r="AK15" s="4"/>
-      <c r="AP15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="30"/>
+      <c r="V15" s="31"/>
+      <c r="W15" s="31"/>
+      <c r="X15" s="31"/>
+      <c r="Y15" s="31"/>
+      <c r="Z15" s="31"/>
+      <c r="AA15" s="31"/>
+      <c r="AB15" s="31"/>
+      <c r="AC15" s="31"/>
+      <c r="AD15" s="31"/>
+      <c r="AE15" s="31"/>
+      <c r="AF15" s="31"/>
+      <c r="AG15" s="31"/>
+      <c r="AH15" s="32"/>
+      <c r="AJ15" s="4"/>
+      <c r="AL15" s="3"/>
+      <c r="AM15" s="10"/>
+      <c r="AN15" s="11"/>
+      <c r="AO15" s="11"/>
+      <c r="AP15" s="11"/>
       <c r="AQ15" s="11"/>
       <c r="AR15" s="11"/>
       <c r="AS15" s="11"/>
       <c r="AT15" s="11"/>
       <c r="AU15" s="11"/>
-      <c r="AV15" s="11"/>
-      <c r="AW15" s="12"/>
+      <c r="AV15" s="12"/>
+      <c r="AW15" s="4"/>
     </row>
     <row r="16" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38"/>
-      <c r="Q16" s="38"/>
-      <c r="R16" s="38"/>
-      <c r="S16" s="39"/>
-      <c r="T16" s="17"/>
-      <c r="U16" s="17"/>
-      <c r="V16" s="37"/>
-      <c r="W16" s="38"/>
-      <c r="X16" s="38"/>
-      <c r="Y16" s="38"/>
-      <c r="Z16" s="38"/>
-      <c r="AA16" s="38"/>
-      <c r="AB16" s="38"/>
-      <c r="AC16" s="38"/>
-      <c r="AD16" s="38"/>
-      <c r="AE16" s="38"/>
-      <c r="AF16" s="38"/>
-      <c r="AG16" s="38"/>
-      <c r="AH16" s="38"/>
-      <c r="AI16" s="39"/>
-      <c r="AJ16" s="17"/>
-      <c r="AK16" s="4"/>
-      <c r="AP16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="32"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="31"/>
+      <c r="W16" s="31"/>
+      <c r="X16" s="31"/>
+      <c r="Y16" s="31"/>
+      <c r="Z16" s="31"/>
+      <c r="AA16" s="31"/>
+      <c r="AB16" s="31"/>
+      <c r="AC16" s="31"/>
+      <c r="AD16" s="31"/>
+      <c r="AE16" s="31"/>
+      <c r="AF16" s="31"/>
+      <c r="AG16" s="31"/>
+      <c r="AH16" s="32"/>
+      <c r="AI16" s="17"/>
+      <c r="AJ16" s="4"/>
+      <c r="AL16" s="3"/>
+      <c r="AM16" s="10"/>
+      <c r="AN16" s="11"/>
+      <c r="AO16" s="11"/>
+      <c r="AP16" s="11"/>
       <c r="AQ16" s="11"/>
       <c r="AR16" s="11"/>
       <c r="AS16" s="11"/>
       <c r="AT16" s="11"/>
       <c r="AU16" s="11"/>
-      <c r="AV16" s="11"/>
-      <c r="AW16" s="12"/>
+      <c r="AV16" s="12"/>
+      <c r="AW16" s="4"/>
     </row>
     <row r="17" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="38"/>
-      <c r="R17" s="38"/>
-      <c r="S17" s="39"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="17"/>
       <c r="T17" s="17"/>
-      <c r="U17" s="17"/>
-      <c r="V17" s="37"/>
-      <c r="W17" s="38"/>
-      <c r="X17" s="38"/>
-      <c r="Y17" s="38"/>
-      <c r="Z17" s="38"/>
-      <c r="AA17" s="38"/>
-      <c r="AB17" s="38"/>
-      <c r="AC17" s="38"/>
-      <c r="AD17" s="38"/>
-      <c r="AE17" s="38"/>
-      <c r="AF17" s="38"/>
-      <c r="AG17" s="38"/>
-      <c r="AH17" s="38"/>
-      <c r="AI17" s="39"/>
-      <c r="AJ17" s="17"/>
-      <c r="AK17" s="4"/>
-      <c r="AP17" s="10"/>
+      <c r="U17" s="30"/>
+      <c r="V17" s="31"/>
+      <c r="W17" s="31"/>
+      <c r="X17" s="31"/>
+      <c r="Y17" s="31"/>
+      <c r="Z17" s="31"/>
+      <c r="AA17" s="31"/>
+      <c r="AB17" s="31"/>
+      <c r="AC17" s="31"/>
+      <c r="AD17" s="31"/>
+      <c r="AE17" s="31"/>
+      <c r="AF17" s="31"/>
+      <c r="AG17" s="31"/>
+      <c r="AH17" s="32"/>
+      <c r="AI17" s="17"/>
+      <c r="AJ17" s="4"/>
+      <c r="AL17" s="3"/>
+      <c r="AM17" s="10"/>
+      <c r="AN17" s="11"/>
+      <c r="AO17" s="11"/>
+      <c r="AP17" s="11"/>
       <c r="AQ17" s="11"/>
       <c r="AR17" s="11"/>
       <c r="AS17" s="11"/>
       <c r="AT17" s="11"/>
       <c r="AU17" s="11"/>
-      <c r="AV17" s="11"/>
-      <c r="AW17" s="12"/>
-    </row>
-    <row r="18" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AV17" s="12"/>
+      <c r="AW17" s="4"/>
+    </row>
+    <row r="18" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="41"/>
-      <c r="Q18" s="41"/>
-      <c r="R18" s="41"/>
-      <c r="S18" s="42"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="17"/>
       <c r="T18" s="17"/>
-      <c r="U18" s="17"/>
-      <c r="V18" s="40"/>
-      <c r="W18" s="41"/>
-      <c r="X18" s="41"/>
-      <c r="Y18" s="41"/>
-      <c r="Z18" s="41"/>
-      <c r="AA18" s="41"/>
-      <c r="AB18" s="41"/>
-      <c r="AC18" s="41"/>
-      <c r="AD18" s="41"/>
-      <c r="AE18" s="41"/>
-      <c r="AF18" s="41"/>
-      <c r="AG18" s="41"/>
-      <c r="AH18" s="41"/>
-      <c r="AI18" s="42"/>
-      <c r="AJ18" s="17"/>
-      <c r="AK18" s="4"/>
-      <c r="AP18" s="10"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="31"/>
+      <c r="W18" s="31"/>
+      <c r="X18" s="31"/>
+      <c r="Y18" s="31"/>
+      <c r="Z18" s="31"/>
+      <c r="AA18" s="31"/>
+      <c r="AB18" s="31"/>
+      <c r="AC18" s="31"/>
+      <c r="AD18" s="31"/>
+      <c r="AE18" s="31"/>
+      <c r="AF18" s="31"/>
+      <c r="AG18" s="31"/>
+      <c r="AH18" s="32"/>
+      <c r="AI18" s="17"/>
+      <c r="AJ18" s="4"/>
+      <c r="AL18" s="3"/>
+      <c r="AM18" s="10"/>
+      <c r="AN18" s="11"/>
+      <c r="AO18" s="11"/>
+      <c r="AP18" s="11"/>
       <c r="AQ18" s="11"/>
       <c r="AR18" s="11"/>
       <c r="AS18" s="11"/>
       <c r="AT18" s="11"/>
       <c r="AU18" s="11"/>
-      <c r="AV18" s="11"/>
-      <c r="AW18" s="12"/>
+      <c r="AV18" s="12"/>
+      <c r="AW18" s="4"/>
     </row>
     <row r="19" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="10"/>
-      <c r="AK19" s="4"/>
-      <c r="AP19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="35"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="33"/>
+      <c r="V19" s="34"/>
+      <c r="W19" s="34"/>
+      <c r="X19" s="34"/>
+      <c r="Y19" s="34"/>
+      <c r="Z19" s="34"/>
+      <c r="AA19" s="34"/>
+      <c r="AB19" s="34"/>
+      <c r="AC19" s="34"/>
+      <c r="AD19" s="34"/>
+      <c r="AE19" s="34"/>
+      <c r="AF19" s="34"/>
+      <c r="AG19" s="34"/>
+      <c r="AH19" s="35"/>
+      <c r="AJ19" s="4"/>
+      <c r="AL19" s="3"/>
+      <c r="AM19" s="10"/>
+      <c r="AN19" s="11"/>
+      <c r="AO19" s="11"/>
+      <c r="AP19" s="11"/>
       <c r="AQ19" s="11"/>
       <c r="AR19" s="11"/>
       <c r="AS19" s="11"/>
       <c r="AT19" s="11"/>
       <c r="AU19" s="11"/>
-      <c r="AV19" s="11"/>
-      <c r="AW19" s="12"/>
-    </row>
-    <row r="20" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AV19" s="12"/>
+      <c r="AW19" s="4"/>
+    </row>
+    <row r="20" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="44"/>
-      <c r="N20" s="44"/>
-      <c r="O20" s="44"/>
-      <c r="P20" s="44"/>
-      <c r="Q20" s="44"/>
-      <c r="R20" s="45"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="17"/>
-      <c r="U20" s="17"/>
-      <c r="V20" s="17"/>
-      <c r="W20" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="X20" s="44"/>
-      <c r="Y20" s="44"/>
-      <c r="Z20" s="44"/>
-      <c r="AA20" s="44"/>
-      <c r="AB20" s="44"/>
-      <c r="AC20" s="44"/>
-      <c r="AD20" s="44"/>
-      <c r="AE20" s="44"/>
-      <c r="AF20" s="44"/>
-      <c r="AG20" s="44"/>
-      <c r="AH20" s="45"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="17"/>
       <c r="AI20" s="17"/>
-      <c r="AJ20" s="17"/>
-      <c r="AK20" s="4"/>
-      <c r="AP20" s="10"/>
+      <c r="AJ20" s="4"/>
+      <c r="AL20" s="3"/>
+      <c r="AM20" s="10"/>
+      <c r="AN20" s="11"/>
+      <c r="AO20" s="11"/>
+      <c r="AP20" s="11"/>
       <c r="AQ20" s="11"/>
       <c r="AR20" s="11"/>
       <c r="AS20" s="11"/>
       <c r="AT20" s="11"/>
       <c r="AU20" s="11"/>
-      <c r="AV20" s="11"/>
-      <c r="AW20" s="12"/>
-    </row>
-    <row r="21" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AV20" s="12"/>
+      <c r="AW20" s="4"/>
+    </row>
+    <row r="21" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="17"/>
       <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="47"/>
-      <c r="P21" s="47"/>
-      <c r="Q21" s="47"/>
-      <c r="R21" s="48"/>
-      <c r="S21" s="17"/>
-      <c r="T21" s="17"/>
+      <c r="F21" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="T21" s="47"/>
       <c r="U21" s="17"/>
-      <c r="V21" s="17"/>
-      <c r="W21" s="46"/>
-      <c r="X21" s="47"/>
-      <c r="Y21" s="47"/>
-      <c r="Z21" s="47"/>
-      <c r="AA21" s="47"/>
-      <c r="AB21" s="47"/>
-      <c r="AC21" s="47"/>
-      <c r="AD21" s="47"/>
-      <c r="AE21" s="47"/>
-      <c r="AF21" s="47"/>
-      <c r="AG21" s="47"/>
-      <c r="AH21" s="48"/>
+      <c r="V21" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="W21" s="37"/>
+      <c r="X21" s="37"/>
+      <c r="Y21" s="37"/>
+      <c r="Z21" s="37"/>
+      <c r="AA21" s="37"/>
+      <c r="AB21" s="37"/>
+      <c r="AC21" s="37"/>
+      <c r="AD21" s="37"/>
+      <c r="AE21" s="37"/>
+      <c r="AF21" s="37"/>
+      <c r="AG21" s="38"/>
+      <c r="AH21" s="17"/>
       <c r="AI21" s="17"/>
-      <c r="AJ21" s="17"/>
-      <c r="AK21" s="4"/>
-      <c r="AP21" s="10"/>
+      <c r="AJ21" s="4"/>
+      <c r="AL21" s="3"/>
+      <c r="AM21" s="10"/>
+      <c r="AN21" s="11"/>
+      <c r="AO21" s="11"/>
+      <c r="AP21" s="11"/>
       <c r="AQ21" s="11"/>
       <c r="AR21" s="11"/>
       <c r="AS21" s="11"/>
       <c r="AT21" s="11"/>
       <c r="AU21" s="11"/>
-      <c r="AV21" s="11"/>
-      <c r="AW21" s="12"/>
-    </row>
-    <row r="22" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AV21" s="12"/>
+      <c r="AW21" s="4"/>
+    </row>
+    <row r="22" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="17"/>
       <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="40"/>
+      <c r="Q22" s="41"/>
       <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
+      <c r="S22" s="47"/>
+      <c r="T22" s="47"/>
       <c r="U22" s="17"/>
-      <c r="V22" s="17"/>
-      <c r="W22" s="17"/>
-      <c r="X22" s="17"/>
-      <c r="Y22" s="17"/>
-      <c r="AA22" s="17"/>
-      <c r="AB22" s="17"/>
-      <c r="AC22" s="17"/>
-      <c r="AD22" s="17"/>
-      <c r="AE22" s="17"/>
-      <c r="AF22" s="17"/>
-      <c r="AG22" s="17"/>
+      <c r="V22" s="39"/>
+      <c r="W22" s="40"/>
+      <c r="X22" s="40"/>
+      <c r="Y22" s="40"/>
+      <c r="Z22" s="40"/>
+      <c r="AA22" s="40"/>
+      <c r="AB22" s="40"/>
+      <c r="AC22" s="40"/>
+      <c r="AD22" s="40"/>
+      <c r="AE22" s="40"/>
+      <c r="AF22" s="40"/>
+      <c r="AG22" s="41"/>
       <c r="AH22" s="17"/>
       <c r="AI22" s="17"/>
-      <c r="AJ22" s="17"/>
-      <c r="AK22" s="4"/>
-      <c r="AP22" s="10"/>
+      <c r="AJ22" s="4"/>
+      <c r="AL22" s="3"/>
+      <c r="AM22" s="10"/>
+      <c r="AN22" s="11"/>
+      <c r="AO22" s="11"/>
+      <c r="AP22" s="11"/>
       <c r="AQ22" s="11"/>
       <c r="AR22" s="11"/>
       <c r="AS22" s="11"/>
       <c r="AT22" s="11"/>
       <c r="AU22" s="11"/>
-      <c r="AV22" s="11"/>
-      <c r="AW22" s="12"/>
+      <c r="AV22" s="12"/>
+      <c r="AW22" s="4"/>
     </row>
     <row r="23" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="10"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
@@ -6221,20 +6281,19 @@
       <c r="AG23" s="14"/>
       <c r="AH23" s="14"/>
       <c r="AI23" s="14"/>
-      <c r="AJ23" s="14"/>
-      <c r="AK23" s="15"/>
+      <c r="AJ23" s="15"/>
       <c r="AL23" s="11"/>
-      <c r="AM23" s="11"/>
-      <c r="AN23" s="11"/>
-      <c r="AO23" s="11"/>
-      <c r="AP23" s="10"/>
-      <c r="AQ23" s="11"/>
-      <c r="AR23" s="11"/>
-      <c r="AS23" s="11"/>
-      <c r="AT23" s="11"/>
-      <c r="AU23" s="11"/>
-      <c r="AV23" s="11"/>
-      <c r="AW23" s="12"/>
+      <c r="AM23" s="13"/>
+      <c r="AN23" s="14"/>
+      <c r="AO23" s="14"/>
+      <c r="AP23" s="14"/>
+      <c r="AQ23" s="14"/>
+      <c r="AR23" s="14"/>
+      <c r="AS23" s="14"/>
+      <c r="AT23" s="14"/>
+      <c r="AU23" s="14"/>
+      <c r="AV23" s="15"/>
+      <c r="AW23" s="4"/>
     </row>
     <row r="24" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
@@ -6277,41 +6336,39 @@
       <c r="AM24" s="11"/>
       <c r="AN24" s="11"/>
       <c r="AO24" s="11"/>
-      <c r="AP24" s="10"/>
-      <c r="AQ24" s="11"/>
-      <c r="AR24" s="11"/>
-      <c r="AS24" s="11"/>
-      <c r="AT24" s="11"/>
-      <c r="AU24" s="11"/>
-      <c r="AV24" s="11"/>
-      <c r="AW24" s="12"/>
+      <c r="AP24" s="3"/>
+      <c r="AQ24" s="3"/>
+      <c r="AR24" s="3"/>
+      <c r="AS24" s="3"/>
+      <c r="AT24" s="3"/>
+      <c r="AU24" s="3"/>
+      <c r="AV24" s="3"/>
+      <c r="AW24" s="4"/>
     </row>
     <row r="25" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="C25" s="11"/>
       <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="21" t="s">
+      <c r="K25" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="O25" s="21"/>
-      <c r="P25" s="21"/>
-      <c r="Q25" s="21"/>
-      <c r="R25" s="21"/>
-      <c r="S25" s="21"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="21" t="s">
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="U25" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="W25" s="21"/>
-      <c r="X25" s="21"/>
-      <c r="Y25" s="21"/>
-      <c r="Z25" s="21"/>
-      <c r="AA25" s="21"/>
-      <c r="AB25" s="11"/>
-      <c r="AC25" s="11"/>
+      <c r="V25" s="23"/>
+      <c r="W25" s="23"/>
+      <c r="X25" s="23"/>
+      <c r="Y25" s="23"/>
+      <c r="Z25" s="23"/>
+      <c r="AA25" s="23"/>
+      <c r="AB25" s="23"/>
       <c r="AD25" s="11"/>
       <c r="AE25" s="11"/>
       <c r="AF25" s="11"/>
@@ -6322,42 +6379,41 @@
       <c r="AK25" s="11"/>
       <c r="AL25" s="11"/>
       <c r="AM25" s="11"/>
-      <c r="AN25" s="11"/>
-      <c r="AO25" s="11"/>
-      <c r="AP25" s="10"/>
-      <c r="AQ25" s="11"/>
-      <c r="AR25" s="11"/>
-      <c r="AS25" s="11"/>
-      <c r="AT25" s="11"/>
-      <c r="AU25" s="11"/>
-      <c r="AV25" s="11"/>
-      <c r="AW25" s="12"/>
-    </row>
-    <row r="26" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AN25" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO25" s="42"/>
+      <c r="AP25" s="42"/>
+      <c r="AQ25" s="42"/>
+      <c r="AR25" s="42"/>
+      <c r="AS25" s="42"/>
+      <c r="AT25" s="42"/>
+      <c r="AU25" s="42"/>
+      <c r="AW25" s="4"/>
+    </row>
+    <row r="26" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
       <c r="D26" t="s">
         <v>4</v>
       </c>
       <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21"/>
-      <c r="P26" s="21"/>
-      <c r="Q26" s="21"/>
-      <c r="R26" s="21"/>
-      <c r="S26" s="21"/>
-      <c r="U26" s="11"/>
-      <c r="V26" s="21"/>
-      <c r="W26" s="21"/>
-      <c r="X26" s="21"/>
-      <c r="Y26" s="21"/>
-      <c r="Z26" s="21"/>
-      <c r="AA26" s="21"/>
-      <c r="AB26" s="11"/>
-      <c r="AC26" s="11"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="23"/>
+      <c r="U26" s="23"/>
+      <c r="V26" s="23"/>
+      <c r="W26" s="23"/>
+      <c r="X26" s="23"/>
+      <c r="Y26" s="23"/>
+      <c r="Z26" s="23"/>
+      <c r="AA26" s="23"/>
+      <c r="AB26" s="23"/>
       <c r="AD26" s="11"/>
       <c r="AE26" s="11"/>
       <c r="AF26" s="11"/>
@@ -6368,16 +6424,15 @@
       <c r="AK26" s="11"/>
       <c r="AL26" s="11"/>
       <c r="AM26" s="11"/>
-      <c r="AN26" s="11"/>
-      <c r="AO26" s="11"/>
-      <c r="AP26" s="13"/>
-      <c r="AQ26" s="14"/>
-      <c r="AR26" s="14"/>
-      <c r="AS26" s="14"/>
-      <c r="AT26" s="14"/>
-      <c r="AU26" s="14"/>
-      <c r="AV26" s="14"/>
-      <c r="AW26" s="15"/>
+      <c r="AN26" s="42"/>
+      <c r="AO26" s="42"/>
+      <c r="AP26" s="42"/>
+      <c r="AQ26" s="42"/>
+      <c r="AR26" s="42"/>
+      <c r="AS26" s="42"/>
+      <c r="AT26" s="42"/>
+      <c r="AU26" s="42"/>
+      <c r="AW26" s="4"/>
     </row>
     <row r="27" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
@@ -6389,25 +6444,23 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="11"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
       <c r="T27" s="11"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
-      <c r="Z27" s="11"/>
-      <c r="AA27" s="11"/>
-      <c r="AB27" s="11"/>
-      <c r="AC27" s="11"/>
+      <c r="U27" s="23"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="23"/>
+      <c r="X27" s="23"/>
+      <c r="Y27" s="23"/>
+      <c r="Z27" s="23"/>
+      <c r="AA27" s="23"/>
+      <c r="AB27" s="23"/>
       <c r="AD27" s="11"/>
       <c r="AE27" s="11"/>
       <c r="AF27" s="11"/>
@@ -6418,18 +6471,15 @@
       <c r="AK27" s="11"/>
       <c r="AL27" s="11"/>
       <c r="AM27" s="11"/>
-      <c r="AN27" s="11"/>
-      <c r="AO27" s="11"/>
-      <c r="AP27" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AQ27" s="29"/>
-      <c r="AR27" s="29"/>
-      <c r="AS27" s="29"/>
-      <c r="AT27" s="29"/>
-      <c r="AU27" s="29"/>
-      <c r="AV27" s="29"/>
-      <c r="AW27" s="30"/>
+      <c r="AN27" s="42"/>
+      <c r="AO27" s="42"/>
+      <c r="AP27" s="42"/>
+      <c r="AQ27" s="42"/>
+      <c r="AR27" s="42"/>
+      <c r="AS27" s="42"/>
+      <c r="AT27" s="42"/>
+      <c r="AU27" s="42"/>
+      <c r="AW27" s="4"/>
     </row>
     <row r="28" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="13"/>
@@ -6472,35 +6522,36 @@
       <c r="AM28" s="14"/>
       <c r="AN28" s="14"/>
       <c r="AO28" s="14"/>
-      <c r="AP28" s="31"/>
-      <c r="AQ28" s="31"/>
-      <c r="AR28" s="31"/>
-      <c r="AS28" s="31"/>
-      <c r="AT28" s="31"/>
-      <c r="AU28" s="31"/>
-      <c r="AV28" s="31"/>
-      <c r="AW28" s="32"/>
+      <c r="AP28" s="43"/>
+      <c r="AQ28" s="43"/>
+      <c r="AR28" s="43"/>
+      <c r="AS28" s="43"/>
+      <c r="AT28" s="43"/>
+      <c r="AU28" s="43"/>
+      <c r="AV28" s="43"/>
+      <c r="AW28" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="E9:R19"/>
+    <mergeCell ref="U9:AH19"/>
+    <mergeCell ref="F21:Q22"/>
+    <mergeCell ref="V21:AG22"/>
+    <mergeCell ref="AM7:AV7"/>
+    <mergeCell ref="AN25:AU27"/>
+    <mergeCell ref="K25:R27"/>
+    <mergeCell ref="U25:AB27"/>
+    <mergeCell ref="S21:T22"/>
     <mergeCell ref="D2:L5"/>
-    <mergeCell ref="AU3:AV4"/>
     <mergeCell ref="M4:P6"/>
-    <mergeCell ref="N25:S26"/>
-    <mergeCell ref="V25:AA26"/>
-    <mergeCell ref="AP27:AW28"/>
-    <mergeCell ref="AR7:AU7"/>
-    <mergeCell ref="F8:S18"/>
-    <mergeCell ref="V8:AI18"/>
-    <mergeCell ref="G20:R21"/>
-    <mergeCell ref="W20:AH21"/>
+    <mergeCell ref="AT3:AV5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="N25:S26" location="Lobby!A1" display="Cancel"/>
-    <hyperlink ref="AU3:AV4" location="Login!A1" display="Logout"/>
-    <hyperlink ref="AP27:AW28" location="Lobby!A1" display="Refresh List"/>
+    <hyperlink ref="M25:R26" location="Lobby!A1" display="Cancel"/>
+    <hyperlink ref="AP25:AU26" location="Lobby!A1" display="Refresh List"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix layout single room, link login to Hieu's server
</commit_message>
<xml_diff>
--- a/References/Layout.xlsx
+++ b/References/Layout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="420" windowWidth="21795" windowHeight="6180" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="420" windowWidth="21795" windowHeight="6180" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -887,6 +887,33 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -971,138 +998,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1184,6 +1079,138 @@
     <xf numFmtId="20" fontId="16" fillId="7" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1245,33 +1272,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4281,7 +4281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V16" sqref="V16:AG20"/>
     </sheetView>
   </sheetViews>
@@ -4297,17 +4297,17 @@
     <row r="2" spans="1:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -4366,18 +4366,18 @@
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
-      <c r="U3" s="57" t="s">
+      <c r="U3" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="V3" s="58"/>
-      <c r="W3" s="58"/>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="58"/>
-      <c r="Z3" s="58"/>
-      <c r="AA3" s="58"/>
-      <c r="AB3" s="58"/>
-      <c r="AC3" s="58"/>
-      <c r="AD3" s="59"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
+      <c r="X3" s="67"/>
+      <c r="Y3" s="67"/>
+      <c r="Z3" s="67"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="68"/>
       <c r="AE3" s="11"/>
       <c r="AF3" s="11"/>
       <c r="AG3" s="11"/>
@@ -4395,11 +4395,11 @@
       <c r="AQ3" s="3"/>
       <c r="AR3" s="11"/>
       <c r="AS3" s="11"/>
-      <c r="AT3" s="64" t="s">
+      <c r="AT3" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="AU3" s="64"/>
-      <c r="AV3" s="64"/>
+      <c r="AU3" s="73"/>
+      <c r="AV3" s="73"/>
       <c r="AW3" s="12"/>
     </row>
     <row r="4" spans="1:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4424,16 +4424,16 @@
       <c r="R4" s="11"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
-      <c r="U4" s="60"/>
-      <c r="V4" s="61"/>
-      <c r="W4" s="61"/>
-      <c r="X4" s="61"/>
-      <c r="Y4" s="61"/>
-      <c r="Z4" s="61"/>
-      <c r="AA4" s="61"/>
-      <c r="AB4" s="61"/>
-      <c r="AC4" s="61"/>
-      <c r="AD4" s="62"/>
+      <c r="U4" s="69"/>
+      <c r="V4" s="70"/>
+      <c r="W4" s="70"/>
+      <c r="X4" s="70"/>
+      <c r="Y4" s="70"/>
+      <c r="Z4" s="70"/>
+      <c r="AA4" s="70"/>
+      <c r="AB4" s="70"/>
+      <c r="AC4" s="70"/>
+      <c r="AD4" s="71"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="11"/>
       <c r="AG4" s="11"/>
@@ -4451,9 +4451,9 @@
       <c r="AQ4" s="3"/>
       <c r="AR4" s="11"/>
       <c r="AS4" s="11"/>
-      <c r="AT4" s="64"/>
-      <c r="AU4" s="64"/>
-      <c r="AV4" s="64"/>
+      <c r="AT4" s="73"/>
+      <c r="AU4" s="73"/>
+      <c r="AV4" s="73"/>
       <c r="AW4" s="12"/>
     </row>
     <row r="5" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4501,9 +4501,9 @@
       <c r="AQ5" s="11"/>
       <c r="AR5" s="11"/>
       <c r="AS5" s="11"/>
-      <c r="AT5" s="64"/>
-      <c r="AU5" s="64"/>
-      <c r="AV5" s="64"/>
+      <c r="AT5" s="73"/>
+      <c r="AU5" s="73"/>
+      <c r="AV5" s="73"/>
       <c r="AW5" s="12"/>
     </row>
     <row r="6" spans="1:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4594,18 +4594,18 @@
       <c r="AJ7" s="9"/>
       <c r="AK7" s="11"/>
       <c r="AL7" s="11"/>
-      <c r="AM7" s="65" t="s">
+      <c r="AM7" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="AN7" s="66"/>
-      <c r="AO7" s="66"/>
-      <c r="AP7" s="66"/>
-      <c r="AQ7" s="66"/>
-      <c r="AR7" s="66"/>
-      <c r="AS7" s="66"/>
-      <c r="AT7" s="66"/>
-      <c r="AU7" s="66"/>
-      <c r="AV7" s="67"/>
+      <c r="AN7" s="75"/>
+      <c r="AO7" s="75"/>
+      <c r="AP7" s="75"/>
+      <c r="AQ7" s="75"/>
+      <c r="AR7" s="75"/>
+      <c r="AS7" s="75"/>
+      <c r="AT7" s="75"/>
+      <c r="AU7" s="75"/>
+      <c r="AV7" s="76"/>
       <c r="AW7" s="4"/>
     </row>
     <row r="8" spans="1:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4661,38 +4661,38 @@
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="17"/>
-      <c r="F9" s="177" t="s">
+      <c r="F9" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="178"/>
-      <c r="H9" s="178"/>
-      <c r="I9" s="178"/>
-      <c r="J9" s="178"/>
-      <c r="K9" s="178"/>
-      <c r="L9" s="178"/>
-      <c r="M9" s="178"/>
-      <c r="N9" s="178"/>
-      <c r="O9" s="178"/>
-      <c r="P9" s="178"/>
-      <c r="Q9" s="179"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="57"/>
+      <c r="N9" s="57"/>
+      <c r="O9" s="57"/>
+      <c r="P9" s="57"/>
+      <c r="Q9" s="58"/>
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
       <c r="T9" s="17"/>
       <c r="U9" s="17"/>
-      <c r="V9" s="177" t="s">
+      <c r="V9" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="W9" s="178"/>
-      <c r="X9" s="178"/>
-      <c r="Y9" s="178"/>
-      <c r="Z9" s="178"/>
-      <c r="AA9" s="178"/>
-      <c r="AB9" s="178"/>
-      <c r="AC9" s="178"/>
-      <c r="AD9" s="178"/>
-      <c r="AE9" s="178"/>
-      <c r="AF9" s="178"/>
-      <c r="AG9" s="179"/>
+      <c r="W9" s="57"/>
+      <c r="X9" s="57"/>
+      <c r="Y9" s="57"/>
+      <c r="Z9" s="57"/>
+      <c r="AA9" s="57"/>
+      <c r="AB9" s="57"/>
+      <c r="AC9" s="57"/>
+      <c r="AD9" s="57"/>
+      <c r="AE9" s="57"/>
+      <c r="AF9" s="57"/>
+      <c r="AG9" s="58"/>
       <c r="AH9" s="19"/>
       <c r="AI9" s="19"/>
       <c r="AJ9" s="4"/>
@@ -4714,34 +4714,34 @@
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="17"/>
-      <c r="F10" s="180"/>
-      <c r="G10" s="176"/>
-      <c r="H10" s="176"/>
-      <c r="I10" s="176"/>
-      <c r="J10" s="176"/>
-      <c r="K10" s="176"/>
-      <c r="L10" s="176"/>
-      <c r="M10" s="176"/>
-      <c r="N10" s="176"/>
-      <c r="O10" s="176"/>
-      <c r="P10" s="176"/>
-      <c r="Q10" s="181"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="60"/>
+      <c r="Q10" s="61"/>
       <c r="R10" s="17"/>
       <c r="S10" s="17"/>
       <c r="T10" s="17"/>
       <c r="U10" s="17"/>
-      <c r="V10" s="180"/>
-      <c r="W10" s="176"/>
-      <c r="X10" s="176"/>
-      <c r="Y10" s="176"/>
-      <c r="Z10" s="176"/>
-      <c r="AA10" s="176"/>
-      <c r="AB10" s="176"/>
-      <c r="AC10" s="176"/>
-      <c r="AD10" s="176"/>
-      <c r="AE10" s="176"/>
-      <c r="AF10" s="176"/>
-      <c r="AG10" s="181"/>
+      <c r="V10" s="59"/>
+      <c r="W10" s="60"/>
+      <c r="X10" s="60"/>
+      <c r="Y10" s="60"/>
+      <c r="Z10" s="60"/>
+      <c r="AA10" s="60"/>
+      <c r="AB10" s="60"/>
+      <c r="AC10" s="60"/>
+      <c r="AD10" s="60"/>
+      <c r="AE10" s="60"/>
+      <c r="AF10" s="60"/>
+      <c r="AG10" s="61"/>
       <c r="AH10" s="19"/>
       <c r="AI10" s="19"/>
       <c r="AJ10" s="4"/>
@@ -4762,30 +4762,30 @@
     <row r="11" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
-      <c r="F11" s="180"/>
-      <c r="G11" s="176"/>
-      <c r="H11" s="176"/>
-      <c r="I11" s="176"/>
-      <c r="J11" s="176"/>
-      <c r="K11" s="176"/>
-      <c r="L11" s="176"/>
-      <c r="M11" s="176"/>
-      <c r="N11" s="176"/>
-      <c r="O11" s="176"/>
-      <c r="P11" s="176"/>
-      <c r="Q11" s="181"/>
-      <c r="V11" s="180"/>
-      <c r="W11" s="176"/>
-      <c r="X11" s="176"/>
-      <c r="Y11" s="176"/>
-      <c r="Z11" s="176"/>
-      <c r="AA11" s="176"/>
-      <c r="AB11" s="176"/>
-      <c r="AC11" s="176"/>
-      <c r="AD11" s="176"/>
-      <c r="AE11" s="176"/>
-      <c r="AF11" s="176"/>
-      <c r="AG11" s="181"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
+      <c r="P11" s="60"/>
+      <c r="Q11" s="61"/>
+      <c r="V11" s="59"/>
+      <c r="W11" s="60"/>
+      <c r="X11" s="60"/>
+      <c r="Y11" s="60"/>
+      <c r="Z11" s="60"/>
+      <c r="AA11" s="60"/>
+      <c r="AB11" s="60"/>
+      <c r="AC11" s="60"/>
+      <c r="AD11" s="60"/>
+      <c r="AE11" s="60"/>
+      <c r="AF11" s="60"/>
+      <c r="AG11" s="61"/>
       <c r="AH11" s="11"/>
       <c r="AI11" s="11"/>
       <c r="AJ11" s="4"/>
@@ -4807,30 +4807,30 @@
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="17"/>
-      <c r="F12" s="180"/>
-      <c r="G12" s="176"/>
-      <c r="H12" s="176"/>
-      <c r="I12" s="176"/>
-      <c r="J12" s="176"/>
-      <c r="K12" s="176"/>
-      <c r="L12" s="176"/>
-      <c r="M12" s="176"/>
-      <c r="N12" s="176"/>
-      <c r="O12" s="176"/>
-      <c r="P12" s="176"/>
-      <c r="Q12" s="181"/>
-      <c r="V12" s="180"/>
-      <c r="W12" s="176"/>
-      <c r="X12" s="176"/>
-      <c r="Y12" s="176"/>
-      <c r="Z12" s="176"/>
-      <c r="AA12" s="176"/>
-      <c r="AB12" s="176"/>
-      <c r="AC12" s="176"/>
-      <c r="AD12" s="176"/>
-      <c r="AE12" s="176"/>
-      <c r="AF12" s="176"/>
-      <c r="AG12" s="181"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="60"/>
+      <c r="P12" s="60"/>
+      <c r="Q12" s="61"/>
+      <c r="V12" s="59"/>
+      <c r="W12" s="60"/>
+      <c r="X12" s="60"/>
+      <c r="Y12" s="60"/>
+      <c r="Z12" s="60"/>
+      <c r="AA12" s="60"/>
+      <c r="AB12" s="60"/>
+      <c r="AC12" s="60"/>
+      <c r="AD12" s="60"/>
+      <c r="AE12" s="60"/>
+      <c r="AF12" s="60"/>
+      <c r="AG12" s="61"/>
       <c r="AH12" s="19"/>
       <c r="AI12" s="19"/>
       <c r="AJ12" s="4"/>
@@ -4852,30 +4852,30 @@
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="17"/>
-      <c r="F13" s="182"/>
-      <c r="G13" s="183"/>
-      <c r="H13" s="183"/>
-      <c r="I13" s="183"/>
-      <c r="J13" s="183"/>
-      <c r="K13" s="183"/>
-      <c r="L13" s="183"/>
-      <c r="M13" s="183"/>
-      <c r="N13" s="183"/>
-      <c r="O13" s="183"/>
-      <c r="P13" s="183"/>
-      <c r="Q13" s="184"/>
-      <c r="V13" s="182"/>
-      <c r="W13" s="183"/>
-      <c r="X13" s="183"/>
-      <c r="Y13" s="183"/>
-      <c r="Z13" s="183"/>
-      <c r="AA13" s="183"/>
-      <c r="AB13" s="183"/>
-      <c r="AC13" s="183"/>
-      <c r="AD13" s="183"/>
-      <c r="AE13" s="183"/>
-      <c r="AF13" s="183"/>
-      <c r="AG13" s="184"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="63"/>
+      <c r="O13" s="63"/>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="64"/>
+      <c r="V13" s="62"/>
+      <c r="W13" s="63"/>
+      <c r="X13" s="63"/>
+      <c r="Y13" s="63"/>
+      <c r="Z13" s="63"/>
+      <c r="AA13" s="63"/>
+      <c r="AB13" s="63"/>
+      <c r="AC13" s="63"/>
+      <c r="AD13" s="63"/>
+      <c r="AE13" s="63"/>
+      <c r="AF13" s="63"/>
+      <c r="AG13" s="64"/>
       <c r="AH13" s="19"/>
       <c r="AI13" s="19"/>
       <c r="AJ13" s="4"/>
@@ -4973,34 +4973,34 @@
       <c r="C16" s="10"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="177" t="s">
+      <c r="F16" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="178"/>
-      <c r="H16" s="178"/>
-      <c r="I16" s="178"/>
-      <c r="J16" s="178"/>
-      <c r="K16" s="178"/>
-      <c r="L16" s="178"/>
-      <c r="M16" s="178"/>
-      <c r="N16" s="178"/>
-      <c r="O16" s="178"/>
-      <c r="P16" s="178"/>
-      <c r="Q16" s="179"/>
-      <c r="V16" s="177" t="s">
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="57"/>
+      <c r="Q16" s="58"/>
+      <c r="V16" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="W16" s="178"/>
-      <c r="X16" s="178"/>
-      <c r="Y16" s="178"/>
-      <c r="Z16" s="178"/>
-      <c r="AA16" s="178"/>
-      <c r="AB16" s="178"/>
-      <c r="AC16" s="178"/>
-      <c r="AD16" s="178"/>
-      <c r="AE16" s="178"/>
-      <c r="AF16" s="178"/>
-      <c r="AG16" s="179"/>
+      <c r="W16" s="57"/>
+      <c r="X16" s="57"/>
+      <c r="Y16" s="57"/>
+      <c r="Z16" s="57"/>
+      <c r="AA16" s="57"/>
+      <c r="AB16" s="57"/>
+      <c r="AC16" s="57"/>
+      <c r="AD16" s="57"/>
+      <c r="AE16" s="57"/>
+      <c r="AF16" s="57"/>
+      <c r="AG16" s="58"/>
       <c r="AH16" s="19"/>
       <c r="AI16" s="19"/>
       <c r="AJ16" s="4"/>
@@ -5023,33 +5023,33 @@
       <c r="C17" s="10"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="180"/>
-      <c r="G17" s="176"/>
-      <c r="H17" s="176"/>
-      <c r="I17" s="176"/>
-      <c r="J17" s="176"/>
-      <c r="K17" s="176"/>
-      <c r="L17" s="176"/>
-      <c r="M17" s="176"/>
-      <c r="N17" s="176"/>
-      <c r="O17" s="176"/>
-      <c r="P17" s="176"/>
-      <c r="Q17" s="181"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="60"/>
+      <c r="O17" s="60"/>
+      <c r="P17" s="60"/>
+      <c r="Q17" s="61"/>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
-      <c r="V17" s="180"/>
-      <c r="W17" s="176"/>
-      <c r="X17" s="176"/>
-      <c r="Y17" s="176"/>
-      <c r="Z17" s="176"/>
-      <c r="AA17" s="176"/>
-      <c r="AB17" s="176"/>
-      <c r="AC17" s="176"/>
-      <c r="AD17" s="176"/>
-      <c r="AE17" s="176"/>
-      <c r="AF17" s="176"/>
-      <c r="AG17" s="181"/>
+      <c r="V17" s="59"/>
+      <c r="W17" s="60"/>
+      <c r="X17" s="60"/>
+      <c r="Y17" s="60"/>
+      <c r="Z17" s="60"/>
+      <c r="AA17" s="60"/>
+      <c r="AB17" s="60"/>
+      <c r="AC17" s="60"/>
+      <c r="AD17" s="60"/>
+      <c r="AE17" s="60"/>
+      <c r="AF17" s="60"/>
+      <c r="AG17" s="61"/>
       <c r="AH17" s="19"/>
       <c r="AI17" s="19"/>
       <c r="AJ17" s="4"/>
@@ -5071,33 +5071,33 @@
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="3"/>
-      <c r="F18" s="180"/>
-      <c r="G18" s="176"/>
-      <c r="H18" s="176"/>
-      <c r="I18" s="176"/>
-      <c r="J18" s="176"/>
-      <c r="K18" s="176"/>
-      <c r="L18" s="176"/>
-      <c r="M18" s="176"/>
-      <c r="N18" s="176"/>
-      <c r="O18" s="176"/>
-      <c r="P18" s="176"/>
-      <c r="Q18" s="181"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="60"/>
+      <c r="P18" s="60"/>
+      <c r="Q18" s="61"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
-      <c r="V18" s="180"/>
-      <c r="W18" s="176"/>
-      <c r="X18" s="176"/>
-      <c r="Y18" s="176"/>
-      <c r="Z18" s="176"/>
-      <c r="AA18" s="176"/>
-      <c r="AB18" s="176"/>
-      <c r="AC18" s="176"/>
-      <c r="AD18" s="176"/>
-      <c r="AE18" s="176"/>
-      <c r="AF18" s="176"/>
-      <c r="AG18" s="181"/>
+      <c r="V18" s="59"/>
+      <c r="W18" s="60"/>
+      <c r="X18" s="60"/>
+      <c r="Y18" s="60"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="60"/>
+      <c r="AB18" s="60"/>
+      <c r="AC18" s="60"/>
+      <c r="AD18" s="60"/>
+      <c r="AE18" s="60"/>
+      <c r="AF18" s="60"/>
+      <c r="AG18" s="61"/>
       <c r="AH18" s="19"/>
       <c r="AI18" s="19"/>
       <c r="AJ18" s="4"/>
@@ -5119,33 +5119,33 @@
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="3"/>
-      <c r="F19" s="180"/>
-      <c r="G19" s="176"/>
-      <c r="H19" s="176"/>
-      <c r="I19" s="176"/>
-      <c r="J19" s="176"/>
-      <c r="K19" s="176"/>
-      <c r="L19" s="176"/>
-      <c r="M19" s="176"/>
-      <c r="N19" s="176"/>
-      <c r="O19" s="176"/>
-      <c r="P19" s="176"/>
-      <c r="Q19" s="181"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="60"/>
+      <c r="N19" s="60"/>
+      <c r="O19" s="60"/>
+      <c r="P19" s="60"/>
+      <c r="Q19" s="61"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
-      <c r="V19" s="180"/>
-      <c r="W19" s="176"/>
-      <c r="X19" s="176"/>
-      <c r="Y19" s="176"/>
-      <c r="Z19" s="176"/>
-      <c r="AA19" s="176"/>
-      <c r="AB19" s="176"/>
-      <c r="AC19" s="176"/>
-      <c r="AD19" s="176"/>
-      <c r="AE19" s="176"/>
-      <c r="AF19" s="176"/>
-      <c r="AG19" s="181"/>
+      <c r="V19" s="59"/>
+      <c r="W19" s="60"/>
+      <c r="X19" s="60"/>
+      <c r="Y19" s="60"/>
+      <c r="Z19" s="60"/>
+      <c r="AA19" s="60"/>
+      <c r="AB19" s="60"/>
+      <c r="AC19" s="60"/>
+      <c r="AD19" s="60"/>
+      <c r="AE19" s="60"/>
+      <c r="AF19" s="60"/>
+      <c r="AG19" s="61"/>
       <c r="AH19" s="11"/>
       <c r="AI19" s="11"/>
       <c r="AJ19" s="4"/>
@@ -5167,33 +5167,33 @@
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="3"/>
-      <c r="F20" s="182"/>
-      <c r="G20" s="183"/>
-      <c r="H20" s="183"/>
-      <c r="I20" s="183"/>
-      <c r="J20" s="183"/>
-      <c r="K20" s="183"/>
-      <c r="L20" s="183"/>
-      <c r="M20" s="183"/>
-      <c r="N20" s="183"/>
-      <c r="O20" s="183"/>
-      <c r="P20" s="183"/>
-      <c r="Q20" s="184"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="63"/>
+      <c r="Q20" s="64"/>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
-      <c r="V20" s="182"/>
-      <c r="W20" s="183"/>
-      <c r="X20" s="183"/>
-      <c r="Y20" s="183"/>
-      <c r="Z20" s="183"/>
-      <c r="AA20" s="183"/>
-      <c r="AB20" s="183"/>
-      <c r="AC20" s="183"/>
-      <c r="AD20" s="183"/>
-      <c r="AE20" s="183"/>
-      <c r="AF20" s="183"/>
-      <c r="AG20" s="184"/>
+      <c r="V20" s="62"/>
+      <c r="W20" s="63"/>
+      <c r="X20" s="63"/>
+      <c r="Y20" s="63"/>
+      <c r="Z20" s="63"/>
+      <c r="AA20" s="63"/>
+      <c r="AB20" s="63"/>
+      <c r="AC20" s="63"/>
+      <c r="AD20" s="63"/>
+      <c r="AE20" s="63"/>
+      <c r="AF20" s="63"/>
+      <c r="AG20" s="64"/>
       <c r="AH20" s="19"/>
       <c r="AI20" s="19"/>
       <c r="AJ20" s="4"/>
@@ -5373,27 +5373,27 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="11"/>
-      <c r="K25" s="56" t="s">
+      <c r="K25" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="L25" s="56"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="56"/>
-      <c r="O25" s="56"/>
-      <c r="P25" s="56"/>
-      <c r="Q25" s="56"/>
-      <c r="R25" s="56"/>
+      <c r="L25" s="65"/>
+      <c r="M25" s="65"/>
+      <c r="N25" s="65"/>
+      <c r="O25" s="65"/>
+      <c r="P25" s="65"/>
+      <c r="Q25" s="65"/>
+      <c r="R25" s="65"/>
       <c r="T25" s="3"/>
-      <c r="U25" s="56" t="s">
+      <c r="U25" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="V25" s="56"/>
-      <c r="W25" s="56"/>
-      <c r="X25" s="56"/>
-      <c r="Y25" s="56"/>
-      <c r="Z25" s="56"/>
-      <c r="AA25" s="56"/>
-      <c r="AB25" s="56"/>
+      <c r="V25" s="65"/>
+      <c r="W25" s="65"/>
+      <c r="X25" s="65"/>
+      <c r="Y25" s="65"/>
+      <c r="Z25" s="65"/>
+      <c r="AA25" s="65"/>
+      <c r="AB25" s="65"/>
       <c r="AD25" s="11"/>
       <c r="AE25" s="11"/>
       <c r="AF25" s="11"/>
@@ -5404,16 +5404,16 @@
       <c r="AK25" s="11"/>
       <c r="AL25" s="11"/>
       <c r="AM25" s="11"/>
-      <c r="AN25" s="56" t="s">
+      <c r="AN25" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="AO25" s="56"/>
-      <c r="AP25" s="56"/>
-      <c r="AQ25" s="56"/>
-      <c r="AR25" s="56"/>
-      <c r="AS25" s="56"/>
-      <c r="AT25" s="56"/>
-      <c r="AU25" s="56"/>
+      <c r="AO25" s="65"/>
+      <c r="AP25" s="65"/>
+      <c r="AQ25" s="65"/>
+      <c r="AR25" s="65"/>
+      <c r="AS25" s="65"/>
+      <c r="AT25" s="65"/>
+      <c r="AU25" s="65"/>
       <c r="AW25" s="4"/>
     </row>
     <row r="26" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -5428,23 +5428,23 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="11"/>
-      <c r="K26" s="56"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="56"/>
-      <c r="N26" s="56"/>
-      <c r="O26" s="56"/>
-      <c r="P26" s="56"/>
-      <c r="Q26" s="56"/>
-      <c r="R26" s="56"/>
+      <c r="K26" s="65"/>
+      <c r="L26" s="65"/>
+      <c r="M26" s="65"/>
+      <c r="N26" s="65"/>
+      <c r="O26" s="65"/>
+      <c r="P26" s="65"/>
+      <c r="Q26" s="65"/>
+      <c r="R26" s="65"/>
       <c r="T26" s="3"/>
-      <c r="U26" s="56"/>
-      <c r="V26" s="56"/>
-      <c r="W26" s="56"/>
-      <c r="X26" s="56"/>
-      <c r="Y26" s="56"/>
-      <c r="Z26" s="56"/>
-      <c r="AA26" s="56"/>
-      <c r="AB26" s="56"/>
+      <c r="U26" s="65"/>
+      <c r="V26" s="65"/>
+      <c r="W26" s="65"/>
+      <c r="X26" s="65"/>
+      <c r="Y26" s="65"/>
+      <c r="Z26" s="65"/>
+      <c r="AA26" s="65"/>
+      <c r="AB26" s="65"/>
       <c r="AD26" s="11"/>
       <c r="AE26" s="11"/>
       <c r="AF26" s="11"/>
@@ -5455,14 +5455,14 @@
       <c r="AK26" s="11"/>
       <c r="AL26" s="11"/>
       <c r="AM26" s="11"/>
-      <c r="AN26" s="56"/>
-      <c r="AO26" s="56"/>
-      <c r="AP26" s="56"/>
-      <c r="AQ26" s="56"/>
-      <c r="AR26" s="56"/>
-      <c r="AS26" s="56"/>
-      <c r="AT26" s="56"/>
-      <c r="AU26" s="56"/>
+      <c r="AN26" s="65"/>
+      <c r="AO26" s="65"/>
+      <c r="AP26" s="65"/>
+      <c r="AQ26" s="65"/>
+      <c r="AR26" s="65"/>
+      <c r="AS26" s="65"/>
+      <c r="AT26" s="65"/>
+      <c r="AU26" s="65"/>
       <c r="AW26" s="4"/>
     </row>
     <row r="27" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -5475,23 +5475,23 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
-      <c r="K27" s="56"/>
-      <c r="L27" s="56"/>
-      <c r="M27" s="56"/>
-      <c r="N27" s="56"/>
-      <c r="O27" s="56"/>
-      <c r="P27" s="56"/>
-      <c r="Q27" s="56"/>
-      <c r="R27" s="56"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="65"/>
+      <c r="N27" s="65"/>
+      <c r="O27" s="65"/>
+      <c r="P27" s="65"/>
+      <c r="Q27" s="65"/>
+      <c r="R27" s="65"/>
       <c r="T27" s="11"/>
-      <c r="U27" s="56"/>
-      <c r="V27" s="56"/>
-      <c r="W27" s="56"/>
-      <c r="X27" s="56"/>
-      <c r="Y27" s="56"/>
-      <c r="Z27" s="56"/>
-      <c r="AA27" s="56"/>
-      <c r="AB27" s="56"/>
+      <c r="U27" s="65"/>
+      <c r="V27" s="65"/>
+      <c r="W27" s="65"/>
+      <c r="X27" s="65"/>
+      <c r="Y27" s="65"/>
+      <c r="Z27" s="65"/>
+      <c r="AA27" s="65"/>
+      <c r="AB27" s="65"/>
       <c r="AD27" s="11"/>
       <c r="AE27" s="11"/>
       <c r="AF27" s="11"/>
@@ -5502,14 +5502,14 @@
       <c r="AK27" s="11"/>
       <c r="AL27" s="11"/>
       <c r="AM27" s="11"/>
-      <c r="AN27" s="56"/>
-      <c r="AO27" s="56"/>
-      <c r="AP27" s="56"/>
-      <c r="AQ27" s="56"/>
-      <c r="AR27" s="56"/>
-      <c r="AS27" s="56"/>
-      <c r="AT27" s="56"/>
-      <c r="AU27" s="56"/>
+      <c r="AN27" s="65"/>
+      <c r="AO27" s="65"/>
+      <c r="AP27" s="65"/>
+      <c r="AQ27" s="65"/>
+      <c r="AR27" s="65"/>
+      <c r="AS27" s="65"/>
+      <c r="AT27" s="65"/>
+      <c r="AU27" s="65"/>
       <c r="AW27" s="4"/>
     </row>
     <row r="28" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5564,18 +5564,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="U3:AD4"/>
+    <mergeCell ref="AN25:AU27"/>
+    <mergeCell ref="D2:L5"/>
+    <mergeCell ref="M4:P6"/>
+    <mergeCell ref="AT3:AV5"/>
+    <mergeCell ref="AM7:AV7"/>
     <mergeCell ref="V16:AG20"/>
     <mergeCell ref="F9:Q13"/>
     <mergeCell ref="V9:AG13"/>
     <mergeCell ref="F16:Q20"/>
     <mergeCell ref="K25:R27"/>
     <mergeCell ref="U25:AB27"/>
-    <mergeCell ref="U3:AD4"/>
-    <mergeCell ref="AN25:AU27"/>
-    <mergeCell ref="D2:L5"/>
-    <mergeCell ref="M4:P6"/>
-    <mergeCell ref="AT3:AV5"/>
-    <mergeCell ref="AM7:AV7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="U25:Z26" location="CreateRoom!A1" display="Create Room"/>
@@ -5595,8 +5595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AW28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25:R27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5609,17 +5609,17 @@
     <row r="2" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -5705,11 +5705,11 @@
       <c r="AQ3" s="3"/>
       <c r="AR3" s="11"/>
       <c r="AS3" s="11"/>
-      <c r="AT3" s="64" t="s">
+      <c r="AT3" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="AU3" s="64"/>
-      <c r="AV3" s="64"/>
+      <c r="AU3" s="73"/>
+      <c r="AV3" s="73"/>
       <c r="AW3" s="12"/>
     </row>
     <row r="4" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -5748,9 +5748,9 @@
       <c r="AQ4" s="3"/>
       <c r="AR4" s="11"/>
       <c r="AS4" s="11"/>
-      <c r="AT4" s="64"/>
-      <c r="AU4" s="64"/>
-      <c r="AV4" s="64"/>
+      <c r="AT4" s="73"/>
+      <c r="AU4" s="73"/>
+      <c r="AV4" s="73"/>
       <c r="AW4" s="12"/>
     </row>
     <row r="5" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -5785,9 +5785,9 @@
       <c r="AQ5" s="11"/>
       <c r="AR5" s="11"/>
       <c r="AS5" s="11"/>
-      <c r="AT5" s="64"/>
-      <c r="AU5" s="64"/>
-      <c r="AV5" s="64"/>
+      <c r="AT5" s="73"/>
+      <c r="AU5" s="73"/>
+      <c r="AV5" s="73"/>
       <c r="AW5" s="12"/>
     </row>
     <row r="6" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5864,18 +5864,18 @@
       <c r="AI7" s="8"/>
       <c r="AJ7" s="9"/>
       <c r="AL7" s="11"/>
-      <c r="AM7" s="65" t="s">
+      <c r="AM7" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="AN7" s="66"/>
-      <c r="AO7" s="66"/>
-      <c r="AP7" s="66"/>
-      <c r="AQ7" s="66"/>
-      <c r="AR7" s="66"/>
-      <c r="AS7" s="66"/>
-      <c r="AT7" s="66"/>
-      <c r="AU7" s="66"/>
-      <c r="AV7" s="67"/>
+      <c r="AN7" s="75"/>
+      <c r="AO7" s="75"/>
+      <c r="AP7" s="75"/>
+      <c r="AQ7" s="75"/>
+      <c r="AR7" s="75"/>
+      <c r="AS7" s="75"/>
+      <c r="AT7" s="75"/>
+      <c r="AU7" s="75"/>
+      <c r="AV7" s="76"/>
       <c r="AW7" s="4"/>
     </row>
     <row r="8" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5901,40 +5901,40 @@
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="69" t="s">
+      <c r="E9" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="70"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="70"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="70"/>
-      <c r="K9" s="70"/>
-      <c r="L9" s="70"/>
-      <c r="M9" s="70"/>
-      <c r="N9" s="70"/>
-      <c r="O9" s="70"/>
-      <c r="P9" s="70"/>
-      <c r="Q9" s="70"/>
-      <c r="R9" s="71"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="79"/>
+      <c r="N9" s="79"/>
+      <c r="O9" s="79"/>
+      <c r="P9" s="79"/>
+      <c r="Q9" s="79"/>
+      <c r="R9" s="80"/>
       <c r="S9" s="17"/>
       <c r="T9" s="17"/>
-      <c r="U9" s="69" t="s">
+      <c r="U9" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="70"/>
-      <c r="W9" s="70"/>
-      <c r="X9" s="70"/>
-      <c r="Y9" s="70"/>
-      <c r="Z9" s="70"/>
-      <c r="AA9" s="70"/>
-      <c r="AB9" s="70"/>
-      <c r="AC9" s="70"/>
-      <c r="AD9" s="70"/>
-      <c r="AE9" s="70"/>
-      <c r="AF9" s="70"/>
-      <c r="AG9" s="70"/>
-      <c r="AH9" s="71"/>
+      <c r="V9" s="79"/>
+      <c r="W9" s="79"/>
+      <c r="X9" s="79"/>
+      <c r="Y9" s="79"/>
+      <c r="Z9" s="79"/>
+      <c r="AA9" s="79"/>
+      <c r="AB9" s="79"/>
+      <c r="AC9" s="79"/>
+      <c r="AD9" s="79"/>
+      <c r="AE9" s="79"/>
+      <c r="AF9" s="79"/>
+      <c r="AG9" s="79"/>
+      <c r="AH9" s="80"/>
       <c r="AI9" s="17"/>
       <c r="AJ9" s="4"/>
       <c r="AL9" s="3"/>
@@ -5954,36 +5954,36 @@
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
-      <c r="R10" s="74"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="82"/>
+      <c r="O10" s="82"/>
+      <c r="P10" s="82"/>
+      <c r="Q10" s="82"/>
+      <c r="R10" s="83"/>
       <c r="S10" s="17"/>
       <c r="T10" s="17"/>
-      <c r="U10" s="72"/>
-      <c r="V10" s="73"/>
-      <c r="W10" s="73"/>
-      <c r="X10" s="73"/>
-      <c r="Y10" s="73"/>
-      <c r="Z10" s="73"/>
-      <c r="AA10" s="73"/>
-      <c r="AB10" s="73"/>
-      <c r="AC10" s="73"/>
-      <c r="AD10" s="73"/>
-      <c r="AE10" s="73"/>
-      <c r="AF10" s="73"/>
-      <c r="AG10" s="73"/>
-      <c r="AH10" s="74"/>
+      <c r="U10" s="81"/>
+      <c r="V10" s="82"/>
+      <c r="W10" s="82"/>
+      <c r="X10" s="82"/>
+      <c r="Y10" s="82"/>
+      <c r="Z10" s="82"/>
+      <c r="AA10" s="82"/>
+      <c r="AB10" s="82"/>
+      <c r="AC10" s="82"/>
+      <c r="AD10" s="82"/>
+      <c r="AE10" s="82"/>
+      <c r="AF10" s="82"/>
+      <c r="AG10" s="82"/>
+      <c r="AH10" s="83"/>
       <c r="AI10" s="17"/>
       <c r="AJ10" s="4"/>
       <c r="AL10" s="3"/>
@@ -6002,36 +6002,36 @@
     <row r="11" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
-      <c r="R11" s="74"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="82"/>
+      <c r="O11" s="82"/>
+      <c r="P11" s="82"/>
+      <c r="Q11" s="82"/>
+      <c r="R11" s="83"/>
       <c r="S11" s="17"/>
       <c r="T11" s="17"/>
-      <c r="U11" s="72"/>
-      <c r="V11" s="73"/>
-      <c r="W11" s="73"/>
-      <c r="X11" s="73"/>
-      <c r="Y11" s="73"/>
-      <c r="Z11" s="73"/>
-      <c r="AA11" s="73"/>
-      <c r="AB11" s="73"/>
-      <c r="AC11" s="73"/>
-      <c r="AD11" s="73"/>
-      <c r="AE11" s="73"/>
-      <c r="AF11" s="73"/>
-      <c r="AG11" s="73"/>
-      <c r="AH11" s="74"/>
+      <c r="U11" s="81"/>
+      <c r="V11" s="82"/>
+      <c r="W11" s="82"/>
+      <c r="X11" s="82"/>
+      <c r="Y11" s="82"/>
+      <c r="Z11" s="82"/>
+      <c r="AA11" s="82"/>
+      <c r="AB11" s="82"/>
+      <c r="AC11" s="82"/>
+      <c r="AD11" s="82"/>
+      <c r="AE11" s="82"/>
+      <c r="AF11" s="82"/>
+      <c r="AG11" s="82"/>
+      <c r="AH11" s="83"/>
       <c r="AJ11" s="4"/>
       <c r="AL11" s="3"/>
       <c r="AM11" s="10"/>
@@ -6050,34 +6050,34 @@
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="17"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
-      <c r="J12" s="73"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="73"/>
-      <c r="M12" s="73"/>
-      <c r="N12" s="73"/>
-      <c r="O12" s="73"/>
-      <c r="P12" s="73"/>
-      <c r="Q12" s="73"/>
-      <c r="R12" s="74"/>
-      <c r="U12" s="72"/>
-      <c r="V12" s="73"/>
-      <c r="W12" s="73"/>
-      <c r="X12" s="73"/>
-      <c r="Y12" s="73"/>
-      <c r="Z12" s="73"/>
-      <c r="AA12" s="73"/>
-      <c r="AB12" s="73"/>
-      <c r="AC12" s="73"/>
-      <c r="AD12" s="73"/>
-      <c r="AE12" s="73"/>
-      <c r="AF12" s="73"/>
-      <c r="AG12" s="73"/>
-      <c r="AH12" s="74"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
+      <c r="O12" s="82"/>
+      <c r="P12" s="82"/>
+      <c r="Q12" s="82"/>
+      <c r="R12" s="83"/>
+      <c r="U12" s="81"/>
+      <c r="V12" s="82"/>
+      <c r="W12" s="82"/>
+      <c r="X12" s="82"/>
+      <c r="Y12" s="82"/>
+      <c r="Z12" s="82"/>
+      <c r="AA12" s="82"/>
+      <c r="AB12" s="82"/>
+      <c r="AC12" s="82"/>
+      <c r="AD12" s="82"/>
+      <c r="AE12" s="82"/>
+      <c r="AF12" s="82"/>
+      <c r="AG12" s="82"/>
+      <c r="AH12" s="83"/>
       <c r="AI12" s="17"/>
       <c r="AJ12" s="4"/>
       <c r="AL12" s="3"/>
@@ -6097,36 +6097,36 @@
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="17"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="73"/>
-      <c r="L13" s="73"/>
-      <c r="M13" s="73"/>
-      <c r="N13" s="73"/>
-      <c r="O13" s="73"/>
-      <c r="P13" s="73"/>
-      <c r="Q13" s="73"/>
-      <c r="R13" s="74"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="82"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
+      <c r="O13" s="82"/>
+      <c r="P13" s="82"/>
+      <c r="Q13" s="82"/>
+      <c r="R13" s="83"/>
       <c r="S13" s="17"/>
       <c r="T13" s="17"/>
-      <c r="U13" s="72"/>
-      <c r="V13" s="73"/>
-      <c r="W13" s="73"/>
-      <c r="X13" s="73"/>
-      <c r="Y13" s="73"/>
-      <c r="Z13" s="73"/>
-      <c r="AA13" s="73"/>
-      <c r="AB13" s="73"/>
-      <c r="AC13" s="73"/>
-      <c r="AD13" s="73"/>
-      <c r="AE13" s="73"/>
-      <c r="AF13" s="73"/>
-      <c r="AG13" s="73"/>
-      <c r="AH13" s="74"/>
+      <c r="U13" s="81"/>
+      <c r="V13" s="82"/>
+      <c r="W13" s="82"/>
+      <c r="X13" s="82"/>
+      <c r="Y13" s="82"/>
+      <c r="Z13" s="82"/>
+      <c r="AA13" s="82"/>
+      <c r="AB13" s="82"/>
+      <c r="AC13" s="82"/>
+      <c r="AD13" s="82"/>
+      <c r="AE13" s="82"/>
+      <c r="AF13" s="82"/>
+      <c r="AG13" s="82"/>
+      <c r="AH13" s="83"/>
       <c r="AI13" s="17"/>
       <c r="AJ13" s="4"/>
       <c r="AL13" s="3"/>
@@ -6146,36 +6146,36 @@
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="17"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="73"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="73"/>
-      <c r="L14" s="73"/>
-      <c r="M14" s="73"/>
-      <c r="N14" s="73"/>
-      <c r="O14" s="73"/>
-      <c r="P14" s="73"/>
-      <c r="Q14" s="73"/>
-      <c r="R14" s="74"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="82"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="82"/>
+      <c r="Q14" s="82"/>
+      <c r="R14" s="83"/>
       <c r="S14" s="17"/>
       <c r="T14" s="17"/>
-      <c r="U14" s="72"/>
-      <c r="V14" s="73"/>
-      <c r="W14" s="73"/>
-      <c r="X14" s="73"/>
-      <c r="Y14" s="73"/>
-      <c r="Z14" s="73"/>
-      <c r="AA14" s="73"/>
-      <c r="AB14" s="73"/>
-      <c r="AC14" s="73"/>
-      <c r="AD14" s="73"/>
-      <c r="AE14" s="73"/>
-      <c r="AF14" s="73"/>
-      <c r="AG14" s="73"/>
-      <c r="AH14" s="74"/>
+      <c r="U14" s="81"/>
+      <c r="V14" s="82"/>
+      <c r="W14" s="82"/>
+      <c r="X14" s="82"/>
+      <c r="Y14" s="82"/>
+      <c r="Z14" s="82"/>
+      <c r="AA14" s="82"/>
+      <c r="AB14" s="82"/>
+      <c r="AC14" s="82"/>
+      <c r="AD14" s="82"/>
+      <c r="AE14" s="82"/>
+      <c r="AF14" s="82"/>
+      <c r="AG14" s="82"/>
+      <c r="AH14" s="83"/>
       <c r="AI14" s="17"/>
       <c r="AJ14" s="4"/>
       <c r="AL14" s="3"/>
@@ -6194,36 +6194,36 @@
     <row r="15" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="73"/>
-      <c r="N15" s="73"/>
-      <c r="O15" s="73"/>
-      <c r="P15" s="73"/>
-      <c r="Q15" s="73"/>
-      <c r="R15" s="74"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="82"/>
+      <c r="K15" s="82"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="82"/>
+      <c r="N15" s="82"/>
+      <c r="O15" s="82"/>
+      <c r="P15" s="82"/>
+      <c r="Q15" s="82"/>
+      <c r="R15" s="83"/>
       <c r="S15" s="17"/>
       <c r="T15" s="17"/>
-      <c r="U15" s="72"/>
-      <c r="V15" s="73"/>
-      <c r="W15" s="73"/>
-      <c r="X15" s="73"/>
-      <c r="Y15" s="73"/>
-      <c r="Z15" s="73"/>
-      <c r="AA15" s="73"/>
-      <c r="AB15" s="73"/>
-      <c r="AC15" s="73"/>
-      <c r="AD15" s="73"/>
-      <c r="AE15" s="73"/>
-      <c r="AF15" s="73"/>
-      <c r="AG15" s="73"/>
-      <c r="AH15" s="74"/>
+      <c r="U15" s="81"/>
+      <c r="V15" s="82"/>
+      <c r="W15" s="82"/>
+      <c r="X15" s="82"/>
+      <c r="Y15" s="82"/>
+      <c r="Z15" s="82"/>
+      <c r="AA15" s="82"/>
+      <c r="AB15" s="82"/>
+      <c r="AC15" s="82"/>
+      <c r="AD15" s="82"/>
+      <c r="AE15" s="82"/>
+      <c r="AF15" s="82"/>
+      <c r="AG15" s="82"/>
+      <c r="AH15" s="83"/>
       <c r="AJ15" s="4"/>
       <c r="AL15" s="3"/>
       <c r="AM15" s="10"/>
@@ -6242,34 +6242,34 @@
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="17"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="73"/>
-      <c r="N16" s="73"/>
-      <c r="O16" s="73"/>
-      <c r="P16" s="73"/>
-      <c r="Q16" s="73"/>
-      <c r="R16" s="74"/>
-      <c r="U16" s="72"/>
-      <c r="V16" s="73"/>
-      <c r="W16" s="73"/>
-      <c r="X16" s="73"/>
-      <c r="Y16" s="73"/>
-      <c r="Z16" s="73"/>
-      <c r="AA16" s="73"/>
-      <c r="AB16" s="73"/>
-      <c r="AC16" s="73"/>
-      <c r="AD16" s="73"/>
-      <c r="AE16" s="73"/>
-      <c r="AF16" s="73"/>
-      <c r="AG16" s="73"/>
-      <c r="AH16" s="74"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="82"/>
+      <c r="G16" s="82"/>
+      <c r="H16" s="82"/>
+      <c r="I16" s="82"/>
+      <c r="J16" s="82"/>
+      <c r="K16" s="82"/>
+      <c r="L16" s="82"/>
+      <c r="M16" s="82"/>
+      <c r="N16" s="82"/>
+      <c r="O16" s="82"/>
+      <c r="P16" s="82"/>
+      <c r="Q16" s="82"/>
+      <c r="R16" s="83"/>
+      <c r="U16" s="81"/>
+      <c r="V16" s="82"/>
+      <c r="W16" s="82"/>
+      <c r="X16" s="82"/>
+      <c r="Y16" s="82"/>
+      <c r="Z16" s="82"/>
+      <c r="AA16" s="82"/>
+      <c r="AB16" s="82"/>
+      <c r="AC16" s="82"/>
+      <c r="AD16" s="82"/>
+      <c r="AE16" s="82"/>
+      <c r="AF16" s="82"/>
+      <c r="AG16" s="82"/>
+      <c r="AH16" s="83"/>
       <c r="AI16" s="17"/>
       <c r="AJ16" s="4"/>
       <c r="AL16" s="3"/>
@@ -6289,36 +6289,36 @@
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="17"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="73"/>
-      <c r="J17" s="73"/>
-      <c r="K17" s="73"/>
-      <c r="L17" s="73"/>
-      <c r="M17" s="73"/>
-      <c r="N17" s="73"/>
-      <c r="O17" s="73"/>
-      <c r="P17" s="73"/>
-      <c r="Q17" s="73"/>
-      <c r="R17" s="74"/>
+      <c r="E17" s="81"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="82"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="82"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="82"/>
+      <c r="N17" s="82"/>
+      <c r="O17" s="82"/>
+      <c r="P17" s="82"/>
+      <c r="Q17" s="82"/>
+      <c r="R17" s="83"/>
       <c r="S17" s="17"/>
       <c r="T17" s="17"/>
-      <c r="U17" s="72"/>
-      <c r="V17" s="73"/>
-      <c r="W17" s="73"/>
-      <c r="X17" s="73"/>
-      <c r="Y17" s="73"/>
-      <c r="Z17" s="73"/>
-      <c r="AA17" s="73"/>
-      <c r="AB17" s="73"/>
-      <c r="AC17" s="73"/>
-      <c r="AD17" s="73"/>
-      <c r="AE17" s="73"/>
-      <c r="AF17" s="73"/>
-      <c r="AG17" s="73"/>
-      <c r="AH17" s="74"/>
+      <c r="U17" s="81"/>
+      <c r="V17" s="82"/>
+      <c r="W17" s="82"/>
+      <c r="X17" s="82"/>
+      <c r="Y17" s="82"/>
+      <c r="Z17" s="82"/>
+      <c r="AA17" s="82"/>
+      <c r="AB17" s="82"/>
+      <c r="AC17" s="82"/>
+      <c r="AD17" s="82"/>
+      <c r="AE17" s="82"/>
+      <c r="AF17" s="82"/>
+      <c r="AG17" s="82"/>
+      <c r="AH17" s="83"/>
       <c r="AI17" s="17"/>
       <c r="AJ17" s="4"/>
       <c r="AL17" s="3"/>
@@ -6338,36 +6338,36 @@
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="17"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="73"/>
-      <c r="K18" s="73"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="73"/>
-      <c r="N18" s="73"/>
-      <c r="O18" s="73"/>
-      <c r="P18" s="73"/>
-      <c r="Q18" s="73"/>
-      <c r="R18" s="74"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="82"/>
+      <c r="G18" s="82"/>
+      <c r="H18" s="82"/>
+      <c r="I18" s="82"/>
+      <c r="J18" s="82"/>
+      <c r="K18" s="82"/>
+      <c r="L18" s="82"/>
+      <c r="M18" s="82"/>
+      <c r="N18" s="82"/>
+      <c r="O18" s="82"/>
+      <c r="P18" s="82"/>
+      <c r="Q18" s="82"/>
+      <c r="R18" s="83"/>
       <c r="S18" s="17"/>
       <c r="T18" s="17"/>
-      <c r="U18" s="72"/>
-      <c r="V18" s="73"/>
-      <c r="W18" s="73"/>
-      <c r="X18" s="73"/>
-      <c r="Y18" s="73"/>
-      <c r="Z18" s="73"/>
-      <c r="AA18" s="73"/>
-      <c r="AB18" s="73"/>
-      <c r="AC18" s="73"/>
-      <c r="AD18" s="73"/>
-      <c r="AE18" s="73"/>
-      <c r="AF18" s="73"/>
-      <c r="AG18" s="73"/>
-      <c r="AH18" s="74"/>
+      <c r="U18" s="81"/>
+      <c r="V18" s="82"/>
+      <c r="W18" s="82"/>
+      <c r="X18" s="82"/>
+      <c r="Y18" s="82"/>
+      <c r="Z18" s="82"/>
+      <c r="AA18" s="82"/>
+      <c r="AB18" s="82"/>
+      <c r="AC18" s="82"/>
+      <c r="AD18" s="82"/>
+      <c r="AE18" s="82"/>
+      <c r="AF18" s="82"/>
+      <c r="AG18" s="82"/>
+      <c r="AH18" s="83"/>
       <c r="AI18" s="17"/>
       <c r="AJ18" s="4"/>
       <c r="AL18" s="3"/>
@@ -6386,36 +6386,36 @@
     <row r="19" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="76"/>
-      <c r="I19" s="76"/>
-      <c r="J19" s="76"/>
-      <c r="K19" s="76"/>
-      <c r="L19" s="76"/>
-      <c r="M19" s="76"/>
-      <c r="N19" s="76"/>
-      <c r="O19" s="76"/>
-      <c r="P19" s="76"/>
-      <c r="Q19" s="76"/>
-      <c r="R19" s="77"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="85"/>
+      <c r="I19" s="85"/>
+      <c r="J19" s="85"/>
+      <c r="K19" s="85"/>
+      <c r="L19" s="85"/>
+      <c r="M19" s="85"/>
+      <c r="N19" s="85"/>
+      <c r="O19" s="85"/>
+      <c r="P19" s="85"/>
+      <c r="Q19" s="85"/>
+      <c r="R19" s="86"/>
       <c r="S19" s="17"/>
       <c r="T19" s="17"/>
-      <c r="U19" s="75"/>
-      <c r="V19" s="76"/>
-      <c r="W19" s="76"/>
-      <c r="X19" s="76"/>
-      <c r="Y19" s="76"/>
-      <c r="Z19" s="76"/>
-      <c r="AA19" s="76"/>
-      <c r="AB19" s="76"/>
-      <c r="AC19" s="76"/>
-      <c r="AD19" s="76"/>
-      <c r="AE19" s="76"/>
-      <c r="AF19" s="76"/>
-      <c r="AG19" s="76"/>
-      <c r="AH19" s="77"/>
+      <c r="U19" s="84"/>
+      <c r="V19" s="85"/>
+      <c r="W19" s="85"/>
+      <c r="X19" s="85"/>
+      <c r="Y19" s="85"/>
+      <c r="Z19" s="85"/>
+      <c r="AA19" s="85"/>
+      <c r="AB19" s="85"/>
+      <c r="AC19" s="85"/>
+      <c r="AD19" s="85"/>
+      <c r="AE19" s="85"/>
+      <c r="AF19" s="85"/>
+      <c r="AG19" s="85"/>
+      <c r="AH19" s="86"/>
       <c r="AJ19" s="4"/>
       <c r="AL19" s="3"/>
       <c r="AM19" s="10"/>
@@ -6454,40 +6454,40 @@
       <c r="C21" s="10"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
-      <c r="F21" s="78" t="s">
+      <c r="F21" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="79"/>
-      <c r="H21" s="79"/>
-      <c r="I21" s="79"/>
-      <c r="J21" s="79"/>
-      <c r="K21" s="79"/>
-      <c r="L21" s="79"/>
-      <c r="M21" s="79"/>
-      <c r="N21" s="79"/>
-      <c r="O21" s="79"/>
-      <c r="P21" s="79"/>
-      <c r="Q21" s="80"/>
+      <c r="G21" s="88"/>
+      <c r="H21" s="88"/>
+      <c r="I21" s="88"/>
+      <c r="J21" s="88"/>
+      <c r="K21" s="88"/>
+      <c r="L21" s="88"/>
+      <c r="M21" s="88"/>
+      <c r="N21" s="88"/>
+      <c r="O21" s="88"/>
+      <c r="P21" s="88"/>
+      <c r="Q21" s="89"/>
       <c r="R21" s="17"/>
-      <c r="S21" s="68" t="s">
+      <c r="S21" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="T21" s="68"/>
+      <c r="T21" s="77"/>
       <c r="U21" s="17"/>
-      <c r="V21" s="78" t="s">
+      <c r="V21" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="W21" s="79"/>
-      <c r="X21" s="79"/>
-      <c r="Y21" s="79"/>
-      <c r="Z21" s="79"/>
-      <c r="AA21" s="79"/>
-      <c r="AB21" s="79"/>
-      <c r="AC21" s="79"/>
-      <c r="AD21" s="79"/>
-      <c r="AE21" s="79"/>
-      <c r="AF21" s="79"/>
-      <c r="AG21" s="80"/>
+      <c r="W21" s="88"/>
+      <c r="X21" s="88"/>
+      <c r="Y21" s="88"/>
+      <c r="Z21" s="88"/>
+      <c r="AA21" s="88"/>
+      <c r="AB21" s="88"/>
+      <c r="AC21" s="88"/>
+      <c r="AD21" s="88"/>
+      <c r="AE21" s="88"/>
+      <c r="AF21" s="88"/>
+      <c r="AG21" s="89"/>
       <c r="AH21" s="17"/>
       <c r="AI21" s="17"/>
       <c r="AJ21" s="4"/>
@@ -6509,34 +6509,34 @@
       <c r="C22" s="10"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="82"/>
-      <c r="H22" s="82"/>
-      <c r="I22" s="82"/>
-      <c r="J22" s="82"/>
-      <c r="K22" s="82"/>
-      <c r="L22" s="82"/>
-      <c r="M22" s="82"/>
-      <c r="N22" s="82"/>
-      <c r="O22" s="82"/>
-      <c r="P22" s="82"/>
-      <c r="Q22" s="83"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="91"/>
+      <c r="H22" s="91"/>
+      <c r="I22" s="91"/>
+      <c r="J22" s="91"/>
+      <c r="K22" s="91"/>
+      <c r="L22" s="91"/>
+      <c r="M22" s="91"/>
+      <c r="N22" s="91"/>
+      <c r="O22" s="91"/>
+      <c r="P22" s="91"/>
+      <c r="Q22" s="92"/>
       <c r="R22" s="17"/>
-      <c r="S22" s="68"/>
-      <c r="T22" s="68"/>
+      <c r="S22" s="77"/>
+      <c r="T22" s="77"/>
       <c r="U22" s="17"/>
-      <c r="V22" s="81"/>
-      <c r="W22" s="82"/>
-      <c r="X22" s="82"/>
-      <c r="Y22" s="82"/>
-      <c r="Z22" s="82"/>
-      <c r="AA22" s="82"/>
-      <c r="AB22" s="82"/>
-      <c r="AC22" s="82"/>
-      <c r="AD22" s="82"/>
-      <c r="AE22" s="82"/>
-      <c r="AF22" s="82"/>
-      <c r="AG22" s="83"/>
+      <c r="V22" s="90"/>
+      <c r="W22" s="91"/>
+      <c r="X22" s="91"/>
+      <c r="Y22" s="91"/>
+      <c r="Z22" s="91"/>
+      <c r="AA22" s="91"/>
+      <c r="AB22" s="91"/>
+      <c r="AC22" s="91"/>
+      <c r="AD22" s="91"/>
+      <c r="AE22" s="91"/>
+      <c r="AF22" s="91"/>
+      <c r="AG22" s="92"/>
       <c r="AH22" s="17"/>
       <c r="AI22" s="17"/>
       <c r="AJ22" s="4"/>
@@ -6686,16 +6686,16 @@
       <c r="AK25" s="11"/>
       <c r="AL25" s="11"/>
       <c r="AM25" s="11"/>
-      <c r="AN25" s="56" t="s">
+      <c r="AN25" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="AO25" s="56"/>
-      <c r="AP25" s="56"/>
-      <c r="AQ25" s="56"/>
-      <c r="AR25" s="56"/>
-      <c r="AS25" s="56"/>
-      <c r="AT25" s="56"/>
-      <c r="AU25" s="56"/>
+      <c r="AO25" s="65"/>
+      <c r="AP25" s="65"/>
+      <c r="AQ25" s="65"/>
+      <c r="AR25" s="65"/>
+      <c r="AS25" s="65"/>
+      <c r="AT25" s="65"/>
+      <c r="AU25" s="65"/>
       <c r="AW25" s="4"/>
     </row>
     <row r="26" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6731,14 +6731,14 @@
       <c r="AK26" s="11"/>
       <c r="AL26" s="11"/>
       <c r="AM26" s="11"/>
-      <c r="AN26" s="56"/>
-      <c r="AO26" s="56"/>
-      <c r="AP26" s="56"/>
-      <c r="AQ26" s="56"/>
-      <c r="AR26" s="56"/>
-      <c r="AS26" s="56"/>
-      <c r="AT26" s="56"/>
-      <c r="AU26" s="56"/>
+      <c r="AN26" s="65"/>
+      <c r="AO26" s="65"/>
+      <c r="AP26" s="65"/>
+      <c r="AQ26" s="65"/>
+      <c r="AR26" s="65"/>
+      <c r="AS26" s="65"/>
+      <c r="AT26" s="65"/>
+      <c r="AU26" s="65"/>
       <c r="AW26" s="4"/>
     </row>
     <row r="27" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6778,14 +6778,14 @@
       <c r="AK27" s="11"/>
       <c r="AL27" s="11"/>
       <c r="AM27" s="11"/>
-      <c r="AN27" s="56"/>
-      <c r="AO27" s="56"/>
-      <c r="AP27" s="56"/>
-      <c r="AQ27" s="56"/>
-      <c r="AR27" s="56"/>
-      <c r="AS27" s="56"/>
-      <c r="AT27" s="56"/>
-      <c r="AU27" s="56"/>
+      <c r="AN27" s="65"/>
+      <c r="AO27" s="65"/>
+      <c r="AP27" s="65"/>
+      <c r="AQ27" s="65"/>
+      <c r="AR27" s="65"/>
+      <c r="AS27" s="65"/>
+      <c r="AT27" s="65"/>
+      <c r="AU27" s="65"/>
       <c r="AW27" s="4"/>
     </row>
     <row r="28" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6930,111 +6930,111 @@
     </row>
     <row r="3" spans="2:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10"/>
-      <c r="C3" s="137" t="s">
+      <c r="C3" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="138"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="139"/>
-      <c r="H3" s="84" t="s">
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="104"/>
+      <c r="H3" s="134" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="85"/>
-      <c r="T3" s="85"/>
-      <c r="U3" s="86"/>
+      <c r="I3" s="135"/>
+      <c r="J3" s="135"/>
+      <c r="K3" s="135"/>
+      <c r="L3" s="135"/>
+      <c r="M3" s="135"/>
+      <c r="N3" s="135"/>
+      <c r="O3" s="135"/>
+      <c r="P3" s="135"/>
+      <c r="Q3" s="135"/>
+      <c r="R3" s="135"/>
+      <c r="S3" s="135"/>
+      <c r="T3" s="135"/>
+      <c r="U3" s="136"/>
       <c r="V3" s="11"/>
       <c r="W3" s="11"/>
-      <c r="X3" s="146" t="s">
+      <c r="X3" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="Y3" s="147"/>
-      <c r="Z3" s="147"/>
-      <c r="AA3" s="148"/>
+      <c r="Y3" s="112"/>
+      <c r="Z3" s="112"/>
+      <c r="AA3" s="113"/>
       <c r="AB3" s="11"/>
-      <c r="AD3" s="90" t="s">
+      <c r="AD3" s="140" t="s">
         <v>25</v>
       </c>
-      <c r="AE3" s="91"/>
-      <c r="AF3" s="91"/>
-      <c r="AG3" s="91"/>
-      <c r="AH3" s="91"/>
-      <c r="AI3" s="91"/>
-      <c r="AJ3" s="91"/>
-      <c r="AK3" s="91"/>
-      <c r="AL3" s="91"/>
-      <c r="AM3" s="91"/>
-      <c r="AN3" s="91"/>
-      <c r="AO3" s="91"/>
-      <c r="AP3" s="91"/>
-      <c r="AQ3" s="92"/>
-      <c r="AS3" s="137" t="s">
+      <c r="AE3" s="141"/>
+      <c r="AF3" s="141"/>
+      <c r="AG3" s="141"/>
+      <c r="AH3" s="141"/>
+      <c r="AI3" s="141"/>
+      <c r="AJ3" s="141"/>
+      <c r="AK3" s="141"/>
+      <c r="AL3" s="141"/>
+      <c r="AM3" s="141"/>
+      <c r="AN3" s="141"/>
+      <c r="AO3" s="141"/>
+      <c r="AP3" s="141"/>
+      <c r="AQ3" s="142"/>
+      <c r="AS3" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="AT3" s="138"/>
-      <c r="AU3" s="138"/>
-      <c r="AV3" s="139"/>
+      <c r="AT3" s="103"/>
+      <c r="AU3" s="103"/>
+      <c r="AV3" s="104"/>
       <c r="AW3" s="12"/>
     </row>
     <row r="4" spans="2:57" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
-      <c r="C4" s="140"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="142"/>
-      <c r="H4" s="87"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="88"/>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="89"/>
-      <c r="X4" s="149"/>
-      <c r="Y4" s="150"/>
-      <c r="Z4" s="150"/>
-      <c r="AA4" s="151"/>
-      <c r="AD4" s="93"/>
-      <c r="AE4" s="94"/>
-      <c r="AF4" s="94"/>
-      <c r="AG4" s="94"/>
-      <c r="AH4" s="94"/>
-      <c r="AI4" s="94"/>
-      <c r="AJ4" s="94"/>
-      <c r="AK4" s="94"/>
-      <c r="AL4" s="94"/>
-      <c r="AM4" s="94"/>
-      <c r="AN4" s="94"/>
-      <c r="AO4" s="94"/>
-      <c r="AP4" s="94"/>
-      <c r="AQ4" s="95"/>
-      <c r="AS4" s="140"/>
-      <c r="AT4" s="141"/>
-      <c r="AU4" s="141"/>
-      <c r="AV4" s="142"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="107"/>
+      <c r="H4" s="137"/>
+      <c r="I4" s="138"/>
+      <c r="J4" s="138"/>
+      <c r="K4" s="138"/>
+      <c r="L4" s="138"/>
+      <c r="M4" s="138"/>
+      <c r="N4" s="138"/>
+      <c r="O4" s="138"/>
+      <c r="P4" s="138"/>
+      <c r="Q4" s="138"/>
+      <c r="R4" s="138"/>
+      <c r="S4" s="138"/>
+      <c r="T4" s="138"/>
+      <c r="U4" s="139"/>
+      <c r="X4" s="114"/>
+      <c r="Y4" s="115"/>
+      <c r="Z4" s="115"/>
+      <c r="AA4" s="116"/>
+      <c r="AD4" s="143"/>
+      <c r="AE4" s="144"/>
+      <c r="AF4" s="144"/>
+      <c r="AG4" s="144"/>
+      <c r="AH4" s="144"/>
+      <c r="AI4" s="144"/>
+      <c r="AJ4" s="144"/>
+      <c r="AK4" s="144"/>
+      <c r="AL4" s="144"/>
+      <c r="AM4" s="144"/>
+      <c r="AN4" s="144"/>
+      <c r="AO4" s="144"/>
+      <c r="AP4" s="144"/>
+      <c r="AQ4" s="145"/>
+      <c r="AS4" s="105"/>
+      <c r="AT4" s="106"/>
+      <c r="AU4" s="106"/>
+      <c r="AV4" s="107"/>
       <c r="AW4" s="12"/>
     </row>
     <row r="5" spans="2:57" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
-      <c r="C5" s="140"/>
-      <c r="D5" s="141"/>
-      <c r="E5" s="141"/>
-      <c r="F5" s="142"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="107"/>
       <c r="L5" s="11"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
@@ -7042,10 +7042,10 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
-      <c r="X5" s="149"/>
-      <c r="Y5" s="150"/>
-      <c r="Z5" s="150"/>
-      <c r="AA5" s="151"/>
+      <c r="X5" s="114"/>
+      <c r="Y5" s="115"/>
+      <c r="Z5" s="115"/>
+      <c r="AA5" s="116"/>
       <c r="AF5" s="11"/>
       <c r="AG5" s="11"/>
       <c r="AH5" s="11"/>
@@ -7058,40 +7058,40 @@
       <c r="AO5" s="11"/>
       <c r="AP5" s="11"/>
       <c r="AQ5" s="11"/>
-      <c r="AS5" s="140"/>
-      <c r="AT5" s="141"/>
-      <c r="AU5" s="141"/>
-      <c r="AV5" s="142"/>
+      <c r="AS5" s="105"/>
+      <c r="AT5" s="106"/>
+      <c r="AU5" s="106"/>
+      <c r="AV5" s="107"/>
       <c r="AW5" s="12"/>
     </row>
     <row r="6" spans="2:57" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="10"/>
-      <c r="C6" s="140"/>
-      <c r="D6" s="141"/>
-      <c r="E6" s="141"/>
-      <c r="F6" s="142"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="106"/>
+      <c r="E6" s="106"/>
+      <c r="F6" s="107"/>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
-      <c r="I6" s="115" t="s">
+      <c r="I6" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="116"/>
+      <c r="J6" s="122"/>
       <c r="K6" s="11"/>
-      <c r="L6" s="115" t="s">
+      <c r="L6" s="121" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="116"/>
+      <c r="M6" s="122"/>
       <c r="N6" s="26"/>
-      <c r="O6" s="115" t="s">
+      <c r="O6" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="116"/>
+      <c r="P6" s="122"/>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
-      <c r="X6" s="152"/>
-      <c r="Y6" s="153"/>
-      <c r="Z6" s="153"/>
-      <c r="AA6" s="154"/>
+      <c r="X6" s="117"/>
+      <c r="Y6" s="118"/>
+      <c r="Z6" s="118"/>
+      <c r="AA6" s="119"/>
       <c r="AF6" s="11"/>
       <c r="AG6" s="11"/>
       <c r="AH6" s="11"/>
@@ -7104,28 +7104,28 @@
       <c r="AO6" s="11"/>
       <c r="AP6" s="11"/>
       <c r="AQ6" s="11"/>
-      <c r="AS6" s="140"/>
-      <c r="AT6" s="141"/>
-      <c r="AU6" s="141"/>
-      <c r="AV6" s="142"/>
+      <c r="AS6" s="105"/>
+      <c r="AT6" s="106"/>
+      <c r="AU6" s="106"/>
+      <c r="AV6" s="107"/>
       <c r="AW6" s="12"/>
     </row>
     <row r="7" spans="2:57" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10"/>
-      <c r="C7" s="143"/>
-      <c r="D7" s="144"/>
-      <c r="E7" s="144"/>
-      <c r="F7" s="145"/>
+      <c r="C7" s="108"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="110"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="117"/>
-      <c r="J7" s="118"/>
+      <c r="I7" s="123"/>
+      <c r="J7" s="124"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="117"/>
-      <c r="M7" s="118"/>
+      <c r="L7" s="123"/>
+      <c r="M7" s="124"/>
       <c r="N7" s="26"/>
-      <c r="O7" s="117"/>
-      <c r="P7" s="118"/>
+      <c r="O7" s="123"/>
+      <c r="P7" s="124"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
@@ -7152,10 +7152,10 @@
       <c r="AO7" s="20"/>
       <c r="AP7" s="20"/>
       <c r="AQ7" s="20"/>
-      <c r="AS7" s="143"/>
-      <c r="AT7" s="144"/>
-      <c r="AU7" s="144"/>
-      <c r="AV7" s="145"/>
+      <c r="AS7" s="108"/>
+      <c r="AT7" s="109"/>
+      <c r="AU7" s="109"/>
+      <c r="AV7" s="110"/>
       <c r="AW7" s="4"/>
     </row>
     <row r="8" spans="2:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7256,12 +7256,12 @@
       <c r="AV9" s="11"/>
       <c r="AW9" s="4"/>
       <c r="AZ9" s="49"/>
-      <c r="BA9" s="114" t="s">
+      <c r="BA9" s="120" t="s">
         <v>45</v>
       </c>
-      <c r="BB9" s="114"/>
-      <c r="BC9" s="114"/>
-      <c r="BD9" s="114"/>
+      <c r="BB9" s="120"/>
+      <c r="BC9" s="120"/>
+      <c r="BD9" s="120"/>
       <c r="BE9" s="4"/>
     </row>
     <row r="10" spans="2:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7297,10 +7297,10 @@
       <c r="AV10" s="11"/>
       <c r="AW10" s="45"/>
       <c r="AZ10" s="49"/>
-      <c r="BA10" s="114"/>
-      <c r="BB10" s="114"/>
-      <c r="BC10" s="114"/>
-      <c r="BD10" s="114"/>
+      <c r="BA10" s="120"/>
+      <c r="BB10" s="120"/>
+      <c r="BC10" s="120"/>
+      <c r="BD10" s="120"/>
       <c r="BE10" s="4"/>
     </row>
     <row r="11" spans="2:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -7338,10 +7338,10 @@
         <v>28</v>
       </c>
       <c r="AZ11" s="49"/>
-      <c r="BA11" s="114"/>
-      <c r="BB11" s="114"/>
-      <c r="BC11" s="114"/>
-      <c r="BD11" s="114"/>
+      <c r="BA11" s="120"/>
+      <c r="BB11" s="120"/>
+      <c r="BC11" s="120"/>
+      <c r="BD11" s="120"/>
       <c r="BE11" s="4"/>
     </row>
     <row r="12" spans="2:57" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7420,17 +7420,17 @@
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
-      <c r="U13" s="119" t="s">
+      <c r="U13" s="125" t="s">
         <v>32</v>
       </c>
-      <c r="V13" s="120"/>
-      <c r="W13" s="120"/>
-      <c r="X13" s="120"/>
-      <c r="Y13" s="120"/>
-      <c r="Z13" s="120"/>
-      <c r="AA13" s="120"/>
-      <c r="AB13" s="120"/>
-      <c r="AC13" s="121"/>
+      <c r="V13" s="126"/>
+      <c r="W13" s="126"/>
+      <c r="X13" s="126"/>
+      <c r="Y13" s="126"/>
+      <c r="Z13" s="126"/>
+      <c r="AA13" s="126"/>
+      <c r="AB13" s="126"/>
+      <c r="AC13" s="127"/>
       <c r="AD13" s="3"/>
       <c r="AE13" s="3"/>
       <c r="AF13" s="3"/>
@@ -7452,12 +7452,12 @@
       <c r="AV13" s="11"/>
       <c r="AW13" s="4"/>
       <c r="AZ13" s="49"/>
-      <c r="BA13" s="114" t="s">
+      <c r="BA13" s="120" t="s">
         <v>46</v>
       </c>
-      <c r="BB13" s="114"/>
-      <c r="BC13" s="114"/>
-      <c r="BD13" s="114"/>
+      <c r="BB13" s="120"/>
+      <c r="BC13" s="120"/>
+      <c r="BD13" s="120"/>
       <c r="BE13" s="4"/>
     </row>
     <row r="14" spans="2:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7480,15 +7480,15 @@
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
-      <c r="U14" s="122"/>
-      <c r="V14" s="123"/>
-      <c r="W14" s="123"/>
-      <c r="X14" s="123"/>
-      <c r="Y14" s="123"/>
-      <c r="Z14" s="123"/>
-      <c r="AA14" s="123"/>
-      <c r="AB14" s="123"/>
-      <c r="AC14" s="124"/>
+      <c r="U14" s="128"/>
+      <c r="V14" s="129"/>
+      <c r="W14" s="129"/>
+      <c r="X14" s="129"/>
+      <c r="Y14" s="129"/>
+      <c r="Z14" s="129"/>
+      <c r="AA14" s="129"/>
+      <c r="AB14" s="129"/>
+      <c r="AC14" s="130"/>
       <c r="AD14" s="3"/>
       <c r="AE14" s="3"/>
       <c r="AF14" s="3"/>
@@ -7510,10 +7510,10 @@
       <c r="AV14" s="11"/>
       <c r="AW14" s="4"/>
       <c r="AZ14" s="49"/>
-      <c r="BA14" s="114"/>
-      <c r="BB14" s="114"/>
-      <c r="BC14" s="114"/>
-      <c r="BD14" s="114"/>
+      <c r="BA14" s="120"/>
+      <c r="BB14" s="120"/>
+      <c r="BC14" s="120"/>
+      <c r="BD14" s="120"/>
       <c r="BE14" s="4"/>
     </row>
     <row r="15" spans="2:57" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7536,15 +7536,15 @@
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
-      <c r="U15" s="125"/>
-      <c r="V15" s="126"/>
-      <c r="W15" s="126"/>
-      <c r="X15" s="126"/>
-      <c r="Y15" s="126"/>
-      <c r="Z15" s="126"/>
-      <c r="AA15" s="126"/>
-      <c r="AB15" s="126"/>
-      <c r="AC15" s="127"/>
+      <c r="U15" s="131"/>
+      <c r="V15" s="132"/>
+      <c r="W15" s="132"/>
+      <c r="X15" s="132"/>
+      <c r="Y15" s="132"/>
+      <c r="Z15" s="132"/>
+      <c r="AA15" s="132"/>
+      <c r="AB15" s="132"/>
+      <c r="AC15" s="133"/>
       <c r="AD15" s="3"/>
       <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
@@ -7566,10 +7566,10 @@
       <c r="AV15" s="11"/>
       <c r="AW15" s="4"/>
       <c r="AZ15" s="49"/>
-      <c r="BA15" s="114"/>
-      <c r="BB15" s="114"/>
-      <c r="BC15" s="114"/>
-      <c r="BD15" s="114"/>
+      <c r="BA15" s="120"/>
+      <c r="BB15" s="120"/>
+      <c r="BC15" s="120"/>
+      <c r="BD15" s="120"/>
       <c r="BE15" s="4"/>
     </row>
     <row r="16" spans="2:57" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7670,12 +7670,12 @@
       <c r="AM17" s="11"/>
       <c r="AN17" s="11"/>
       <c r="AO17" s="11"/>
-      <c r="AP17" s="96" t="s">
+      <c r="AP17" s="146" t="s">
         <v>41</v>
       </c>
-      <c r="AQ17" s="97"/>
-      <c r="AR17" s="97"/>
-      <c r="AS17" s="98"/>
+      <c r="AQ17" s="147"/>
+      <c r="AR17" s="147"/>
+      <c r="AS17" s="148"/>
       <c r="AU17" s="11"/>
       <c r="AV17" s="11"/>
       <c r="AW17" s="4"/>
@@ -7723,10 +7723,10 @@
       <c r="AM18" s="11"/>
       <c r="AN18" s="11"/>
       <c r="AO18" s="11"/>
-      <c r="AP18" s="99"/>
-      <c r="AQ18" s="100"/>
-      <c r="AR18" s="100"/>
-      <c r="AS18" s="101"/>
+      <c r="AP18" s="149"/>
+      <c r="AQ18" s="150"/>
+      <c r="AR18" s="150"/>
+      <c r="AS18" s="151"/>
       <c r="AU18" s="11"/>
       <c r="AV18" s="11"/>
       <c r="AW18" s="4"/>
@@ -7771,10 +7771,10 @@
       <c r="AM19" s="11"/>
       <c r="AN19" s="11"/>
       <c r="AO19" s="11"/>
-      <c r="AP19" s="99"/>
-      <c r="AQ19" s="100"/>
-      <c r="AR19" s="100"/>
-      <c r="AS19" s="101"/>
+      <c r="AP19" s="149"/>
+      <c r="AQ19" s="150"/>
+      <c r="AR19" s="150"/>
+      <c r="AS19" s="151"/>
       <c r="AU19" s="11"/>
       <c r="AV19" s="11"/>
       <c r="AW19" s="4"/>
@@ -7820,10 +7820,10 @@
       <c r="AM20" s="3"/>
       <c r="AN20" s="23"/>
       <c r="AO20" s="23"/>
-      <c r="AP20" s="102"/>
-      <c r="AQ20" s="103"/>
-      <c r="AR20" s="103"/>
-      <c r="AS20" s="104"/>
+      <c r="AP20" s="152"/>
+      <c r="AQ20" s="153"/>
+      <c r="AR20" s="153"/>
+      <c r="AS20" s="154"/>
       <c r="AU20" s="23"/>
       <c r="AV20" s="23"/>
       <c r="AW20" s="4"/>
@@ -7914,21 +7914,21 @@
       <c r="AH22" s="3"/>
       <c r="AI22" s="19"/>
       <c r="AJ22" s="3"/>
-      <c r="AK22" s="96" t="s">
+      <c r="AK22" s="146" t="s">
         <v>40</v>
       </c>
-      <c r="AL22" s="97"/>
-      <c r="AM22" s="97"/>
-      <c r="AN22" s="98"/>
+      <c r="AL22" s="147"/>
+      <c r="AM22" s="147"/>
+      <c r="AN22" s="148"/>
       <c r="AO22" s="23"/>
-      <c r="AP22" s="105" t="s">
+      <c r="AP22" s="155" t="s">
         <v>24</v>
       </c>
-      <c r="AQ22" s="106"/>
-      <c r="AR22" s="106"/>
-      <c r="AS22" s="106"/>
-      <c r="AT22" s="106"/>
-      <c r="AU22" s="107"/>
+      <c r="AQ22" s="156"/>
+      <c r="AR22" s="156"/>
+      <c r="AS22" s="156"/>
+      <c r="AT22" s="156"/>
+      <c r="AU22" s="157"/>
       <c r="AV22" s="25"/>
       <c r="AW22" s="4"/>
     </row>
@@ -7968,17 +7968,17 @@
       <c r="AH23" s="3"/>
       <c r="AI23" s="11"/>
       <c r="AJ23" s="3"/>
-      <c r="AK23" s="99"/>
-      <c r="AL23" s="100"/>
-      <c r="AM23" s="100"/>
-      <c r="AN23" s="101"/>
+      <c r="AK23" s="149"/>
+      <c r="AL23" s="150"/>
+      <c r="AM23" s="150"/>
+      <c r="AN23" s="151"/>
       <c r="AO23" s="23"/>
-      <c r="AP23" s="108"/>
-      <c r="AQ23" s="109"/>
-      <c r="AR23" s="109"/>
-      <c r="AS23" s="109"/>
-      <c r="AT23" s="109"/>
-      <c r="AU23" s="110"/>
+      <c r="AP23" s="158"/>
+      <c r="AQ23" s="159"/>
+      <c r="AR23" s="159"/>
+      <c r="AS23" s="159"/>
+      <c r="AT23" s="159"/>
+      <c r="AU23" s="160"/>
       <c r="AV23" s="25"/>
       <c r="AW23" s="4"/>
     </row>
@@ -7989,56 +7989,56 @@
       <c r="T24" s="11"/>
       <c r="AI24" s="11"/>
       <c r="AJ24" s="11"/>
-      <c r="AK24" s="99"/>
-      <c r="AL24" s="100"/>
-      <c r="AM24" s="100"/>
-      <c r="AN24" s="101"/>
+      <c r="AK24" s="149"/>
+      <c r="AL24" s="150"/>
+      <c r="AM24" s="150"/>
+      <c r="AN24" s="151"/>
       <c r="AO24" s="23"/>
-      <c r="AP24" s="108"/>
-      <c r="AQ24" s="109"/>
-      <c r="AR24" s="109"/>
-      <c r="AS24" s="109"/>
-      <c r="AT24" s="109"/>
-      <c r="AU24" s="110"/>
+      <c r="AP24" s="158"/>
+      <c r="AQ24" s="159"/>
+      <c r="AR24" s="159"/>
+      <c r="AS24" s="159"/>
+      <c r="AT24" s="159"/>
+      <c r="AU24" s="160"/>
       <c r="AV24" s="22"/>
       <c r="AW24" s="4"/>
     </row>
     <row r="25" spans="2:49" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
-      <c r="C25" s="128" t="s">
+      <c r="C25" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="129"/>
-      <c r="E25" s="130"/>
-      <c r="G25" s="128" t="s">
+      <c r="D25" s="94"/>
+      <c r="E25" s="95"/>
+      <c r="G25" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="H25" s="129"/>
-      <c r="I25" s="130"/>
+      <c r="H25" s="94"/>
+      <c r="I25" s="95"/>
       <c r="AI25" s="11"/>
       <c r="AJ25" s="11"/>
-      <c r="AK25" s="102"/>
-      <c r="AL25" s="103"/>
-      <c r="AM25" s="103"/>
-      <c r="AN25" s="104"/>
+      <c r="AK25" s="152"/>
+      <c r="AL25" s="153"/>
+      <c r="AM25" s="153"/>
+      <c r="AN25" s="154"/>
       <c r="AO25" s="24"/>
-      <c r="AP25" s="108"/>
-      <c r="AQ25" s="109"/>
-      <c r="AR25" s="109"/>
-      <c r="AS25" s="109"/>
-      <c r="AT25" s="109"/>
-      <c r="AU25" s="110"/>
+      <c r="AP25" s="158"/>
+      <c r="AQ25" s="159"/>
+      <c r="AR25" s="159"/>
+      <c r="AS25" s="159"/>
+      <c r="AT25" s="159"/>
+      <c r="AU25" s="160"/>
       <c r="AV25" s="22"/>
       <c r="AW25" s="4"/>
     </row>
     <row r="26" spans="2:49" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
-      <c r="C26" s="131"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="133"/>
-      <c r="G26" s="131"/>
-      <c r="H26" s="132"/>
-      <c r="I26" s="133"/>
+      <c r="C26" s="96"/>
+      <c r="D26" s="97"/>
+      <c r="E26" s="98"/>
+      <c r="G26" s="96"/>
+      <c r="H26" s="97"/>
+      <c r="I26" s="98"/>
       <c r="AI26" s="11"/>
       <c r="AJ26" s="11"/>
       <c r="AK26" s="11"/>
@@ -8046,23 +8046,23 @@
       <c r="AM26" s="23"/>
       <c r="AN26" s="24"/>
       <c r="AO26" s="24"/>
-      <c r="AP26" s="108"/>
-      <c r="AQ26" s="109"/>
-      <c r="AR26" s="109"/>
-      <c r="AS26" s="109"/>
-      <c r="AT26" s="109"/>
-      <c r="AU26" s="110"/>
+      <c r="AP26" s="158"/>
+      <c r="AQ26" s="159"/>
+      <c r="AR26" s="159"/>
+      <c r="AS26" s="159"/>
+      <c r="AT26" s="159"/>
+      <c r="AU26" s="160"/>
       <c r="AV26" s="22"/>
       <c r="AW26" s="4"/>
     </row>
     <row r="27" spans="2:49" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="10"/>
-      <c r="C27" s="134"/>
-      <c r="D27" s="135"/>
-      <c r="E27" s="136"/>
-      <c r="G27" s="134"/>
-      <c r="H27" s="135"/>
-      <c r="I27" s="136"/>
+      <c r="C27" s="99"/>
+      <c r="D27" s="100"/>
+      <c r="E27" s="101"/>
+      <c r="G27" s="99"/>
+      <c r="H27" s="100"/>
+      <c r="I27" s="101"/>
       <c r="T27" s="11"/>
       <c r="AI27" s="11"/>
       <c r="AJ27" s="11"/>
@@ -8071,12 +8071,12 @@
       <c r="AM27" s="23"/>
       <c r="AN27" s="24"/>
       <c r="AO27" s="24"/>
-      <c r="AP27" s="111"/>
-      <c r="AQ27" s="112"/>
-      <c r="AR27" s="112"/>
-      <c r="AS27" s="112"/>
-      <c r="AT27" s="112"/>
-      <c r="AU27" s="113"/>
+      <c r="AP27" s="161"/>
+      <c r="AQ27" s="162"/>
+      <c r="AR27" s="162"/>
+      <c r="AS27" s="162"/>
+      <c r="AT27" s="162"/>
+      <c r="AU27" s="163"/>
       <c r="AV27" s="22"/>
       <c r="AW27" s="4"/>
     </row>
@@ -8134,17 +8134,17 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C25:E27"/>
-    <mergeCell ref="G25:I27"/>
-    <mergeCell ref="AS3:AV7"/>
-    <mergeCell ref="C3:F7"/>
-    <mergeCell ref="X3:AA6"/>
     <mergeCell ref="BA9:BD11"/>
     <mergeCell ref="BA13:BD15"/>
     <mergeCell ref="I6:J7"/>
     <mergeCell ref="L6:M7"/>
     <mergeCell ref="O6:P7"/>
     <mergeCell ref="U13:AC15"/>
+    <mergeCell ref="C25:E27"/>
+    <mergeCell ref="G25:I27"/>
+    <mergeCell ref="AS3:AV7"/>
+    <mergeCell ref="C3:F7"/>
+    <mergeCell ref="X3:AA6"/>
     <mergeCell ref="H3:U4"/>
     <mergeCell ref="AD3:AQ4"/>
     <mergeCell ref="AP17:AS20"/>
@@ -8194,18 +8194,18 @@
       <c r="R2" s="8"/>
       <c r="S2" s="8"/>
       <c r="T2" s="8"/>
-      <c r="U2" s="155" t="s">
+      <c r="U2" s="164" t="s">
         <v>34</v>
       </c>
-      <c r="V2" s="156"/>
-      <c r="W2" s="156"/>
-      <c r="X2" s="156"/>
-      <c r="Y2" s="156"/>
-      <c r="Z2" s="156"/>
-      <c r="AA2" s="156"/>
-      <c r="AB2" s="156"/>
-      <c r="AC2" s="156"/>
-      <c r="AD2" s="157"/>
+      <c r="V2" s="165"/>
+      <c r="W2" s="165"/>
+      <c r="X2" s="165"/>
+      <c r="Y2" s="165"/>
+      <c r="Z2" s="165"/>
+      <c r="AA2" s="165"/>
+      <c r="AB2" s="165"/>
+      <c r="AC2" s="165"/>
+      <c r="AD2" s="166"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="8"/>
       <c r="AG2" s="8"/>
@@ -8246,16 +8246,16 @@
       <c r="R3" s="29"/>
       <c r="S3" s="29"/>
       <c r="T3" s="29"/>
-      <c r="U3" s="158"/>
-      <c r="V3" s="159"/>
-      <c r="W3" s="159"/>
-      <c r="X3" s="159"/>
-      <c r="Y3" s="159"/>
-      <c r="Z3" s="159"/>
-      <c r="AA3" s="159"/>
-      <c r="AB3" s="159"/>
-      <c r="AC3" s="159"/>
-      <c r="AD3" s="160"/>
+      <c r="U3" s="167"/>
+      <c r="V3" s="168"/>
+      <c r="W3" s="168"/>
+      <c r="X3" s="168"/>
+      <c r="Y3" s="168"/>
+      <c r="Z3" s="168"/>
+      <c r="AA3" s="168"/>
+      <c r="AB3" s="168"/>
+      <c r="AC3" s="168"/>
+      <c r="AD3" s="169"/>
       <c r="AE3" s="3"/>
       <c r="AF3" s="29"/>
       <c r="AG3" s="29"/>
@@ -8281,19 +8281,19 @@
       <c r="C4" s="22"/>
       <c r="D4" s="31"/>
       <c r="E4" s="31"/>
-      <c r="F4" s="161" t="s">
+      <c r="F4" s="170" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="162"/>
-      <c r="H4" s="162"/>
-      <c r="I4" s="162"/>
-      <c r="J4" s="162"/>
-      <c r="K4" s="162"/>
-      <c r="L4" s="162"/>
-      <c r="M4" s="162"/>
-      <c r="N4" s="162"/>
-      <c r="O4" s="162"/>
-      <c r="P4" s="163"/>
+      <c r="G4" s="171"/>
+      <c r="H4" s="171"/>
+      <c r="I4" s="171"/>
+      <c r="J4" s="171"/>
+      <c r="K4" s="171"/>
+      <c r="L4" s="171"/>
+      <c r="M4" s="171"/>
+      <c r="N4" s="171"/>
+      <c r="O4" s="171"/>
+      <c r="P4" s="172"/>
       <c r="Q4" s="29"/>
       <c r="R4" s="29"/>
       <c r="S4" s="29"/>
@@ -8311,19 +8311,19 @@
       <c r="AE4" s="28"/>
       <c r="AF4" s="28"/>
       <c r="AG4" s="29"/>
-      <c r="AH4" s="161" t="s">
+      <c r="AH4" s="170" t="s">
         <v>35</v>
       </c>
-      <c r="AI4" s="162"/>
-      <c r="AJ4" s="162"/>
-      <c r="AK4" s="162"/>
-      <c r="AL4" s="162"/>
-      <c r="AM4" s="162"/>
-      <c r="AN4" s="162"/>
-      <c r="AO4" s="162"/>
-      <c r="AP4" s="162"/>
-      <c r="AQ4" s="162"/>
-      <c r="AR4" s="163"/>
+      <c r="AI4" s="171"/>
+      <c r="AJ4" s="171"/>
+      <c r="AK4" s="171"/>
+      <c r="AL4" s="171"/>
+      <c r="AM4" s="171"/>
+      <c r="AN4" s="171"/>
+      <c r="AO4" s="171"/>
+      <c r="AP4" s="171"/>
+      <c r="AQ4" s="171"/>
+      <c r="AR4" s="172"/>
       <c r="AS4" s="3"/>
       <c r="AT4" s="3"/>
       <c r="AU4" s="34"/>
@@ -8335,17 +8335,17 @@
       <c r="C5" s="22"/>
       <c r="D5" s="31"/>
       <c r="E5" s="31"/>
-      <c r="F5" s="164"/>
-      <c r="G5" s="165"/>
-      <c r="H5" s="165"/>
-      <c r="I5" s="165"/>
-      <c r="J5" s="165"/>
-      <c r="K5" s="165"/>
-      <c r="L5" s="165"/>
-      <c r="M5" s="165"/>
-      <c r="N5" s="165"/>
-      <c r="O5" s="165"/>
-      <c r="P5" s="166"/>
+      <c r="F5" s="173"/>
+      <c r="G5" s="174"/>
+      <c r="H5" s="174"/>
+      <c r="I5" s="174"/>
+      <c r="J5" s="174"/>
+      <c r="K5" s="174"/>
+      <c r="L5" s="174"/>
+      <c r="M5" s="174"/>
+      <c r="N5" s="174"/>
+      <c r="O5" s="174"/>
+      <c r="P5" s="175"/>
       <c r="Q5" s="23"/>
       <c r="R5" s="23"/>
       <c r="S5" s="22"/>
@@ -8363,17 +8363,17 @@
       <c r="AE5" s="22"/>
       <c r="AF5" s="23"/>
       <c r="AG5" s="23"/>
-      <c r="AH5" s="164"/>
-      <c r="AI5" s="165"/>
-      <c r="AJ5" s="165"/>
-      <c r="AK5" s="165"/>
-      <c r="AL5" s="165"/>
-      <c r="AM5" s="165"/>
-      <c r="AN5" s="165"/>
-      <c r="AO5" s="165"/>
-      <c r="AP5" s="165"/>
-      <c r="AQ5" s="165"/>
-      <c r="AR5" s="166"/>
+      <c r="AH5" s="173"/>
+      <c r="AI5" s="174"/>
+      <c r="AJ5" s="174"/>
+      <c r="AK5" s="174"/>
+      <c r="AL5" s="174"/>
+      <c r="AM5" s="174"/>
+      <c r="AN5" s="174"/>
+      <c r="AO5" s="174"/>
+      <c r="AP5" s="174"/>
+      <c r="AQ5" s="174"/>
+      <c r="AR5" s="175"/>
       <c r="AS5" s="3"/>
       <c r="AT5" s="3"/>
       <c r="AU5" s="23"/>
@@ -8434,23 +8434,23 @@
       <c r="B7" s="10"/>
       <c r="C7" s="22"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="167" t="s">
+      <c r="E7" s="176" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="168"/>
-      <c r="G7" s="168"/>
-      <c r="H7" s="168"/>
-      <c r="I7" s="168"/>
-      <c r="J7" s="168"/>
-      <c r="K7" s="168"/>
-      <c r="L7" s="168"/>
-      <c r="M7" s="168"/>
-      <c r="N7" s="168"/>
-      <c r="O7" s="168"/>
-      <c r="P7" s="168"/>
-      <c r="Q7" s="168"/>
-      <c r="R7" s="168"/>
-      <c r="S7" s="169"/>
+      <c r="F7" s="177"/>
+      <c r="G7" s="177"/>
+      <c r="H7" s="177"/>
+      <c r="I7" s="177"/>
+      <c r="J7" s="177"/>
+      <c r="K7" s="177"/>
+      <c r="L7" s="177"/>
+      <c r="M7" s="177"/>
+      <c r="N7" s="177"/>
+      <c r="O7" s="177"/>
+      <c r="P7" s="177"/>
+      <c r="Q7" s="177"/>
+      <c r="R7" s="177"/>
+      <c r="S7" s="178"/>
       <c r="T7" s="22"/>
       <c r="U7" s="22"/>
       <c r="V7" s="22"/>
@@ -8463,23 +8463,23 @@
       <c r="AC7" s="22"/>
       <c r="AD7" s="22"/>
       <c r="AE7" s="23"/>
-      <c r="AF7" s="167" t="s">
+      <c r="AF7" s="176" t="s">
         <v>37</v>
       </c>
-      <c r="AG7" s="168"/>
-      <c r="AH7" s="168"/>
-      <c r="AI7" s="168"/>
-      <c r="AJ7" s="168"/>
-      <c r="AK7" s="168"/>
-      <c r="AL7" s="168"/>
-      <c r="AM7" s="168"/>
-      <c r="AN7" s="168"/>
-      <c r="AO7" s="168"/>
-      <c r="AP7" s="168"/>
-      <c r="AQ7" s="168"/>
-      <c r="AR7" s="168"/>
-      <c r="AS7" s="168"/>
-      <c r="AT7" s="169"/>
+      <c r="AG7" s="177"/>
+      <c r="AH7" s="177"/>
+      <c r="AI7" s="177"/>
+      <c r="AJ7" s="177"/>
+      <c r="AK7" s="177"/>
+      <c r="AL7" s="177"/>
+      <c r="AM7" s="177"/>
+      <c r="AN7" s="177"/>
+      <c r="AO7" s="177"/>
+      <c r="AP7" s="177"/>
+      <c r="AQ7" s="177"/>
+      <c r="AR7" s="177"/>
+      <c r="AS7" s="177"/>
+      <c r="AT7" s="178"/>
       <c r="AU7" s="23"/>
       <c r="AV7" s="23"/>
       <c r="AW7" s="4"/>
@@ -8488,21 +8488,21 @@
       <c r="B8" s="10"/>
       <c r="C8" s="23"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="170"/>
-      <c r="F8" s="171"/>
-      <c r="G8" s="171"/>
-      <c r="H8" s="171"/>
-      <c r="I8" s="171"/>
-      <c r="J8" s="171"/>
-      <c r="K8" s="171"/>
-      <c r="L8" s="171"/>
-      <c r="M8" s="171"/>
-      <c r="N8" s="171"/>
-      <c r="O8" s="171"/>
-      <c r="P8" s="171"/>
-      <c r="Q8" s="171"/>
-      <c r="R8" s="171"/>
-      <c r="S8" s="172"/>
+      <c r="E8" s="179"/>
+      <c r="F8" s="180"/>
+      <c r="G8" s="180"/>
+      <c r="H8" s="180"/>
+      <c r="I8" s="180"/>
+      <c r="J8" s="180"/>
+      <c r="K8" s="180"/>
+      <c r="L8" s="180"/>
+      <c r="M8" s="180"/>
+      <c r="N8" s="180"/>
+      <c r="O8" s="180"/>
+      <c r="P8" s="180"/>
+      <c r="Q8" s="180"/>
+      <c r="R8" s="180"/>
+      <c r="S8" s="181"/>
       <c r="T8" s="22"/>
       <c r="U8" s="22"/>
       <c r="V8" s="22"/>
@@ -8515,21 +8515,21 @@
       <c r="AC8" s="22"/>
       <c r="AD8" s="22"/>
       <c r="AE8" s="22"/>
-      <c r="AF8" s="170"/>
-      <c r="AG8" s="171"/>
-      <c r="AH8" s="171"/>
-      <c r="AI8" s="171"/>
-      <c r="AJ8" s="171"/>
-      <c r="AK8" s="171"/>
-      <c r="AL8" s="171"/>
-      <c r="AM8" s="171"/>
-      <c r="AN8" s="171"/>
-      <c r="AO8" s="171"/>
-      <c r="AP8" s="171"/>
-      <c r="AQ8" s="171"/>
-      <c r="AR8" s="171"/>
-      <c r="AS8" s="171"/>
-      <c r="AT8" s="172"/>
+      <c r="AF8" s="179"/>
+      <c r="AG8" s="180"/>
+      <c r="AH8" s="180"/>
+      <c r="AI8" s="180"/>
+      <c r="AJ8" s="180"/>
+      <c r="AK8" s="180"/>
+      <c r="AL8" s="180"/>
+      <c r="AM8" s="180"/>
+      <c r="AN8" s="180"/>
+      <c r="AO8" s="180"/>
+      <c r="AP8" s="180"/>
+      <c r="AQ8" s="180"/>
+      <c r="AR8" s="180"/>
+      <c r="AS8" s="180"/>
+      <c r="AT8" s="181"/>
       <c r="AU8" s="23"/>
       <c r="AV8" s="23"/>
       <c r="AW8" s="4"/>
@@ -8538,21 +8538,21 @@
       <c r="B9" s="10"/>
       <c r="C9" s="23"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="170"/>
-      <c r="F9" s="171"/>
-      <c r="G9" s="171"/>
-      <c r="H9" s="171"/>
-      <c r="I9" s="171"/>
-      <c r="J9" s="171"/>
-      <c r="K9" s="171"/>
-      <c r="L9" s="171"/>
-      <c r="M9" s="171"/>
-      <c r="N9" s="171"/>
-      <c r="O9" s="171"/>
-      <c r="P9" s="171"/>
-      <c r="Q9" s="171"/>
-      <c r="R9" s="171"/>
-      <c r="S9" s="172"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="180"/>
+      <c r="G9" s="180"/>
+      <c r="H9" s="180"/>
+      <c r="I9" s="180"/>
+      <c r="J9" s="180"/>
+      <c r="K9" s="180"/>
+      <c r="L9" s="180"/>
+      <c r="M9" s="180"/>
+      <c r="N9" s="180"/>
+      <c r="O9" s="180"/>
+      <c r="P9" s="180"/>
+      <c r="Q9" s="180"/>
+      <c r="R9" s="180"/>
+      <c r="S9" s="181"/>
       <c r="T9" s="22"/>
       <c r="U9" s="22"/>
       <c r="V9" s="22"/>
@@ -8565,21 +8565,21 @@
       <c r="AC9" s="22"/>
       <c r="AD9" s="22"/>
       <c r="AE9" s="22"/>
-      <c r="AF9" s="170"/>
-      <c r="AG9" s="171"/>
-      <c r="AH9" s="171"/>
-      <c r="AI9" s="171"/>
-      <c r="AJ9" s="171"/>
-      <c r="AK9" s="171"/>
-      <c r="AL9" s="171"/>
-      <c r="AM9" s="171"/>
-      <c r="AN9" s="171"/>
-      <c r="AO9" s="171"/>
-      <c r="AP9" s="171"/>
-      <c r="AQ9" s="171"/>
-      <c r="AR9" s="171"/>
-      <c r="AS9" s="171"/>
-      <c r="AT9" s="172"/>
+      <c r="AF9" s="179"/>
+      <c r="AG9" s="180"/>
+      <c r="AH9" s="180"/>
+      <c r="AI9" s="180"/>
+      <c r="AJ9" s="180"/>
+      <c r="AK9" s="180"/>
+      <c r="AL9" s="180"/>
+      <c r="AM9" s="180"/>
+      <c r="AN9" s="180"/>
+      <c r="AO9" s="180"/>
+      <c r="AP9" s="180"/>
+      <c r="AQ9" s="180"/>
+      <c r="AR9" s="180"/>
+      <c r="AS9" s="180"/>
+      <c r="AT9" s="181"/>
       <c r="AU9" s="23"/>
       <c r="AV9" s="23"/>
       <c r="AW9" s="4"/>
@@ -8588,21 +8588,21 @@
       <c r="B10" s="10"/>
       <c r="C10" s="23"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="170"/>
-      <c r="F10" s="171"/>
-      <c r="G10" s="171"/>
-      <c r="H10" s="171"/>
-      <c r="I10" s="171"/>
-      <c r="J10" s="171"/>
-      <c r="K10" s="171"/>
-      <c r="L10" s="171"/>
-      <c r="M10" s="171"/>
-      <c r="N10" s="171"/>
-      <c r="O10" s="171"/>
-      <c r="P10" s="171"/>
-      <c r="Q10" s="171"/>
-      <c r="R10" s="171"/>
-      <c r="S10" s="172"/>
+      <c r="E10" s="179"/>
+      <c r="F10" s="180"/>
+      <c r="G10" s="180"/>
+      <c r="H10" s="180"/>
+      <c r="I10" s="180"/>
+      <c r="J10" s="180"/>
+      <c r="K10" s="180"/>
+      <c r="L10" s="180"/>
+      <c r="M10" s="180"/>
+      <c r="N10" s="180"/>
+      <c r="O10" s="180"/>
+      <c r="P10" s="180"/>
+      <c r="Q10" s="180"/>
+      <c r="R10" s="180"/>
+      <c r="S10" s="181"/>
       <c r="T10" s="22"/>
       <c r="U10" s="22"/>
       <c r="V10" s="22"/>
@@ -8615,21 +8615,21 @@
       <c r="AC10" s="22"/>
       <c r="AD10" s="22"/>
       <c r="AE10" s="22"/>
-      <c r="AF10" s="170"/>
-      <c r="AG10" s="171"/>
-      <c r="AH10" s="171"/>
-      <c r="AI10" s="171"/>
-      <c r="AJ10" s="171"/>
-      <c r="AK10" s="171"/>
-      <c r="AL10" s="171"/>
-      <c r="AM10" s="171"/>
-      <c r="AN10" s="171"/>
-      <c r="AO10" s="171"/>
-      <c r="AP10" s="171"/>
-      <c r="AQ10" s="171"/>
-      <c r="AR10" s="171"/>
-      <c r="AS10" s="171"/>
-      <c r="AT10" s="172"/>
+      <c r="AF10" s="179"/>
+      <c r="AG10" s="180"/>
+      <c r="AH10" s="180"/>
+      <c r="AI10" s="180"/>
+      <c r="AJ10" s="180"/>
+      <c r="AK10" s="180"/>
+      <c r="AL10" s="180"/>
+      <c r="AM10" s="180"/>
+      <c r="AN10" s="180"/>
+      <c r="AO10" s="180"/>
+      <c r="AP10" s="180"/>
+      <c r="AQ10" s="180"/>
+      <c r="AR10" s="180"/>
+      <c r="AS10" s="180"/>
+      <c r="AT10" s="181"/>
       <c r="AU10" s="22"/>
       <c r="AV10" s="23"/>
       <c r="AW10" s="4"/>
@@ -8638,21 +8638,21 @@
       <c r="B11" s="10"/>
       <c r="C11" s="23"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="170"/>
-      <c r="F11" s="171"/>
-      <c r="G11" s="171"/>
-      <c r="H11" s="171"/>
-      <c r="I11" s="171"/>
-      <c r="J11" s="171"/>
-      <c r="K11" s="171"/>
-      <c r="L11" s="171"/>
-      <c r="M11" s="171"/>
-      <c r="N11" s="171"/>
-      <c r="O11" s="171"/>
-      <c r="P11" s="171"/>
-      <c r="Q11" s="171"/>
-      <c r="R11" s="171"/>
-      <c r="S11" s="172"/>
+      <c r="E11" s="179"/>
+      <c r="F11" s="180"/>
+      <c r="G11" s="180"/>
+      <c r="H11" s="180"/>
+      <c r="I11" s="180"/>
+      <c r="J11" s="180"/>
+      <c r="K11" s="180"/>
+      <c r="L11" s="180"/>
+      <c r="M11" s="180"/>
+      <c r="N11" s="180"/>
+      <c r="O11" s="180"/>
+      <c r="P11" s="180"/>
+      <c r="Q11" s="180"/>
+      <c r="R11" s="180"/>
+      <c r="S11" s="181"/>
       <c r="T11" s="22"/>
       <c r="U11" s="22"/>
       <c r="V11" s="22"/>
@@ -8665,21 +8665,21 @@
       <c r="AC11" s="22"/>
       <c r="AD11" s="22"/>
       <c r="AE11" s="22"/>
-      <c r="AF11" s="170"/>
-      <c r="AG11" s="171"/>
-      <c r="AH11" s="171"/>
-      <c r="AI11" s="171"/>
-      <c r="AJ11" s="171"/>
-      <c r="AK11" s="171"/>
-      <c r="AL11" s="171"/>
-      <c r="AM11" s="171"/>
-      <c r="AN11" s="171"/>
-      <c r="AO11" s="171"/>
-      <c r="AP11" s="171"/>
-      <c r="AQ11" s="171"/>
-      <c r="AR11" s="171"/>
-      <c r="AS11" s="171"/>
-      <c r="AT11" s="172"/>
+      <c r="AF11" s="179"/>
+      <c r="AG11" s="180"/>
+      <c r="AH11" s="180"/>
+      <c r="AI11" s="180"/>
+      <c r="AJ11" s="180"/>
+      <c r="AK11" s="180"/>
+      <c r="AL11" s="180"/>
+      <c r="AM11" s="180"/>
+      <c r="AN11" s="180"/>
+      <c r="AO11" s="180"/>
+      <c r="AP11" s="180"/>
+      <c r="AQ11" s="180"/>
+      <c r="AR11" s="180"/>
+      <c r="AS11" s="180"/>
+      <c r="AT11" s="181"/>
       <c r="AU11" s="22"/>
       <c r="AV11" s="23"/>
       <c r="AW11" s="4"/>
@@ -8688,21 +8688,21 @@
       <c r="B12" s="10"/>
       <c r="C12" s="23"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="170"/>
-      <c r="F12" s="171"/>
-      <c r="G12" s="171"/>
-      <c r="H12" s="171"/>
-      <c r="I12" s="171"/>
-      <c r="J12" s="171"/>
-      <c r="K12" s="171"/>
-      <c r="L12" s="171"/>
-      <c r="M12" s="171"/>
-      <c r="N12" s="171"/>
-      <c r="O12" s="171"/>
-      <c r="P12" s="171"/>
-      <c r="Q12" s="171"/>
-      <c r="R12" s="171"/>
-      <c r="S12" s="172"/>
+      <c r="E12" s="179"/>
+      <c r="F12" s="180"/>
+      <c r="G12" s="180"/>
+      <c r="H12" s="180"/>
+      <c r="I12" s="180"/>
+      <c r="J12" s="180"/>
+      <c r="K12" s="180"/>
+      <c r="L12" s="180"/>
+      <c r="M12" s="180"/>
+      <c r="N12" s="180"/>
+      <c r="O12" s="180"/>
+      <c r="P12" s="180"/>
+      <c r="Q12" s="180"/>
+      <c r="R12" s="180"/>
+      <c r="S12" s="181"/>
       <c r="T12" s="22"/>
       <c r="U12" s="22"/>
       <c r="V12" s="22"/>
@@ -8715,21 +8715,21 @@
       <c r="AC12" s="22"/>
       <c r="AD12" s="22"/>
       <c r="AE12" s="22"/>
-      <c r="AF12" s="170"/>
-      <c r="AG12" s="171"/>
-      <c r="AH12" s="171"/>
-      <c r="AI12" s="171"/>
-      <c r="AJ12" s="171"/>
-      <c r="AK12" s="171"/>
-      <c r="AL12" s="171"/>
-      <c r="AM12" s="171"/>
-      <c r="AN12" s="171"/>
-      <c r="AO12" s="171"/>
-      <c r="AP12" s="171"/>
-      <c r="AQ12" s="171"/>
-      <c r="AR12" s="171"/>
-      <c r="AS12" s="171"/>
-      <c r="AT12" s="172"/>
+      <c r="AF12" s="179"/>
+      <c r="AG12" s="180"/>
+      <c r="AH12" s="180"/>
+      <c r="AI12" s="180"/>
+      <c r="AJ12" s="180"/>
+      <c r="AK12" s="180"/>
+      <c r="AL12" s="180"/>
+      <c r="AM12" s="180"/>
+      <c r="AN12" s="180"/>
+      <c r="AO12" s="180"/>
+      <c r="AP12" s="180"/>
+      <c r="AQ12" s="180"/>
+      <c r="AR12" s="180"/>
+      <c r="AS12" s="180"/>
+      <c r="AT12" s="181"/>
       <c r="AU12" s="23"/>
       <c r="AV12" s="23"/>
       <c r="AW12" s="4"/>
@@ -8738,21 +8738,21 @@
       <c r="B13" s="10"/>
       <c r="C13" s="23"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="170"/>
-      <c r="F13" s="171"/>
-      <c r="G13" s="171"/>
-      <c r="H13" s="171"/>
-      <c r="I13" s="171"/>
-      <c r="J13" s="171"/>
-      <c r="K13" s="171"/>
-      <c r="L13" s="171"/>
-      <c r="M13" s="171"/>
-      <c r="N13" s="171"/>
-      <c r="O13" s="171"/>
-      <c r="P13" s="171"/>
-      <c r="Q13" s="171"/>
-      <c r="R13" s="171"/>
-      <c r="S13" s="172"/>
+      <c r="E13" s="179"/>
+      <c r="F13" s="180"/>
+      <c r="G13" s="180"/>
+      <c r="H13" s="180"/>
+      <c r="I13" s="180"/>
+      <c r="J13" s="180"/>
+      <c r="K13" s="180"/>
+      <c r="L13" s="180"/>
+      <c r="M13" s="180"/>
+      <c r="N13" s="180"/>
+      <c r="O13" s="180"/>
+      <c r="P13" s="180"/>
+      <c r="Q13" s="180"/>
+      <c r="R13" s="180"/>
+      <c r="S13" s="181"/>
       <c r="T13" s="22"/>
       <c r="U13" s="36"/>
       <c r="V13" s="36"/>
@@ -8765,21 +8765,21 @@
       <c r="AC13" s="36"/>
       <c r="AD13" s="22"/>
       <c r="AE13" s="22"/>
-      <c r="AF13" s="170"/>
-      <c r="AG13" s="171"/>
-      <c r="AH13" s="171"/>
-      <c r="AI13" s="171"/>
-      <c r="AJ13" s="171"/>
-      <c r="AK13" s="171"/>
-      <c r="AL13" s="171"/>
-      <c r="AM13" s="171"/>
-      <c r="AN13" s="171"/>
-      <c r="AO13" s="171"/>
-      <c r="AP13" s="171"/>
-      <c r="AQ13" s="171"/>
-      <c r="AR13" s="171"/>
-      <c r="AS13" s="171"/>
-      <c r="AT13" s="172"/>
+      <c r="AF13" s="179"/>
+      <c r="AG13" s="180"/>
+      <c r="AH13" s="180"/>
+      <c r="AI13" s="180"/>
+      <c r="AJ13" s="180"/>
+      <c r="AK13" s="180"/>
+      <c r="AL13" s="180"/>
+      <c r="AM13" s="180"/>
+      <c r="AN13" s="180"/>
+      <c r="AO13" s="180"/>
+      <c r="AP13" s="180"/>
+      <c r="AQ13" s="180"/>
+      <c r="AR13" s="180"/>
+      <c r="AS13" s="180"/>
+      <c r="AT13" s="181"/>
       <c r="AU13" s="23"/>
       <c r="AV13" s="23"/>
       <c r="AW13" s="4"/>
@@ -8788,21 +8788,21 @@
       <c r="B14" s="10"/>
       <c r="C14" s="23"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="170"/>
-      <c r="F14" s="171"/>
-      <c r="G14" s="171"/>
-      <c r="H14" s="171"/>
-      <c r="I14" s="171"/>
-      <c r="J14" s="171"/>
-      <c r="K14" s="171"/>
-      <c r="L14" s="171"/>
-      <c r="M14" s="171"/>
-      <c r="N14" s="171"/>
-      <c r="O14" s="171"/>
-      <c r="P14" s="171"/>
-      <c r="Q14" s="171"/>
-      <c r="R14" s="171"/>
-      <c r="S14" s="172"/>
+      <c r="E14" s="179"/>
+      <c r="F14" s="180"/>
+      <c r="G14" s="180"/>
+      <c r="H14" s="180"/>
+      <c r="I14" s="180"/>
+      <c r="J14" s="180"/>
+      <c r="K14" s="180"/>
+      <c r="L14" s="180"/>
+      <c r="M14" s="180"/>
+      <c r="N14" s="180"/>
+      <c r="O14" s="180"/>
+      <c r="P14" s="180"/>
+      <c r="Q14" s="180"/>
+      <c r="R14" s="180"/>
+      <c r="S14" s="181"/>
       <c r="T14" s="22"/>
       <c r="U14" s="37"/>
       <c r="V14" s="37"/>
@@ -8815,21 +8815,21 @@
       <c r="AC14" s="39"/>
       <c r="AD14" s="22"/>
       <c r="AE14" s="22"/>
-      <c r="AF14" s="170"/>
-      <c r="AG14" s="171"/>
-      <c r="AH14" s="171"/>
-      <c r="AI14" s="171"/>
-      <c r="AJ14" s="171"/>
-      <c r="AK14" s="171"/>
-      <c r="AL14" s="171"/>
-      <c r="AM14" s="171"/>
-      <c r="AN14" s="171"/>
-      <c r="AO14" s="171"/>
-      <c r="AP14" s="171"/>
-      <c r="AQ14" s="171"/>
-      <c r="AR14" s="171"/>
-      <c r="AS14" s="171"/>
-      <c r="AT14" s="172"/>
+      <c r="AF14" s="179"/>
+      <c r="AG14" s="180"/>
+      <c r="AH14" s="180"/>
+      <c r="AI14" s="180"/>
+      <c r="AJ14" s="180"/>
+      <c r="AK14" s="180"/>
+      <c r="AL14" s="180"/>
+      <c r="AM14" s="180"/>
+      <c r="AN14" s="180"/>
+      <c r="AO14" s="180"/>
+      <c r="AP14" s="180"/>
+      <c r="AQ14" s="180"/>
+      <c r="AR14" s="180"/>
+      <c r="AS14" s="180"/>
+      <c r="AT14" s="181"/>
       <c r="AU14" s="23"/>
       <c r="AV14" s="23"/>
       <c r="AW14" s="4"/>
@@ -8838,21 +8838,21 @@
       <c r="B15" s="10"/>
       <c r="C15" s="23"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="170"/>
-      <c r="F15" s="171"/>
-      <c r="G15" s="171"/>
-      <c r="H15" s="171"/>
-      <c r="I15" s="171"/>
-      <c r="J15" s="171"/>
-      <c r="K15" s="171"/>
-      <c r="L15" s="171"/>
-      <c r="M15" s="171"/>
-      <c r="N15" s="171"/>
-      <c r="O15" s="171"/>
-      <c r="P15" s="171"/>
-      <c r="Q15" s="171"/>
-      <c r="R15" s="171"/>
-      <c r="S15" s="172"/>
+      <c r="E15" s="179"/>
+      <c r="F15" s="180"/>
+      <c r="G15" s="180"/>
+      <c r="H15" s="180"/>
+      <c r="I15" s="180"/>
+      <c r="J15" s="180"/>
+      <c r="K15" s="180"/>
+      <c r="L15" s="180"/>
+      <c r="M15" s="180"/>
+      <c r="N15" s="180"/>
+      <c r="O15" s="180"/>
+      <c r="P15" s="180"/>
+      <c r="Q15" s="180"/>
+      <c r="R15" s="180"/>
+      <c r="S15" s="181"/>
       <c r="T15" s="22"/>
       <c r="U15" s="37"/>
       <c r="V15" s="37"/>
@@ -8865,21 +8865,21 @@
       <c r="AC15" s="39"/>
       <c r="AD15" s="22"/>
       <c r="AE15" s="22"/>
-      <c r="AF15" s="170"/>
-      <c r="AG15" s="171"/>
-      <c r="AH15" s="171"/>
-      <c r="AI15" s="171"/>
-      <c r="AJ15" s="171"/>
-      <c r="AK15" s="171"/>
-      <c r="AL15" s="171"/>
-      <c r="AM15" s="171"/>
-      <c r="AN15" s="171"/>
-      <c r="AO15" s="171"/>
-      <c r="AP15" s="171"/>
-      <c r="AQ15" s="171"/>
-      <c r="AR15" s="171"/>
-      <c r="AS15" s="171"/>
-      <c r="AT15" s="172"/>
+      <c r="AF15" s="179"/>
+      <c r="AG15" s="180"/>
+      <c r="AH15" s="180"/>
+      <c r="AI15" s="180"/>
+      <c r="AJ15" s="180"/>
+      <c r="AK15" s="180"/>
+      <c r="AL15" s="180"/>
+      <c r="AM15" s="180"/>
+      <c r="AN15" s="180"/>
+      <c r="AO15" s="180"/>
+      <c r="AP15" s="180"/>
+      <c r="AQ15" s="180"/>
+      <c r="AR15" s="180"/>
+      <c r="AS15" s="180"/>
+      <c r="AT15" s="181"/>
       <c r="AU15" s="23"/>
       <c r="AV15" s="23"/>
       <c r="AW15" s="4"/>
@@ -8888,21 +8888,21 @@
       <c r="B16" s="10"/>
       <c r="C16" s="23"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="170"/>
-      <c r="F16" s="171"/>
-      <c r="G16" s="171"/>
-      <c r="H16" s="171"/>
-      <c r="I16" s="171"/>
-      <c r="J16" s="171"/>
-      <c r="K16" s="171"/>
-      <c r="L16" s="171"/>
-      <c r="M16" s="171"/>
-      <c r="N16" s="171"/>
-      <c r="O16" s="171"/>
-      <c r="P16" s="171"/>
-      <c r="Q16" s="171"/>
-      <c r="R16" s="171"/>
-      <c r="S16" s="172"/>
+      <c r="E16" s="179"/>
+      <c r="F16" s="180"/>
+      <c r="G16" s="180"/>
+      <c r="H16" s="180"/>
+      <c r="I16" s="180"/>
+      <c r="J16" s="180"/>
+      <c r="K16" s="180"/>
+      <c r="L16" s="180"/>
+      <c r="M16" s="180"/>
+      <c r="N16" s="180"/>
+      <c r="O16" s="180"/>
+      <c r="P16" s="180"/>
+      <c r="Q16" s="180"/>
+      <c r="R16" s="180"/>
+      <c r="S16" s="181"/>
       <c r="T16" s="22"/>
       <c r="U16" s="22"/>
       <c r="V16" s="22"/>
@@ -8915,21 +8915,21 @@
       <c r="AC16" s="22"/>
       <c r="AD16" s="22"/>
       <c r="AE16" s="22"/>
-      <c r="AF16" s="170"/>
-      <c r="AG16" s="171"/>
-      <c r="AH16" s="171"/>
-      <c r="AI16" s="171"/>
-      <c r="AJ16" s="171"/>
-      <c r="AK16" s="171"/>
-      <c r="AL16" s="171"/>
-      <c r="AM16" s="171"/>
-      <c r="AN16" s="171"/>
-      <c r="AO16" s="171"/>
-      <c r="AP16" s="171"/>
-      <c r="AQ16" s="171"/>
-      <c r="AR16" s="171"/>
-      <c r="AS16" s="171"/>
-      <c r="AT16" s="172"/>
+      <c r="AF16" s="179"/>
+      <c r="AG16" s="180"/>
+      <c r="AH16" s="180"/>
+      <c r="AI16" s="180"/>
+      <c r="AJ16" s="180"/>
+      <c r="AK16" s="180"/>
+      <c r="AL16" s="180"/>
+      <c r="AM16" s="180"/>
+      <c r="AN16" s="180"/>
+      <c r="AO16" s="180"/>
+      <c r="AP16" s="180"/>
+      <c r="AQ16" s="180"/>
+      <c r="AR16" s="180"/>
+      <c r="AS16" s="180"/>
+      <c r="AT16" s="181"/>
       <c r="AU16" s="23"/>
       <c r="AV16" s="23"/>
       <c r="AW16" s="4"/>
@@ -8938,21 +8938,21 @@
       <c r="B17" s="10"/>
       <c r="C17" s="23"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="170"/>
-      <c r="F17" s="171"/>
-      <c r="G17" s="171"/>
-      <c r="H17" s="171"/>
-      <c r="I17" s="171"/>
-      <c r="J17" s="171"/>
-      <c r="K17" s="171"/>
-      <c r="L17" s="171"/>
-      <c r="M17" s="171"/>
-      <c r="N17" s="171"/>
-      <c r="O17" s="171"/>
-      <c r="P17" s="171"/>
-      <c r="Q17" s="171"/>
-      <c r="R17" s="171"/>
-      <c r="S17" s="172"/>
+      <c r="E17" s="179"/>
+      <c r="F17" s="180"/>
+      <c r="G17" s="180"/>
+      <c r="H17" s="180"/>
+      <c r="I17" s="180"/>
+      <c r="J17" s="180"/>
+      <c r="K17" s="180"/>
+      <c r="L17" s="180"/>
+      <c r="M17" s="180"/>
+      <c r="N17" s="180"/>
+      <c r="O17" s="180"/>
+      <c r="P17" s="180"/>
+      <c r="Q17" s="180"/>
+      <c r="R17" s="180"/>
+      <c r="S17" s="181"/>
       <c r="T17" s="22"/>
       <c r="U17" s="22"/>
       <c r="V17" s="22"/>
@@ -8965,21 +8965,21 @@
       <c r="AC17" s="22"/>
       <c r="AD17" s="22"/>
       <c r="AE17" s="22"/>
-      <c r="AF17" s="170"/>
-      <c r="AG17" s="171"/>
-      <c r="AH17" s="171"/>
-      <c r="AI17" s="171"/>
-      <c r="AJ17" s="171"/>
-      <c r="AK17" s="171"/>
-      <c r="AL17" s="171"/>
-      <c r="AM17" s="171"/>
-      <c r="AN17" s="171"/>
-      <c r="AO17" s="171"/>
-      <c r="AP17" s="171"/>
-      <c r="AQ17" s="171"/>
-      <c r="AR17" s="171"/>
-      <c r="AS17" s="171"/>
-      <c r="AT17" s="172"/>
+      <c r="AF17" s="179"/>
+      <c r="AG17" s="180"/>
+      <c r="AH17" s="180"/>
+      <c r="AI17" s="180"/>
+      <c r="AJ17" s="180"/>
+      <c r="AK17" s="180"/>
+      <c r="AL17" s="180"/>
+      <c r="AM17" s="180"/>
+      <c r="AN17" s="180"/>
+      <c r="AO17" s="180"/>
+      <c r="AP17" s="180"/>
+      <c r="AQ17" s="180"/>
+      <c r="AR17" s="180"/>
+      <c r="AS17" s="180"/>
+      <c r="AT17" s="181"/>
       <c r="AU17" s="23"/>
       <c r="AV17" s="23"/>
       <c r="AW17" s="4"/>
@@ -8988,21 +8988,21 @@
       <c r="B18" s="10"/>
       <c r="C18" s="23"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="170"/>
-      <c r="F18" s="171"/>
-      <c r="G18" s="171"/>
-      <c r="H18" s="171"/>
-      <c r="I18" s="171"/>
-      <c r="J18" s="171"/>
-      <c r="K18" s="171"/>
-      <c r="L18" s="171"/>
-      <c r="M18" s="171"/>
-      <c r="N18" s="171"/>
-      <c r="O18" s="171"/>
-      <c r="P18" s="171"/>
-      <c r="Q18" s="171"/>
-      <c r="R18" s="171"/>
-      <c r="S18" s="172"/>
+      <c r="E18" s="179"/>
+      <c r="F18" s="180"/>
+      <c r="G18" s="180"/>
+      <c r="H18" s="180"/>
+      <c r="I18" s="180"/>
+      <c r="J18" s="180"/>
+      <c r="K18" s="180"/>
+      <c r="L18" s="180"/>
+      <c r="M18" s="180"/>
+      <c r="N18" s="180"/>
+      <c r="O18" s="180"/>
+      <c r="P18" s="180"/>
+      <c r="Q18" s="180"/>
+      <c r="R18" s="180"/>
+      <c r="S18" s="181"/>
       <c r="T18" s="22"/>
       <c r="U18" s="22"/>
       <c r="V18" s="22"/>
@@ -9015,21 +9015,21 @@
       <c r="AC18" s="22"/>
       <c r="AD18" s="22"/>
       <c r="AE18" s="22"/>
-      <c r="AF18" s="170"/>
-      <c r="AG18" s="171"/>
-      <c r="AH18" s="171"/>
-      <c r="AI18" s="171"/>
-      <c r="AJ18" s="171"/>
-      <c r="AK18" s="171"/>
-      <c r="AL18" s="171"/>
-      <c r="AM18" s="171"/>
-      <c r="AN18" s="171"/>
-      <c r="AO18" s="171"/>
-      <c r="AP18" s="171"/>
-      <c r="AQ18" s="171"/>
-      <c r="AR18" s="171"/>
-      <c r="AS18" s="171"/>
-      <c r="AT18" s="172"/>
+      <c r="AF18" s="179"/>
+      <c r="AG18" s="180"/>
+      <c r="AH18" s="180"/>
+      <c r="AI18" s="180"/>
+      <c r="AJ18" s="180"/>
+      <c r="AK18" s="180"/>
+      <c r="AL18" s="180"/>
+      <c r="AM18" s="180"/>
+      <c r="AN18" s="180"/>
+      <c r="AO18" s="180"/>
+      <c r="AP18" s="180"/>
+      <c r="AQ18" s="180"/>
+      <c r="AR18" s="180"/>
+      <c r="AS18" s="180"/>
+      <c r="AT18" s="181"/>
       <c r="AU18" s="23"/>
       <c r="AV18" s="23"/>
       <c r="AW18" s="4"/>
@@ -9038,21 +9038,21 @@
       <c r="B19" s="10"/>
       <c r="C19" s="23"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="170"/>
-      <c r="F19" s="171"/>
-      <c r="G19" s="171"/>
-      <c r="H19" s="171"/>
-      <c r="I19" s="171"/>
-      <c r="J19" s="171"/>
-      <c r="K19" s="171"/>
-      <c r="L19" s="171"/>
-      <c r="M19" s="171"/>
-      <c r="N19" s="171"/>
-      <c r="O19" s="171"/>
-      <c r="P19" s="171"/>
-      <c r="Q19" s="171"/>
-      <c r="R19" s="171"/>
-      <c r="S19" s="172"/>
+      <c r="E19" s="179"/>
+      <c r="F19" s="180"/>
+      <c r="G19" s="180"/>
+      <c r="H19" s="180"/>
+      <c r="I19" s="180"/>
+      <c r="J19" s="180"/>
+      <c r="K19" s="180"/>
+      <c r="L19" s="180"/>
+      <c r="M19" s="180"/>
+      <c r="N19" s="180"/>
+      <c r="O19" s="180"/>
+      <c r="P19" s="180"/>
+      <c r="Q19" s="180"/>
+      <c r="R19" s="180"/>
+      <c r="S19" s="181"/>
       <c r="T19" s="22"/>
       <c r="U19" s="22"/>
       <c r="V19" s="22"/>
@@ -9065,21 +9065,21 @@
       <c r="AC19" s="22"/>
       <c r="AD19" s="22"/>
       <c r="AE19" s="22"/>
-      <c r="AF19" s="170"/>
-      <c r="AG19" s="171"/>
-      <c r="AH19" s="171"/>
-      <c r="AI19" s="171"/>
-      <c r="AJ19" s="171"/>
-      <c r="AK19" s="171"/>
-      <c r="AL19" s="171"/>
-      <c r="AM19" s="171"/>
-      <c r="AN19" s="171"/>
-      <c r="AO19" s="171"/>
-      <c r="AP19" s="171"/>
-      <c r="AQ19" s="171"/>
-      <c r="AR19" s="171"/>
-      <c r="AS19" s="171"/>
-      <c r="AT19" s="172"/>
+      <c r="AF19" s="179"/>
+      <c r="AG19" s="180"/>
+      <c r="AH19" s="180"/>
+      <c r="AI19" s="180"/>
+      <c r="AJ19" s="180"/>
+      <c r="AK19" s="180"/>
+      <c r="AL19" s="180"/>
+      <c r="AM19" s="180"/>
+      <c r="AN19" s="180"/>
+      <c r="AO19" s="180"/>
+      <c r="AP19" s="180"/>
+      <c r="AQ19" s="180"/>
+      <c r="AR19" s="180"/>
+      <c r="AS19" s="180"/>
+      <c r="AT19" s="181"/>
       <c r="AU19" s="23"/>
       <c r="AV19" s="23"/>
       <c r="AW19" s="4"/>
@@ -9088,21 +9088,21 @@
       <c r="B20" s="10"/>
       <c r="C20" s="23"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="170"/>
-      <c r="F20" s="171"/>
-      <c r="G20" s="171"/>
-      <c r="H20" s="171"/>
-      <c r="I20" s="171"/>
-      <c r="J20" s="171"/>
-      <c r="K20" s="171"/>
-      <c r="L20" s="171"/>
-      <c r="M20" s="171"/>
-      <c r="N20" s="171"/>
-      <c r="O20" s="171"/>
-      <c r="P20" s="171"/>
-      <c r="Q20" s="171"/>
-      <c r="R20" s="171"/>
-      <c r="S20" s="172"/>
+      <c r="E20" s="179"/>
+      <c r="F20" s="180"/>
+      <c r="G20" s="180"/>
+      <c r="H20" s="180"/>
+      <c r="I20" s="180"/>
+      <c r="J20" s="180"/>
+      <c r="K20" s="180"/>
+      <c r="L20" s="180"/>
+      <c r="M20" s="180"/>
+      <c r="N20" s="180"/>
+      <c r="O20" s="180"/>
+      <c r="P20" s="180"/>
+      <c r="Q20" s="180"/>
+      <c r="R20" s="180"/>
+      <c r="S20" s="181"/>
       <c r="T20" s="22"/>
       <c r="U20" s="22"/>
       <c r="V20" s="22"/>
@@ -9115,21 +9115,21 @@
       <c r="AC20" s="22"/>
       <c r="AD20" s="22"/>
       <c r="AE20" s="22"/>
-      <c r="AF20" s="170"/>
-      <c r="AG20" s="171"/>
-      <c r="AH20" s="171"/>
-      <c r="AI20" s="171"/>
-      <c r="AJ20" s="171"/>
-      <c r="AK20" s="171"/>
-      <c r="AL20" s="171"/>
-      <c r="AM20" s="171"/>
-      <c r="AN20" s="171"/>
-      <c r="AO20" s="171"/>
-      <c r="AP20" s="171"/>
-      <c r="AQ20" s="171"/>
-      <c r="AR20" s="171"/>
-      <c r="AS20" s="171"/>
-      <c r="AT20" s="172"/>
+      <c r="AF20" s="179"/>
+      <c r="AG20" s="180"/>
+      <c r="AH20" s="180"/>
+      <c r="AI20" s="180"/>
+      <c r="AJ20" s="180"/>
+      <c r="AK20" s="180"/>
+      <c r="AL20" s="180"/>
+      <c r="AM20" s="180"/>
+      <c r="AN20" s="180"/>
+      <c r="AO20" s="180"/>
+      <c r="AP20" s="180"/>
+      <c r="AQ20" s="180"/>
+      <c r="AR20" s="180"/>
+      <c r="AS20" s="180"/>
+      <c r="AT20" s="181"/>
       <c r="AU20" s="23"/>
       <c r="AV20" s="23"/>
       <c r="AW20" s="4"/>
@@ -9138,21 +9138,21 @@
       <c r="B21" s="10"/>
       <c r="C21" s="23"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="170"/>
-      <c r="F21" s="171"/>
-      <c r="G21" s="171"/>
-      <c r="H21" s="171"/>
-      <c r="I21" s="171"/>
-      <c r="J21" s="171"/>
-      <c r="K21" s="171"/>
-      <c r="L21" s="171"/>
-      <c r="M21" s="171"/>
-      <c r="N21" s="171"/>
-      <c r="O21" s="171"/>
-      <c r="P21" s="171"/>
-      <c r="Q21" s="171"/>
-      <c r="R21" s="171"/>
-      <c r="S21" s="172"/>
+      <c r="E21" s="179"/>
+      <c r="F21" s="180"/>
+      <c r="G21" s="180"/>
+      <c r="H21" s="180"/>
+      <c r="I21" s="180"/>
+      <c r="J21" s="180"/>
+      <c r="K21" s="180"/>
+      <c r="L21" s="180"/>
+      <c r="M21" s="180"/>
+      <c r="N21" s="180"/>
+      <c r="O21" s="180"/>
+      <c r="P21" s="180"/>
+      <c r="Q21" s="180"/>
+      <c r="R21" s="180"/>
+      <c r="S21" s="181"/>
       <c r="T21" s="40"/>
       <c r="U21" s="22"/>
       <c r="V21" s="22"/>
@@ -9165,21 +9165,21 @@
       <c r="AC21" s="22"/>
       <c r="AD21" s="22"/>
       <c r="AE21" s="22"/>
-      <c r="AF21" s="170"/>
-      <c r="AG21" s="171"/>
-      <c r="AH21" s="171"/>
-      <c r="AI21" s="171"/>
-      <c r="AJ21" s="171"/>
-      <c r="AK21" s="171"/>
-      <c r="AL21" s="171"/>
-      <c r="AM21" s="171"/>
-      <c r="AN21" s="171"/>
-      <c r="AO21" s="171"/>
-      <c r="AP21" s="171"/>
-      <c r="AQ21" s="171"/>
-      <c r="AR21" s="171"/>
-      <c r="AS21" s="171"/>
-      <c r="AT21" s="172"/>
+      <c r="AF21" s="179"/>
+      <c r="AG21" s="180"/>
+      <c r="AH21" s="180"/>
+      <c r="AI21" s="180"/>
+      <c r="AJ21" s="180"/>
+      <c r="AK21" s="180"/>
+      <c r="AL21" s="180"/>
+      <c r="AM21" s="180"/>
+      <c r="AN21" s="180"/>
+      <c r="AO21" s="180"/>
+      <c r="AP21" s="180"/>
+      <c r="AQ21" s="180"/>
+      <c r="AR21" s="180"/>
+      <c r="AS21" s="180"/>
+      <c r="AT21" s="181"/>
       <c r="AU21" s="22"/>
       <c r="AV21" s="22"/>
       <c r="AW21" s="4"/>
@@ -9188,21 +9188,21 @@
       <c r="B22" s="10"/>
       <c r="C22" s="23"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="170"/>
-      <c r="F22" s="171"/>
-      <c r="G22" s="171"/>
-      <c r="H22" s="171"/>
-      <c r="I22" s="171"/>
-      <c r="J22" s="171"/>
-      <c r="K22" s="171"/>
-      <c r="L22" s="171"/>
-      <c r="M22" s="171"/>
-      <c r="N22" s="171"/>
-      <c r="O22" s="171"/>
-      <c r="P22" s="171"/>
-      <c r="Q22" s="171"/>
-      <c r="R22" s="171"/>
-      <c r="S22" s="172"/>
+      <c r="E22" s="179"/>
+      <c r="F22" s="180"/>
+      <c r="G22" s="180"/>
+      <c r="H22" s="180"/>
+      <c r="I22" s="180"/>
+      <c r="J22" s="180"/>
+      <c r="K22" s="180"/>
+      <c r="L22" s="180"/>
+      <c r="M22" s="180"/>
+      <c r="N22" s="180"/>
+      <c r="O22" s="180"/>
+      <c r="P22" s="180"/>
+      <c r="Q22" s="180"/>
+      <c r="R22" s="180"/>
+      <c r="S22" s="181"/>
       <c r="T22" s="40"/>
       <c r="U22" s="22"/>
       <c r="V22" s="22"/>
@@ -9215,21 +9215,21 @@
       <c r="AC22" s="22"/>
       <c r="AD22" s="22"/>
       <c r="AE22" s="22"/>
-      <c r="AF22" s="170"/>
-      <c r="AG22" s="171"/>
-      <c r="AH22" s="171"/>
-      <c r="AI22" s="171"/>
-      <c r="AJ22" s="171"/>
-      <c r="AK22" s="171"/>
-      <c r="AL22" s="171"/>
-      <c r="AM22" s="171"/>
-      <c r="AN22" s="171"/>
-      <c r="AO22" s="171"/>
-      <c r="AP22" s="171"/>
-      <c r="AQ22" s="171"/>
-      <c r="AR22" s="171"/>
-      <c r="AS22" s="171"/>
-      <c r="AT22" s="172"/>
+      <c r="AF22" s="179"/>
+      <c r="AG22" s="180"/>
+      <c r="AH22" s="180"/>
+      <c r="AI22" s="180"/>
+      <c r="AJ22" s="180"/>
+      <c r="AK22" s="180"/>
+      <c r="AL22" s="180"/>
+      <c r="AM22" s="180"/>
+      <c r="AN22" s="180"/>
+      <c r="AO22" s="180"/>
+      <c r="AP22" s="180"/>
+      <c r="AQ22" s="180"/>
+      <c r="AR22" s="180"/>
+      <c r="AS22" s="180"/>
+      <c r="AT22" s="181"/>
       <c r="AU22" s="24"/>
       <c r="AV22" s="22"/>
       <c r="AW22" s="4"/>
@@ -9238,21 +9238,21 @@
       <c r="B23" s="10"/>
       <c r="C23" s="23"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="170"/>
-      <c r="F23" s="171"/>
-      <c r="G23" s="171"/>
-      <c r="H23" s="171"/>
-      <c r="I23" s="171"/>
-      <c r="J23" s="171"/>
-      <c r="K23" s="171"/>
-      <c r="L23" s="171"/>
-      <c r="M23" s="171"/>
-      <c r="N23" s="171"/>
-      <c r="O23" s="171"/>
-      <c r="P23" s="171"/>
-      <c r="Q23" s="171"/>
-      <c r="R23" s="171"/>
-      <c r="S23" s="172"/>
+      <c r="E23" s="179"/>
+      <c r="F23" s="180"/>
+      <c r="G23" s="180"/>
+      <c r="H23" s="180"/>
+      <c r="I23" s="180"/>
+      <c r="J23" s="180"/>
+      <c r="K23" s="180"/>
+      <c r="L23" s="180"/>
+      <c r="M23" s="180"/>
+      <c r="N23" s="180"/>
+      <c r="O23" s="180"/>
+      <c r="P23" s="180"/>
+      <c r="Q23" s="180"/>
+      <c r="R23" s="180"/>
+      <c r="S23" s="181"/>
       <c r="T23" s="23"/>
       <c r="U23" s="22"/>
       <c r="V23" s="22"/>
@@ -9265,21 +9265,21 @@
       <c r="AC23" s="22"/>
       <c r="AD23" s="22"/>
       <c r="AE23" s="22"/>
-      <c r="AF23" s="170"/>
-      <c r="AG23" s="171"/>
-      <c r="AH23" s="171"/>
-      <c r="AI23" s="171"/>
-      <c r="AJ23" s="171"/>
-      <c r="AK23" s="171"/>
-      <c r="AL23" s="171"/>
-      <c r="AM23" s="171"/>
-      <c r="AN23" s="171"/>
-      <c r="AO23" s="171"/>
-      <c r="AP23" s="171"/>
-      <c r="AQ23" s="171"/>
-      <c r="AR23" s="171"/>
-      <c r="AS23" s="171"/>
-      <c r="AT23" s="172"/>
+      <c r="AF23" s="179"/>
+      <c r="AG23" s="180"/>
+      <c r="AH23" s="180"/>
+      <c r="AI23" s="180"/>
+      <c r="AJ23" s="180"/>
+      <c r="AK23" s="180"/>
+      <c r="AL23" s="180"/>
+      <c r="AM23" s="180"/>
+      <c r="AN23" s="180"/>
+      <c r="AO23" s="180"/>
+      <c r="AP23" s="180"/>
+      <c r="AQ23" s="180"/>
+      <c r="AR23" s="180"/>
+      <c r="AS23" s="180"/>
+      <c r="AT23" s="181"/>
       <c r="AU23" s="24"/>
       <c r="AV23" s="22"/>
       <c r="AW23" s="4"/>
@@ -9288,21 +9288,21 @@
       <c r="B24" s="10"/>
       <c r="C24" s="23"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="173"/>
-      <c r="F24" s="174"/>
-      <c r="G24" s="174"/>
-      <c r="H24" s="174"/>
-      <c r="I24" s="174"/>
-      <c r="J24" s="174"/>
-      <c r="K24" s="174"/>
-      <c r="L24" s="174"/>
-      <c r="M24" s="174"/>
-      <c r="N24" s="174"/>
-      <c r="O24" s="174"/>
-      <c r="P24" s="174"/>
-      <c r="Q24" s="174"/>
-      <c r="R24" s="174"/>
-      <c r="S24" s="175"/>
+      <c r="E24" s="182"/>
+      <c r="F24" s="183"/>
+      <c r="G24" s="183"/>
+      <c r="H24" s="183"/>
+      <c r="I24" s="183"/>
+      <c r="J24" s="183"/>
+      <c r="K24" s="183"/>
+      <c r="L24" s="183"/>
+      <c r="M24" s="183"/>
+      <c r="N24" s="183"/>
+      <c r="O24" s="183"/>
+      <c r="P24" s="183"/>
+      <c r="Q24" s="183"/>
+      <c r="R24" s="183"/>
+      <c r="S24" s="184"/>
       <c r="T24" s="23"/>
       <c r="U24" s="22"/>
       <c r="V24" s="22"/>
@@ -9315,21 +9315,21 @@
       <c r="AC24" s="22"/>
       <c r="AD24" s="22"/>
       <c r="AE24" s="22"/>
-      <c r="AF24" s="173"/>
-      <c r="AG24" s="174"/>
-      <c r="AH24" s="174"/>
-      <c r="AI24" s="174"/>
-      <c r="AJ24" s="174"/>
-      <c r="AK24" s="174"/>
-      <c r="AL24" s="174"/>
-      <c r="AM24" s="174"/>
-      <c r="AN24" s="174"/>
-      <c r="AO24" s="174"/>
-      <c r="AP24" s="174"/>
-      <c r="AQ24" s="174"/>
-      <c r="AR24" s="174"/>
-      <c r="AS24" s="174"/>
-      <c r="AT24" s="175"/>
+      <c r="AF24" s="182"/>
+      <c r="AG24" s="183"/>
+      <c r="AH24" s="183"/>
+      <c r="AI24" s="183"/>
+      <c r="AJ24" s="183"/>
+      <c r="AK24" s="183"/>
+      <c r="AL24" s="183"/>
+      <c r="AM24" s="183"/>
+      <c r="AN24" s="183"/>
+      <c r="AO24" s="183"/>
+      <c r="AP24" s="183"/>
+      <c r="AQ24" s="183"/>
+      <c r="AR24" s="183"/>
+      <c r="AS24" s="183"/>
+      <c r="AT24" s="184"/>
       <c r="AU24" s="24"/>
       <c r="AV24" s="22"/>
       <c r="AW24" s="4"/>
@@ -9427,13 +9427,13 @@
       <c r="AO26" s="24"/>
       <c r="AP26" s="24"/>
       <c r="AQ26" s="24"/>
-      <c r="AR26" s="56" t="s">
+      <c r="AR26" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="AS26" s="56"/>
-      <c r="AT26" s="56"/>
-      <c r="AU26" s="56"/>
-      <c r="AV26" s="56"/>
+      <c r="AS26" s="65"/>
+      <c r="AT26" s="65"/>
+      <c r="AU26" s="65"/>
+      <c r="AV26" s="65"/>
       <c r="AW26" s="4"/>
     </row>
     <row r="27" spans="2:49" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9479,11 +9479,11 @@
       <c r="AO27" s="24"/>
       <c r="AP27" s="24"/>
       <c r="AQ27" s="24"/>
-      <c r="AR27" s="56"/>
-      <c r="AS27" s="56"/>
-      <c r="AT27" s="56"/>
-      <c r="AU27" s="56"/>
-      <c r="AV27" s="56"/>
+      <c r="AR27" s="65"/>
+      <c r="AS27" s="65"/>
+      <c r="AT27" s="65"/>
+      <c r="AU27" s="65"/>
+      <c r="AV27" s="65"/>
       <c r="AW27" s="4"/>
     </row>
     <row r="28" spans="2:49" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update Camera, Lobby Layout, Login process
</commit_message>
<xml_diff>
--- a/References/Layout.xlsx
+++ b/References/Layout.xlsx
@@ -772,7 +772,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -887,6 +887,42 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -912,42 +948,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -998,6 +998,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1079,48 +1121,6 @@
     <xf numFmtId="20" fontId="16" fillId="7" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1272,6 +1272,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4297,17 +4312,17 @@
     <row r="2" spans="1:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="72" t="s">
+      <c r="D2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -4366,18 +4381,18 @@
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
-      <c r="U3" s="66" t="s">
+      <c r="U3" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="V3" s="67"/>
-      <c r="W3" s="67"/>
-      <c r="X3" s="67"/>
-      <c r="Y3" s="67"/>
-      <c r="Z3" s="67"/>
-      <c r="AA3" s="67"/>
-      <c r="AB3" s="67"/>
-      <c r="AC3" s="67"/>
-      <c r="AD3" s="68"/>
+      <c r="V3" s="57"/>
+      <c r="W3" s="57"/>
+      <c r="X3" s="57"/>
+      <c r="Y3" s="57"/>
+      <c r="Z3" s="57"/>
+      <c r="AA3" s="57"/>
+      <c r="AB3" s="57"/>
+      <c r="AC3" s="57"/>
+      <c r="AD3" s="58"/>
       <c r="AE3" s="11"/>
       <c r="AF3" s="11"/>
       <c r="AG3" s="11"/>
@@ -4395,11 +4410,11 @@
       <c r="AQ3" s="3"/>
       <c r="AR3" s="11"/>
       <c r="AS3" s="11"/>
-      <c r="AT3" s="73" t="s">
+      <c r="AT3" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="AU3" s="73"/>
-      <c r="AV3" s="73"/>
+      <c r="AU3" s="64"/>
+      <c r="AV3" s="64"/>
       <c r="AW3" s="12"/>
     </row>
     <row r="4" spans="1:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4424,16 +4439,16 @@
       <c r="R4" s="11"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
-      <c r="U4" s="69"/>
-      <c r="V4" s="70"/>
-      <c r="W4" s="70"/>
-      <c r="X4" s="70"/>
-      <c r="Y4" s="70"/>
-      <c r="Z4" s="70"/>
-      <c r="AA4" s="70"/>
-      <c r="AB4" s="70"/>
-      <c r="AC4" s="70"/>
-      <c r="AD4" s="71"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="60"/>
+      <c r="W4" s="60"/>
+      <c r="X4" s="60"/>
+      <c r="Y4" s="60"/>
+      <c r="Z4" s="60"/>
+      <c r="AA4" s="60"/>
+      <c r="AB4" s="60"/>
+      <c r="AC4" s="60"/>
+      <c r="AD4" s="61"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="11"/>
       <c r="AG4" s="11"/>
@@ -4451,9 +4466,9 @@
       <c r="AQ4" s="3"/>
       <c r="AR4" s="11"/>
       <c r="AS4" s="11"/>
-      <c r="AT4" s="73"/>
-      <c r="AU4" s="73"/>
-      <c r="AV4" s="73"/>
+      <c r="AT4" s="64"/>
+      <c r="AU4" s="64"/>
+      <c r="AV4" s="64"/>
       <c r="AW4" s="12"/>
     </row>
     <row r="5" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4501,9 +4516,9 @@
       <c r="AQ5" s="11"/>
       <c r="AR5" s="11"/>
       <c r="AS5" s="11"/>
-      <c r="AT5" s="73"/>
-      <c r="AU5" s="73"/>
-      <c r="AV5" s="73"/>
+      <c r="AT5" s="64"/>
+      <c r="AU5" s="64"/>
+      <c r="AV5" s="64"/>
       <c r="AW5" s="12"/>
     </row>
     <row r="6" spans="1:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4594,18 +4609,18 @@
       <c r="AJ7" s="9"/>
       <c r="AK7" s="11"/>
       <c r="AL7" s="11"/>
-      <c r="AM7" s="74" t="s">
+      <c r="AM7" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="AN7" s="75"/>
-      <c r="AO7" s="75"/>
-      <c r="AP7" s="75"/>
-      <c r="AQ7" s="75"/>
-      <c r="AR7" s="75"/>
-      <c r="AS7" s="75"/>
-      <c r="AT7" s="75"/>
-      <c r="AU7" s="75"/>
-      <c r="AV7" s="76"/>
+      <c r="AN7" s="66"/>
+      <c r="AO7" s="66"/>
+      <c r="AP7" s="66"/>
+      <c r="AQ7" s="66"/>
+      <c r="AR7" s="66"/>
+      <c r="AS7" s="66"/>
+      <c r="AT7" s="66"/>
+      <c r="AU7" s="66"/>
+      <c r="AV7" s="67"/>
       <c r="AW7" s="4"/>
     </row>
     <row r="8" spans="1:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4661,38 +4676,38 @@
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="17"/>
-      <c r="F9" s="56" t="s">
+      <c r="F9" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="57"/>
-      <c r="L9" s="57"/>
-      <c r="M9" s="57"/>
-      <c r="N9" s="57"/>
-      <c r="O9" s="57"/>
-      <c r="P9" s="57"/>
-      <c r="Q9" s="58"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="69"/>
+      <c r="N9" s="69"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="69"/>
+      <c r="Q9" s="70"/>
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
       <c r="T9" s="17"/>
       <c r="U9" s="17"/>
-      <c r="V9" s="56" t="s">
+      <c r="V9" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="W9" s="57"/>
-      <c r="X9" s="57"/>
-      <c r="Y9" s="57"/>
-      <c r="Z9" s="57"/>
-      <c r="AA9" s="57"/>
-      <c r="AB9" s="57"/>
-      <c r="AC9" s="57"/>
-      <c r="AD9" s="57"/>
-      <c r="AE9" s="57"/>
-      <c r="AF9" s="57"/>
-      <c r="AG9" s="58"/>
+      <c r="W9" s="69"/>
+      <c r="X9" s="69"/>
+      <c r="Y9" s="69"/>
+      <c r="Z9" s="69"/>
+      <c r="AA9" s="69"/>
+      <c r="AB9" s="69"/>
+      <c r="AC9" s="69"/>
+      <c r="AD9" s="69"/>
+      <c r="AE9" s="69"/>
+      <c r="AF9" s="69"/>
+      <c r="AG9" s="70"/>
       <c r="AH9" s="19"/>
       <c r="AI9" s="19"/>
       <c r="AJ9" s="4"/>
@@ -4714,34 +4729,34 @@
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="17"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="61"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="72"/>
+      <c r="N10" s="72"/>
+      <c r="O10" s="72"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="73"/>
       <c r="R10" s="17"/>
       <c r="S10" s="17"/>
       <c r="T10" s="17"/>
       <c r="U10" s="17"/>
-      <c r="V10" s="59"/>
-      <c r="W10" s="60"/>
-      <c r="X10" s="60"/>
-      <c r="Y10" s="60"/>
-      <c r="Z10" s="60"/>
-      <c r="AA10" s="60"/>
-      <c r="AB10" s="60"/>
-      <c r="AC10" s="60"/>
-      <c r="AD10" s="60"/>
-      <c r="AE10" s="60"/>
-      <c r="AF10" s="60"/>
-      <c r="AG10" s="61"/>
+      <c r="V10" s="71"/>
+      <c r="W10" s="72"/>
+      <c r="X10" s="72"/>
+      <c r="Y10" s="72"/>
+      <c r="Z10" s="72"/>
+      <c r="AA10" s="72"/>
+      <c r="AB10" s="72"/>
+      <c r="AC10" s="72"/>
+      <c r="AD10" s="72"/>
+      <c r="AE10" s="72"/>
+      <c r="AF10" s="72"/>
+      <c r="AG10" s="73"/>
       <c r="AH10" s="19"/>
       <c r="AI10" s="19"/>
       <c r="AJ10" s="4"/>
@@ -4762,30 +4777,30 @@
     <row r="11" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="60"/>
-      <c r="O11" s="60"/>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="61"/>
-      <c r="V11" s="59"/>
-      <c r="W11" s="60"/>
-      <c r="X11" s="60"/>
-      <c r="Y11" s="60"/>
-      <c r="Z11" s="60"/>
-      <c r="AA11" s="60"/>
-      <c r="AB11" s="60"/>
-      <c r="AC11" s="60"/>
-      <c r="AD11" s="60"/>
-      <c r="AE11" s="60"/>
-      <c r="AF11" s="60"/>
-      <c r="AG11" s="61"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="72"/>
+      <c r="M11" s="72"/>
+      <c r="N11" s="72"/>
+      <c r="O11" s="72"/>
+      <c r="P11" s="72"/>
+      <c r="Q11" s="73"/>
+      <c r="V11" s="71"/>
+      <c r="W11" s="72"/>
+      <c r="X11" s="72"/>
+      <c r="Y11" s="72"/>
+      <c r="Z11" s="72"/>
+      <c r="AA11" s="72"/>
+      <c r="AB11" s="72"/>
+      <c r="AC11" s="72"/>
+      <c r="AD11" s="72"/>
+      <c r="AE11" s="72"/>
+      <c r="AF11" s="72"/>
+      <c r="AG11" s="73"/>
       <c r="AH11" s="11"/>
       <c r="AI11" s="11"/>
       <c r="AJ11" s="4"/>
@@ -4807,30 +4822,30 @@
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="17"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="60"/>
-      <c r="O12" s="60"/>
-      <c r="P12" s="60"/>
-      <c r="Q12" s="61"/>
-      <c r="V12" s="59"/>
-      <c r="W12" s="60"/>
-      <c r="X12" s="60"/>
-      <c r="Y12" s="60"/>
-      <c r="Z12" s="60"/>
-      <c r="AA12" s="60"/>
-      <c r="AB12" s="60"/>
-      <c r="AC12" s="60"/>
-      <c r="AD12" s="60"/>
-      <c r="AE12" s="60"/>
-      <c r="AF12" s="60"/>
-      <c r="AG12" s="61"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="72"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="72"/>
+      <c r="N12" s="72"/>
+      <c r="O12" s="72"/>
+      <c r="P12" s="72"/>
+      <c r="Q12" s="73"/>
+      <c r="V12" s="71"/>
+      <c r="W12" s="72"/>
+      <c r="X12" s="72"/>
+      <c r="Y12" s="72"/>
+      <c r="Z12" s="72"/>
+      <c r="AA12" s="72"/>
+      <c r="AB12" s="72"/>
+      <c r="AC12" s="72"/>
+      <c r="AD12" s="72"/>
+      <c r="AE12" s="72"/>
+      <c r="AF12" s="72"/>
+      <c r="AG12" s="73"/>
       <c r="AH12" s="19"/>
       <c r="AI12" s="19"/>
       <c r="AJ12" s="4"/>
@@ -4852,30 +4867,30 @@
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="17"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="63"/>
-      <c r="L13" s="63"/>
-      <c r="M13" s="63"/>
-      <c r="N13" s="63"/>
-      <c r="O13" s="63"/>
-      <c r="P13" s="63"/>
-      <c r="Q13" s="64"/>
-      <c r="V13" s="62"/>
-      <c r="W13" s="63"/>
-      <c r="X13" s="63"/>
-      <c r="Y13" s="63"/>
-      <c r="Z13" s="63"/>
-      <c r="AA13" s="63"/>
-      <c r="AB13" s="63"/>
-      <c r="AC13" s="63"/>
-      <c r="AD13" s="63"/>
-      <c r="AE13" s="63"/>
-      <c r="AF13" s="63"/>
-      <c r="AG13" s="64"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="75"/>
+      <c r="M13" s="75"/>
+      <c r="N13" s="75"/>
+      <c r="O13" s="75"/>
+      <c r="P13" s="75"/>
+      <c r="Q13" s="76"/>
+      <c r="V13" s="74"/>
+      <c r="W13" s="75"/>
+      <c r="X13" s="75"/>
+      <c r="Y13" s="75"/>
+      <c r="Z13" s="75"/>
+      <c r="AA13" s="75"/>
+      <c r="AB13" s="75"/>
+      <c r="AC13" s="75"/>
+      <c r="AD13" s="75"/>
+      <c r="AE13" s="75"/>
+      <c r="AF13" s="75"/>
+      <c r="AG13" s="76"/>
       <c r="AH13" s="19"/>
       <c r="AI13" s="19"/>
       <c r="AJ13" s="4"/>
@@ -4973,34 +4988,34 @@
       <c r="C16" s="10"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="56" t="s">
+      <c r="F16" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="57"/>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="58"/>
-      <c r="V16" s="56" t="s">
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="69"/>
+      <c r="M16" s="69"/>
+      <c r="N16" s="69"/>
+      <c r="O16" s="69"/>
+      <c r="P16" s="69"/>
+      <c r="Q16" s="70"/>
+      <c r="V16" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="W16" s="57"/>
-      <c r="X16" s="57"/>
-      <c r="Y16" s="57"/>
-      <c r="Z16" s="57"/>
-      <c r="AA16" s="57"/>
-      <c r="AB16" s="57"/>
-      <c r="AC16" s="57"/>
-      <c r="AD16" s="57"/>
-      <c r="AE16" s="57"/>
-      <c r="AF16" s="57"/>
-      <c r="AG16" s="58"/>
+      <c r="W16" s="69"/>
+      <c r="X16" s="69"/>
+      <c r="Y16" s="69"/>
+      <c r="Z16" s="69"/>
+      <c r="AA16" s="69"/>
+      <c r="AB16" s="69"/>
+      <c r="AC16" s="69"/>
+      <c r="AD16" s="69"/>
+      <c r="AE16" s="69"/>
+      <c r="AF16" s="69"/>
+      <c r="AG16" s="70"/>
       <c r="AH16" s="19"/>
       <c r="AI16" s="19"/>
       <c r="AJ16" s="4"/>
@@ -5023,33 +5038,33 @@
       <c r="C17" s="10"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="60"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="60"/>
-      <c r="M17" s="60"/>
-      <c r="N17" s="60"/>
-      <c r="O17" s="60"/>
-      <c r="P17" s="60"/>
-      <c r="Q17" s="61"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="72"/>
+      <c r="J17" s="72"/>
+      <c r="K17" s="72"/>
+      <c r="L17" s="72"/>
+      <c r="M17" s="72"/>
+      <c r="N17" s="72"/>
+      <c r="O17" s="72"/>
+      <c r="P17" s="72"/>
+      <c r="Q17" s="73"/>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
-      <c r="V17" s="59"/>
-      <c r="W17" s="60"/>
-      <c r="X17" s="60"/>
-      <c r="Y17" s="60"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="60"/>
-      <c r="AB17" s="60"/>
-      <c r="AC17" s="60"/>
-      <c r="AD17" s="60"/>
-      <c r="AE17" s="60"/>
-      <c r="AF17" s="60"/>
-      <c r="AG17" s="61"/>
+      <c r="V17" s="71"/>
+      <c r="W17" s="72"/>
+      <c r="X17" s="72"/>
+      <c r="Y17" s="72"/>
+      <c r="Z17" s="72"/>
+      <c r="AA17" s="72"/>
+      <c r="AB17" s="72"/>
+      <c r="AC17" s="72"/>
+      <c r="AD17" s="72"/>
+      <c r="AE17" s="72"/>
+      <c r="AF17" s="72"/>
+      <c r="AG17" s="73"/>
       <c r="AH17" s="19"/>
       <c r="AI17" s="19"/>
       <c r="AJ17" s="4"/>
@@ -5071,33 +5086,33 @@
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="3"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="60"/>
-      <c r="O18" s="60"/>
-      <c r="P18" s="60"/>
-      <c r="Q18" s="61"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72"/>
+      <c r="L18" s="72"/>
+      <c r="M18" s="72"/>
+      <c r="N18" s="72"/>
+      <c r="O18" s="72"/>
+      <c r="P18" s="72"/>
+      <c r="Q18" s="73"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
-      <c r="V18" s="59"/>
-      <c r="W18" s="60"/>
-      <c r="X18" s="60"/>
-      <c r="Y18" s="60"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="60"/>
-      <c r="AB18" s="60"/>
-      <c r="AC18" s="60"/>
-      <c r="AD18" s="60"/>
-      <c r="AE18" s="60"/>
-      <c r="AF18" s="60"/>
-      <c r="AG18" s="61"/>
+      <c r="V18" s="71"/>
+      <c r="W18" s="72"/>
+      <c r="X18" s="72"/>
+      <c r="Y18" s="72"/>
+      <c r="Z18" s="72"/>
+      <c r="AA18" s="72"/>
+      <c r="AB18" s="72"/>
+      <c r="AC18" s="72"/>
+      <c r="AD18" s="72"/>
+      <c r="AE18" s="72"/>
+      <c r="AF18" s="72"/>
+      <c r="AG18" s="73"/>
       <c r="AH18" s="19"/>
       <c r="AI18" s="19"/>
       <c r="AJ18" s="4"/>
@@ -5119,33 +5134,33 @@
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="3"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="60"/>
-      <c r="M19" s="60"/>
-      <c r="N19" s="60"/>
-      <c r="O19" s="60"/>
-      <c r="P19" s="60"/>
-      <c r="Q19" s="61"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="72"/>
+      <c r="L19" s="72"/>
+      <c r="M19" s="72"/>
+      <c r="N19" s="72"/>
+      <c r="O19" s="72"/>
+      <c r="P19" s="72"/>
+      <c r="Q19" s="73"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
-      <c r="V19" s="59"/>
-      <c r="W19" s="60"/>
-      <c r="X19" s="60"/>
-      <c r="Y19" s="60"/>
-      <c r="Z19" s="60"/>
-      <c r="AA19" s="60"/>
-      <c r="AB19" s="60"/>
-      <c r="AC19" s="60"/>
-      <c r="AD19" s="60"/>
-      <c r="AE19" s="60"/>
-      <c r="AF19" s="60"/>
-      <c r="AG19" s="61"/>
+      <c r="V19" s="71"/>
+      <c r="W19" s="72"/>
+      <c r="X19" s="72"/>
+      <c r="Y19" s="72"/>
+      <c r="Z19" s="72"/>
+      <c r="AA19" s="72"/>
+      <c r="AB19" s="72"/>
+      <c r="AC19" s="72"/>
+      <c r="AD19" s="72"/>
+      <c r="AE19" s="72"/>
+      <c r="AF19" s="72"/>
+      <c r="AG19" s="73"/>
       <c r="AH19" s="11"/>
       <c r="AI19" s="11"/>
       <c r="AJ19" s="4"/>
@@ -5167,33 +5182,33 @@
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="3"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="63"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="63"/>
-      <c r="K20" s="63"/>
-      <c r="L20" s="63"/>
-      <c r="M20" s="63"/>
-      <c r="N20" s="63"/>
-      <c r="O20" s="63"/>
-      <c r="P20" s="63"/>
-      <c r="Q20" s="64"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="75"/>
+      <c r="J20" s="75"/>
+      <c r="K20" s="75"/>
+      <c r="L20" s="75"/>
+      <c r="M20" s="75"/>
+      <c r="N20" s="75"/>
+      <c r="O20" s="75"/>
+      <c r="P20" s="75"/>
+      <c r="Q20" s="76"/>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
-      <c r="V20" s="62"/>
-      <c r="W20" s="63"/>
-      <c r="X20" s="63"/>
-      <c r="Y20" s="63"/>
-      <c r="Z20" s="63"/>
-      <c r="AA20" s="63"/>
-      <c r="AB20" s="63"/>
-      <c r="AC20" s="63"/>
-      <c r="AD20" s="63"/>
-      <c r="AE20" s="63"/>
-      <c r="AF20" s="63"/>
-      <c r="AG20" s="64"/>
+      <c r="V20" s="74"/>
+      <c r="W20" s="75"/>
+      <c r="X20" s="75"/>
+      <c r="Y20" s="75"/>
+      <c r="Z20" s="75"/>
+      <c r="AA20" s="75"/>
+      <c r="AB20" s="75"/>
+      <c r="AC20" s="75"/>
+      <c r="AD20" s="75"/>
+      <c r="AE20" s="75"/>
+      <c r="AF20" s="75"/>
+      <c r="AG20" s="76"/>
       <c r="AH20" s="19"/>
       <c r="AI20" s="19"/>
       <c r="AJ20" s="4"/>
@@ -5373,27 +5388,27 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="11"/>
-      <c r="K25" s="65" t="s">
+      <c r="K25" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="L25" s="65"/>
-      <c r="M25" s="65"/>
-      <c r="N25" s="65"/>
-      <c r="O25" s="65"/>
-      <c r="P25" s="65"/>
-      <c r="Q25" s="65"/>
-      <c r="R25" s="65"/>
+      <c r="L25" s="62"/>
+      <c r="M25" s="62"/>
+      <c r="N25" s="62"/>
+      <c r="O25" s="62"/>
+      <c r="P25" s="62"/>
+      <c r="Q25" s="62"/>
+      <c r="R25" s="62"/>
       <c r="T25" s="3"/>
-      <c r="U25" s="65" t="s">
+      <c r="U25" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="V25" s="65"/>
-      <c r="W25" s="65"/>
-      <c r="X25" s="65"/>
-      <c r="Y25" s="65"/>
-      <c r="Z25" s="65"/>
-      <c r="AA25" s="65"/>
-      <c r="AB25" s="65"/>
+      <c r="V25" s="62"/>
+      <c r="W25" s="62"/>
+      <c r="X25" s="62"/>
+      <c r="Y25" s="62"/>
+      <c r="Z25" s="62"/>
+      <c r="AA25" s="62"/>
+      <c r="AB25" s="62"/>
       <c r="AD25" s="11"/>
       <c r="AE25" s="11"/>
       <c r="AF25" s="11"/>
@@ -5404,16 +5419,16 @@
       <c r="AK25" s="11"/>
       <c r="AL25" s="11"/>
       <c r="AM25" s="11"/>
-      <c r="AN25" s="65" t="s">
+      <c r="AN25" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="AO25" s="65"/>
-      <c r="AP25" s="65"/>
-      <c r="AQ25" s="65"/>
-      <c r="AR25" s="65"/>
-      <c r="AS25" s="65"/>
-      <c r="AT25" s="65"/>
-      <c r="AU25" s="65"/>
+      <c r="AO25" s="62"/>
+      <c r="AP25" s="62"/>
+      <c r="AQ25" s="62"/>
+      <c r="AR25" s="62"/>
+      <c r="AS25" s="62"/>
+      <c r="AT25" s="62"/>
+      <c r="AU25" s="62"/>
       <c r="AW25" s="4"/>
     </row>
     <row r="26" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -5428,23 +5443,23 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="11"/>
-      <c r="K26" s="65"/>
-      <c r="L26" s="65"/>
-      <c r="M26" s="65"/>
-      <c r="N26" s="65"/>
-      <c r="O26" s="65"/>
-      <c r="P26" s="65"/>
-      <c r="Q26" s="65"/>
-      <c r="R26" s="65"/>
+      <c r="K26" s="62"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="62"/>
+      <c r="N26" s="62"/>
+      <c r="O26" s="62"/>
+      <c r="P26" s="62"/>
+      <c r="Q26" s="62"/>
+      <c r="R26" s="62"/>
       <c r="T26" s="3"/>
-      <c r="U26" s="65"/>
-      <c r="V26" s="65"/>
-      <c r="W26" s="65"/>
-      <c r="X26" s="65"/>
-      <c r="Y26" s="65"/>
-      <c r="Z26" s="65"/>
-      <c r="AA26" s="65"/>
-      <c r="AB26" s="65"/>
+      <c r="U26" s="62"/>
+      <c r="V26" s="62"/>
+      <c r="W26" s="62"/>
+      <c r="X26" s="62"/>
+      <c r="Y26" s="62"/>
+      <c r="Z26" s="62"/>
+      <c r="AA26" s="62"/>
+      <c r="AB26" s="62"/>
       <c r="AD26" s="11"/>
       <c r="AE26" s="11"/>
       <c r="AF26" s="11"/>
@@ -5455,14 +5470,14 @@
       <c r="AK26" s="11"/>
       <c r="AL26" s="11"/>
       <c r="AM26" s="11"/>
-      <c r="AN26" s="65"/>
-      <c r="AO26" s="65"/>
-      <c r="AP26" s="65"/>
-      <c r="AQ26" s="65"/>
-      <c r="AR26" s="65"/>
-      <c r="AS26" s="65"/>
-      <c r="AT26" s="65"/>
-      <c r="AU26" s="65"/>
+      <c r="AN26" s="62"/>
+      <c r="AO26" s="62"/>
+      <c r="AP26" s="62"/>
+      <c r="AQ26" s="62"/>
+      <c r="AR26" s="62"/>
+      <c r="AS26" s="62"/>
+      <c r="AT26" s="62"/>
+      <c r="AU26" s="62"/>
       <c r="AW26" s="4"/>
     </row>
     <row r="27" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -5475,23 +5490,23 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
-      <c r="K27" s="65"/>
-      <c r="L27" s="65"/>
-      <c r="M27" s="65"/>
-      <c r="N27" s="65"/>
-      <c r="O27" s="65"/>
-      <c r="P27" s="65"/>
-      <c r="Q27" s="65"/>
-      <c r="R27" s="65"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="62"/>
+      <c r="N27" s="62"/>
+      <c r="O27" s="62"/>
+      <c r="P27" s="62"/>
+      <c r="Q27" s="62"/>
+      <c r="R27" s="62"/>
       <c r="T27" s="11"/>
-      <c r="U27" s="65"/>
-      <c r="V27" s="65"/>
-      <c r="W27" s="65"/>
-      <c r="X27" s="65"/>
-      <c r="Y27" s="65"/>
-      <c r="Z27" s="65"/>
-      <c r="AA27" s="65"/>
-      <c r="AB27" s="65"/>
+      <c r="U27" s="62"/>
+      <c r="V27" s="62"/>
+      <c r="W27" s="62"/>
+      <c r="X27" s="62"/>
+      <c r="Y27" s="62"/>
+      <c r="Z27" s="62"/>
+      <c r="AA27" s="62"/>
+      <c r="AB27" s="62"/>
       <c r="AD27" s="11"/>
       <c r="AE27" s="11"/>
       <c r="AF27" s="11"/>
@@ -5502,14 +5517,14 @@
       <c r="AK27" s="11"/>
       <c r="AL27" s="11"/>
       <c r="AM27" s="11"/>
-      <c r="AN27" s="65"/>
-      <c r="AO27" s="65"/>
-      <c r="AP27" s="65"/>
-      <c r="AQ27" s="65"/>
-      <c r="AR27" s="65"/>
-      <c r="AS27" s="65"/>
-      <c r="AT27" s="65"/>
-      <c r="AU27" s="65"/>
+      <c r="AN27" s="62"/>
+      <c r="AO27" s="62"/>
+      <c r="AP27" s="62"/>
+      <c r="AQ27" s="62"/>
+      <c r="AR27" s="62"/>
+      <c r="AS27" s="62"/>
+      <c r="AT27" s="62"/>
+      <c r="AU27" s="62"/>
       <c r="AW27" s="4"/>
     </row>
     <row r="28" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5596,7 +5611,7 @@
   <dimension ref="B1:AW28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD19"/>
+      <selection activeCell="AL1" sqref="AL1:AV1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5606,20 +5621,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="72" t="s">
+      <c r="D2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -5695,21 +5710,21 @@
       <c r="AI3" s="11"/>
       <c r="AJ3" s="11"/>
       <c r="AK3" s="11"/>
-      <c r="AL3" s="11"/>
-      <c r="AM3" s="11" t="s">
+      <c r="AL3" s="7"/>
+      <c r="AM3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="AN3" s="11"/>
-      <c r="AO3" s="11"/>
-      <c r="AP3" s="3"/>
-      <c r="AQ3" s="3"/>
-      <c r="AR3" s="11"/>
-      <c r="AS3" s="11"/>
-      <c r="AT3" s="73" t="s">
+      <c r="AN3" s="8"/>
+      <c r="AO3" s="8"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="8"/>
+      <c r="AS3" s="8"/>
+      <c r="AT3" s="185" t="s">
         <v>10</v>
       </c>
-      <c r="AU3" s="73"/>
-      <c r="AV3" s="73"/>
+      <c r="AU3" s="185"/>
+      <c r="AV3" s="186"/>
       <c r="AW3" s="12"/>
     </row>
     <row r="4" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -5738,7 +5753,7 @@
       <c r="AI4" s="11"/>
       <c r="AJ4" s="11"/>
       <c r="AK4" s="11"/>
-      <c r="AL4" s="11"/>
+      <c r="AL4" s="10"/>
       <c r="AM4" s="11" t="s">
         <v>11</v>
       </c>
@@ -5748,12 +5763,12 @@
       <c r="AQ4" s="3"/>
       <c r="AR4" s="11"/>
       <c r="AS4" s="11"/>
-      <c r="AT4" s="73"/>
-      <c r="AU4" s="73"/>
-      <c r="AV4" s="73"/>
+      <c r="AT4" s="64"/>
+      <c r="AU4" s="64"/>
+      <c r="AV4" s="187"/>
       <c r="AW4" s="12"/>
     </row>
-    <row r="5" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
       <c r="D5" s="51"/>
@@ -5777,17 +5792,17 @@
       <c r="AI5" s="11"/>
       <c r="AJ5" s="11"/>
       <c r="AK5" s="11"/>
-      <c r="AL5" s="11"/>
-      <c r="AM5" s="11"/>
-      <c r="AN5" s="11"/>
-      <c r="AO5" s="11"/>
-      <c r="AP5" s="11"/>
-      <c r="AQ5" s="11"/>
-      <c r="AR5" s="11"/>
-      <c r="AS5" s="11"/>
-      <c r="AT5" s="73"/>
-      <c r="AU5" s="73"/>
-      <c r="AV5" s="73"/>
+      <c r="AL5" s="13"/>
+      <c r="AM5" s="14"/>
+      <c r="AN5" s="14"/>
+      <c r="AO5" s="14"/>
+      <c r="AP5" s="14"/>
+      <c r="AQ5" s="14"/>
+      <c r="AR5" s="14"/>
+      <c r="AS5" s="14"/>
+      <c r="AT5" s="188"/>
+      <c r="AU5" s="188"/>
+      <c r="AV5" s="189"/>
       <c r="AW5" s="12"/>
     </row>
     <row r="6" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5864,18 +5879,18 @@
       <c r="AI7" s="8"/>
       <c r="AJ7" s="9"/>
       <c r="AL7" s="11"/>
-      <c r="AM7" s="74" t="s">
+      <c r="AM7" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="AN7" s="75"/>
-      <c r="AO7" s="75"/>
-      <c r="AP7" s="75"/>
-      <c r="AQ7" s="75"/>
-      <c r="AR7" s="75"/>
-      <c r="AS7" s="75"/>
-      <c r="AT7" s="75"/>
-      <c r="AU7" s="75"/>
-      <c r="AV7" s="76"/>
+      <c r="AN7" s="66"/>
+      <c r="AO7" s="66"/>
+      <c r="AP7" s="66"/>
+      <c r="AQ7" s="66"/>
+      <c r="AR7" s="66"/>
+      <c r="AS7" s="66"/>
+      <c r="AT7" s="66"/>
+      <c r="AU7" s="66"/>
+      <c r="AV7" s="67"/>
       <c r="AW7" s="4"/>
     </row>
     <row r="8" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6686,16 +6701,16 @@
       <c r="AK25" s="11"/>
       <c r="AL25" s="11"/>
       <c r="AM25" s="11"/>
-      <c r="AN25" s="65" t="s">
+      <c r="AN25" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="AO25" s="65"/>
-      <c r="AP25" s="65"/>
-      <c r="AQ25" s="65"/>
-      <c r="AR25" s="65"/>
-      <c r="AS25" s="65"/>
-      <c r="AT25" s="65"/>
-      <c r="AU25" s="65"/>
+      <c r="AO25" s="62"/>
+      <c r="AP25" s="62"/>
+      <c r="AQ25" s="62"/>
+      <c r="AR25" s="62"/>
+      <c r="AS25" s="62"/>
+      <c r="AT25" s="62"/>
+      <c r="AU25" s="62"/>
       <c r="AW25" s="4"/>
     </row>
     <row r="26" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6731,14 +6746,14 @@
       <c r="AK26" s="11"/>
       <c r="AL26" s="11"/>
       <c r="AM26" s="11"/>
-      <c r="AN26" s="65"/>
-      <c r="AO26" s="65"/>
-      <c r="AP26" s="65"/>
-      <c r="AQ26" s="65"/>
-      <c r="AR26" s="65"/>
-      <c r="AS26" s="65"/>
-      <c r="AT26" s="65"/>
-      <c r="AU26" s="65"/>
+      <c r="AN26" s="62"/>
+      <c r="AO26" s="62"/>
+      <c r="AP26" s="62"/>
+      <c r="AQ26" s="62"/>
+      <c r="AR26" s="62"/>
+      <c r="AS26" s="62"/>
+      <c r="AT26" s="62"/>
+      <c r="AU26" s="62"/>
       <c r="AW26" s="4"/>
     </row>
     <row r="27" spans="2:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6778,14 +6793,14 @@
       <c r="AK27" s="11"/>
       <c r="AL27" s="11"/>
       <c r="AM27" s="11"/>
-      <c r="AN27" s="65"/>
-      <c r="AO27" s="65"/>
-      <c r="AP27" s="65"/>
-      <c r="AQ27" s="65"/>
-      <c r="AR27" s="65"/>
-      <c r="AS27" s="65"/>
-      <c r="AT27" s="65"/>
-      <c r="AU27" s="65"/>
+      <c r="AN27" s="62"/>
+      <c r="AO27" s="62"/>
+      <c r="AP27" s="62"/>
+      <c r="AQ27" s="62"/>
+      <c r="AR27" s="62"/>
+      <c r="AS27" s="62"/>
+      <c r="AT27" s="62"/>
+      <c r="AU27" s="62"/>
       <c r="AW27" s="4"/>
     </row>
     <row r="28" spans="2:49" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6930,12 +6945,12 @@
     </row>
     <row r="3" spans="2:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10"/>
-      <c r="C3" s="102" t="s">
+      <c r="C3" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="104"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="118"/>
       <c r="H3" s="134" t="s">
         <v>25</v>
       </c>
@@ -6954,12 +6969,12 @@
       <c r="U3" s="136"/>
       <c r="V3" s="11"/>
       <c r="W3" s="11"/>
-      <c r="X3" s="111" t="s">
+      <c r="X3" s="125" t="s">
         <v>31</v>
       </c>
-      <c r="Y3" s="112"/>
-      <c r="Z3" s="112"/>
-      <c r="AA3" s="113"/>
+      <c r="Y3" s="126"/>
+      <c r="Z3" s="126"/>
+      <c r="AA3" s="127"/>
       <c r="AB3" s="11"/>
       <c r="AD3" s="140" t="s">
         <v>25</v>
@@ -6977,20 +6992,20 @@
       <c r="AO3" s="141"/>
       <c r="AP3" s="141"/>
       <c r="AQ3" s="142"/>
-      <c r="AS3" s="102" t="s">
+      <c r="AS3" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="AT3" s="103"/>
-      <c r="AU3" s="103"/>
-      <c r="AV3" s="104"/>
+      <c r="AT3" s="117"/>
+      <c r="AU3" s="117"/>
+      <c r="AV3" s="118"/>
       <c r="AW3" s="12"/>
     </row>
     <row r="4" spans="2:57" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
-      <c r="C4" s="105"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="107"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="121"/>
       <c r="H4" s="137"/>
       <c r="I4" s="138"/>
       <c r="J4" s="138"/>
@@ -7005,10 +7020,10 @@
       <c r="S4" s="138"/>
       <c r="T4" s="138"/>
       <c r="U4" s="139"/>
-      <c r="X4" s="114"/>
-      <c r="Y4" s="115"/>
-      <c r="Z4" s="115"/>
-      <c r="AA4" s="116"/>
+      <c r="X4" s="128"/>
+      <c r="Y4" s="129"/>
+      <c r="Z4" s="129"/>
+      <c r="AA4" s="130"/>
       <c r="AD4" s="143"/>
       <c r="AE4" s="144"/>
       <c r="AF4" s="144"/>
@@ -7023,18 +7038,18 @@
       <c r="AO4" s="144"/>
       <c r="AP4" s="144"/>
       <c r="AQ4" s="145"/>
-      <c r="AS4" s="105"/>
-      <c r="AT4" s="106"/>
-      <c r="AU4" s="106"/>
-      <c r="AV4" s="107"/>
+      <c r="AS4" s="119"/>
+      <c r="AT4" s="120"/>
+      <c r="AU4" s="120"/>
+      <c r="AV4" s="121"/>
       <c r="AW4" s="12"/>
     </row>
     <row r="5" spans="2:57" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="107"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="120"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="121"/>
       <c r="L5" s="11"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
@@ -7042,10 +7057,10 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
-      <c r="X5" s="114"/>
-      <c r="Y5" s="115"/>
-      <c r="Z5" s="115"/>
-      <c r="AA5" s="116"/>
+      <c r="X5" s="128"/>
+      <c r="Y5" s="129"/>
+      <c r="Z5" s="129"/>
+      <c r="AA5" s="130"/>
       <c r="AF5" s="11"/>
       <c r="AG5" s="11"/>
       <c r="AH5" s="11"/>
@@ -7058,40 +7073,40 @@
       <c r="AO5" s="11"/>
       <c r="AP5" s="11"/>
       <c r="AQ5" s="11"/>
-      <c r="AS5" s="105"/>
-      <c r="AT5" s="106"/>
-      <c r="AU5" s="106"/>
-      <c r="AV5" s="107"/>
+      <c r="AS5" s="119"/>
+      <c r="AT5" s="120"/>
+      <c r="AU5" s="120"/>
+      <c r="AV5" s="121"/>
       <c r="AW5" s="12"/>
     </row>
     <row r="6" spans="2:57" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="10"/>
-      <c r="C6" s="105"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="107"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="121"/>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
-      <c r="I6" s="121" t="s">
+      <c r="I6" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="122"/>
+      <c r="J6" s="95"/>
       <c r="K6" s="11"/>
-      <c r="L6" s="121" t="s">
+      <c r="L6" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="122"/>
+      <c r="M6" s="95"/>
       <c r="N6" s="26"/>
-      <c r="O6" s="121" t="s">
+      <c r="O6" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="122"/>
+      <c r="P6" s="95"/>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
-      <c r="X6" s="117"/>
-      <c r="Y6" s="118"/>
-      <c r="Z6" s="118"/>
-      <c r="AA6" s="119"/>
+      <c r="X6" s="131"/>
+      <c r="Y6" s="132"/>
+      <c r="Z6" s="132"/>
+      <c r="AA6" s="133"/>
       <c r="AF6" s="11"/>
       <c r="AG6" s="11"/>
       <c r="AH6" s="11"/>
@@ -7104,28 +7119,28 @@
       <c r="AO6" s="11"/>
       <c r="AP6" s="11"/>
       <c r="AQ6" s="11"/>
-      <c r="AS6" s="105"/>
-      <c r="AT6" s="106"/>
-      <c r="AU6" s="106"/>
-      <c r="AV6" s="107"/>
+      <c r="AS6" s="119"/>
+      <c r="AT6" s="120"/>
+      <c r="AU6" s="120"/>
+      <c r="AV6" s="121"/>
       <c r="AW6" s="12"/>
     </row>
     <row r="7" spans="2:57" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10"/>
-      <c r="C7" s="108"/>
-      <c r="D7" s="109"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="110"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="123"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="124"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="123"/>
-      <c r="J7" s="124"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="97"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="123"/>
-      <c r="M7" s="124"/>
+      <c r="L7" s="96"/>
+      <c r="M7" s="97"/>
       <c r="N7" s="26"/>
-      <c r="O7" s="123"/>
-      <c r="P7" s="124"/>
+      <c r="O7" s="96"/>
+      <c r="P7" s="97"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
@@ -7152,10 +7167,10 @@
       <c r="AO7" s="20"/>
       <c r="AP7" s="20"/>
       <c r="AQ7" s="20"/>
-      <c r="AS7" s="108"/>
-      <c r="AT7" s="109"/>
-      <c r="AU7" s="109"/>
-      <c r="AV7" s="110"/>
+      <c r="AS7" s="122"/>
+      <c r="AT7" s="123"/>
+      <c r="AU7" s="123"/>
+      <c r="AV7" s="124"/>
       <c r="AW7" s="4"/>
     </row>
     <row r="8" spans="2:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7256,12 +7271,12 @@
       <c r="AV9" s="11"/>
       <c r="AW9" s="4"/>
       <c r="AZ9" s="49"/>
-      <c r="BA9" s="120" t="s">
+      <c r="BA9" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="BB9" s="120"/>
-      <c r="BC9" s="120"/>
-      <c r="BD9" s="120"/>
+      <c r="BB9" s="93"/>
+      <c r="BC9" s="93"/>
+      <c r="BD9" s="93"/>
       <c r="BE9" s="4"/>
     </row>
     <row r="10" spans="2:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7297,10 +7312,10 @@
       <c r="AV10" s="11"/>
       <c r="AW10" s="45"/>
       <c r="AZ10" s="49"/>
-      <c r="BA10" s="120"/>
-      <c r="BB10" s="120"/>
-      <c r="BC10" s="120"/>
-      <c r="BD10" s="120"/>
+      <c r="BA10" s="93"/>
+      <c r="BB10" s="93"/>
+      <c r="BC10" s="93"/>
+      <c r="BD10" s="93"/>
       <c r="BE10" s="4"/>
     </row>
     <row r="11" spans="2:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -7338,10 +7353,10 @@
         <v>28</v>
       </c>
       <c r="AZ11" s="49"/>
-      <c r="BA11" s="120"/>
-      <c r="BB11" s="120"/>
-      <c r="BC11" s="120"/>
-      <c r="BD11" s="120"/>
+      <c r="BA11" s="93"/>
+      <c r="BB11" s="93"/>
+      <c r="BC11" s="93"/>
+      <c r="BD11" s="93"/>
       <c r="BE11" s="4"/>
     </row>
     <row r="12" spans="2:57" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7420,17 +7435,17 @@
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
-      <c r="U13" s="125" t="s">
+      <c r="U13" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="V13" s="126"/>
-      <c r="W13" s="126"/>
-      <c r="X13" s="126"/>
-      <c r="Y13" s="126"/>
-      <c r="Z13" s="126"/>
-      <c r="AA13" s="126"/>
-      <c r="AB13" s="126"/>
-      <c r="AC13" s="127"/>
+      <c r="V13" s="99"/>
+      <c r="W13" s="99"/>
+      <c r="X13" s="99"/>
+      <c r="Y13" s="99"/>
+      <c r="Z13" s="99"/>
+      <c r="AA13" s="99"/>
+      <c r="AB13" s="99"/>
+      <c r="AC13" s="100"/>
       <c r="AD13" s="3"/>
       <c r="AE13" s="3"/>
       <c r="AF13" s="3"/>
@@ -7452,12 +7467,12 @@
       <c r="AV13" s="11"/>
       <c r="AW13" s="4"/>
       <c r="AZ13" s="49"/>
-      <c r="BA13" s="120" t="s">
+      <c r="BA13" s="93" t="s">
         <v>46</v>
       </c>
-      <c r="BB13" s="120"/>
-      <c r="BC13" s="120"/>
-      <c r="BD13" s="120"/>
+      <c r="BB13" s="93"/>
+      <c r="BC13" s="93"/>
+      <c r="BD13" s="93"/>
       <c r="BE13" s="4"/>
     </row>
     <row r="14" spans="2:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7480,15 +7495,15 @@
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
-      <c r="U14" s="128"/>
-      <c r="V14" s="129"/>
-      <c r="W14" s="129"/>
-      <c r="X14" s="129"/>
-      <c r="Y14" s="129"/>
-      <c r="Z14" s="129"/>
-      <c r="AA14" s="129"/>
-      <c r="AB14" s="129"/>
-      <c r="AC14" s="130"/>
+      <c r="U14" s="101"/>
+      <c r="V14" s="102"/>
+      <c r="W14" s="102"/>
+      <c r="X14" s="102"/>
+      <c r="Y14" s="102"/>
+      <c r="Z14" s="102"/>
+      <c r="AA14" s="102"/>
+      <c r="AB14" s="102"/>
+      <c r="AC14" s="103"/>
       <c r="AD14" s="3"/>
       <c r="AE14" s="3"/>
       <c r="AF14" s="3"/>
@@ -7510,10 +7525,10 @@
       <c r="AV14" s="11"/>
       <c r="AW14" s="4"/>
       <c r="AZ14" s="49"/>
-      <c r="BA14" s="120"/>
-      <c r="BB14" s="120"/>
-      <c r="BC14" s="120"/>
-      <c r="BD14" s="120"/>
+      <c r="BA14" s="93"/>
+      <c r="BB14" s="93"/>
+      <c r="BC14" s="93"/>
+      <c r="BD14" s="93"/>
       <c r="BE14" s="4"/>
     </row>
     <row r="15" spans="2:57" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7536,15 +7551,15 @@
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
-      <c r="U15" s="131"/>
-      <c r="V15" s="132"/>
-      <c r="W15" s="132"/>
-      <c r="X15" s="132"/>
-      <c r="Y15" s="132"/>
-      <c r="Z15" s="132"/>
-      <c r="AA15" s="132"/>
-      <c r="AB15" s="132"/>
-      <c r="AC15" s="133"/>
+      <c r="U15" s="104"/>
+      <c r="V15" s="105"/>
+      <c r="W15" s="105"/>
+      <c r="X15" s="105"/>
+      <c r="Y15" s="105"/>
+      <c r="Z15" s="105"/>
+      <c r="AA15" s="105"/>
+      <c r="AB15" s="105"/>
+      <c r="AC15" s="106"/>
       <c r="AD15" s="3"/>
       <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
@@ -7566,10 +7581,10 @@
       <c r="AV15" s="11"/>
       <c r="AW15" s="4"/>
       <c r="AZ15" s="49"/>
-      <c r="BA15" s="120"/>
-      <c r="BB15" s="120"/>
-      <c r="BC15" s="120"/>
-      <c r="BD15" s="120"/>
+      <c r="BA15" s="93"/>
+      <c r="BB15" s="93"/>
+      <c r="BC15" s="93"/>
+      <c r="BD15" s="93"/>
       <c r="BE15" s="4"/>
     </row>
     <row r="16" spans="2:57" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8005,16 +8020,16 @@
     </row>
     <row r="25" spans="2:49" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
-      <c r="C25" s="93" t="s">
+      <c r="C25" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="94"/>
-      <c r="E25" s="95"/>
-      <c r="G25" s="93" t="s">
+      <c r="D25" s="108"/>
+      <c r="E25" s="109"/>
+      <c r="G25" s="107" t="s">
         <v>27</v>
       </c>
-      <c r="H25" s="94"/>
-      <c r="I25" s="95"/>
+      <c r="H25" s="108"/>
+      <c r="I25" s="109"/>
       <c r="AI25" s="11"/>
       <c r="AJ25" s="11"/>
       <c r="AK25" s="152"/>
@@ -8033,12 +8048,12 @@
     </row>
     <row r="26" spans="2:49" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
-      <c r="C26" s="96"/>
-      <c r="D26" s="97"/>
-      <c r="E26" s="98"/>
-      <c r="G26" s="96"/>
-      <c r="H26" s="97"/>
-      <c r="I26" s="98"/>
+      <c r="C26" s="110"/>
+      <c r="D26" s="111"/>
+      <c r="E26" s="112"/>
+      <c r="G26" s="110"/>
+      <c r="H26" s="111"/>
+      <c r="I26" s="112"/>
       <c r="AI26" s="11"/>
       <c r="AJ26" s="11"/>
       <c r="AK26" s="11"/>
@@ -8057,12 +8072,12 @@
     </row>
     <row r="27" spans="2:49" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="10"/>
-      <c r="C27" s="99"/>
-      <c r="D27" s="100"/>
-      <c r="E27" s="101"/>
-      <c r="G27" s="99"/>
-      <c r="H27" s="100"/>
-      <c r="I27" s="101"/>
+      <c r="C27" s="113"/>
+      <c r="D27" s="114"/>
+      <c r="E27" s="115"/>
+      <c r="G27" s="113"/>
+      <c r="H27" s="114"/>
+      <c r="I27" s="115"/>
       <c r="T27" s="11"/>
       <c r="AI27" s="11"/>
       <c r="AJ27" s="11"/>
@@ -8134,12 +8149,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="BA9:BD11"/>
-    <mergeCell ref="BA13:BD15"/>
-    <mergeCell ref="I6:J7"/>
-    <mergeCell ref="L6:M7"/>
-    <mergeCell ref="O6:P7"/>
-    <mergeCell ref="U13:AC15"/>
     <mergeCell ref="C25:E27"/>
     <mergeCell ref="G25:I27"/>
     <mergeCell ref="AS3:AV7"/>
@@ -8150,6 +8159,12 @@
     <mergeCell ref="AP17:AS20"/>
     <mergeCell ref="AK22:AN25"/>
     <mergeCell ref="AP22:AU27"/>
+    <mergeCell ref="BA9:BD11"/>
+    <mergeCell ref="BA13:BD15"/>
+    <mergeCell ref="I6:J7"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="O6:P7"/>
+    <mergeCell ref="U13:AC15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="U13" location="Result!A1" display="Victory/Defeat"/>
@@ -9427,13 +9442,13 @@
       <c r="AO26" s="24"/>
       <c r="AP26" s="24"/>
       <c r="AQ26" s="24"/>
-      <c r="AR26" s="65" t="s">
+      <c r="AR26" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="AS26" s="65"/>
-      <c r="AT26" s="65"/>
-      <c r="AU26" s="65"/>
-      <c r="AV26" s="65"/>
+      <c r="AS26" s="62"/>
+      <c r="AT26" s="62"/>
+      <c r="AU26" s="62"/>
+      <c r="AV26" s="62"/>
       <c r="AW26" s="4"/>
     </row>
     <row r="27" spans="2:49" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9479,11 +9494,11 @@
       <c r="AO27" s="24"/>
       <c r="AP27" s="24"/>
       <c r="AQ27" s="24"/>
-      <c r="AR27" s="65"/>
-      <c r="AS27" s="65"/>
-      <c r="AT27" s="65"/>
-      <c r="AU27" s="65"/>
-      <c r="AV27" s="65"/>
+      <c r="AR27" s="62"/>
+      <c r="AS27" s="62"/>
+      <c r="AT27" s="62"/>
+      <c r="AU27" s="62"/>
+      <c r="AV27" s="62"/>
       <c r="AW27" s="4"/>
     </row>
     <row r="28" spans="2:49" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>